<commit_message>
chore: remove R24 and R25 part number and designator in BOM
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="230">
   <si>
     <t xml:space="preserve">S3Main PCS BOM</t>
   </si>
@@ -566,13 +566,7 @@
     <t xml:space="preserve">R24, R25</t>
   </si>
   <si>
-    <t xml:space="preserve">RC0805FR-074K7L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RES 4.7K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not fitted</t>
+    <t xml:space="preserve">DNP</t>
   </si>
   <si>
     <t xml:space="preserve">R28</t>
@@ -1072,9 +1066,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>651600</xdr:colOff>
+      <xdr:colOff>651240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1088,7 +1082,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="211680"/>
-          <a:ext cx="1362240" cy="361080"/>
+          <a:ext cx="1361880" cy="360720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1217,7 +1211,7 @@
   <dimension ref="A2:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
+      <selection pane="topLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2310,20 +2304,14 @@
       <c r="C45" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E45" s="7" t="s">
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="F45" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>156</v>
-      </c>
       <c r="H45" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I45" s="10"/>
     </row>
@@ -2332,7 +2320,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C46" s="6" t="n">
         <v>1</v>
@@ -2341,10 +2329,10 @@
         <v>122</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>14</v>
@@ -2359,7 +2347,7 @@
         <v>41</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C47" s="6" t="n">
         <v>4</v>
@@ -2368,10 +2356,10 @@
         <v>122</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G47" s="9" t="s">
         <v>14</v>
@@ -2386,7 +2374,7 @@
         <v>42</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C48" s="6" t="n">
         <v>1</v>
@@ -2395,10 +2383,10 @@
         <v>122</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>14</v>
@@ -2413,7 +2401,7 @@
         <v>43</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C49" s="6" t="n">
         <v>2</v>
@@ -2422,10 +2410,10 @@
         <v>122</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G49" s="9" t="s">
         <v>14</v>
@@ -2440,7 +2428,7 @@
         <v>44</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C50" s="6" t="n">
         <v>1</v>
@@ -2449,10 +2437,10 @@
         <v>122</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>14</v>
@@ -2467,7 +2455,7 @@
         <v>45</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C51" s="6" t="n">
         <v>1</v>
@@ -2476,10 +2464,10 @@
         <v>122</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G51" s="9" t="s">
         <v>14</v>
@@ -2494,7 +2482,7 @@
         <v>46</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C52" s="6" t="n">
         <v>2</v>
@@ -2503,10 +2491,10 @@
         <v>122</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>14</v>
@@ -2521,7 +2509,7 @@
         <v>47</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C53" s="6" t="n">
         <v>1</v>
@@ -2530,10 +2518,10 @@
         <v>122</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G53" s="9" t="s">
         <v>14</v>
@@ -2548,19 +2536,19 @@
         <v>48</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C54" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D54" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>182</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>184</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>14</v>
@@ -2575,22 +2563,22 @@
         <v>49</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C55" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E55" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G55" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="H55" s="10" t="s">
         <v>15</v>
@@ -2602,7 +2590,7 @@
         <v>50</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C56" s="6" t="n">
         <v>1</v>
@@ -2611,13 +2599,13 @@
         <v>49</v>
       </c>
       <c r="E56" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G56" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>192</v>
       </c>
       <c r="H56" s="10" t="s">
         <v>15</v>
@@ -2629,22 +2617,22 @@
         <v>51</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C57" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D57" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F57" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="G57" s="9" t="s">
         <v>195</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>197</v>
       </c>
       <c r="H57" s="10" t="s">
         <v>15</v>
@@ -2656,22 +2644,22 @@
         <v>52</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C58" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D58" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F58" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="G58" s="9" t="s">
         <v>200</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>202</v>
       </c>
       <c r="H58" s="10" t="s">
         <v>15</v>
@@ -2683,19 +2671,19 @@
         <v>53</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C59" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D59" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="F59" s="8" t="s">
         <v>204</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="G59" s="9"/>
       <c r="H59" s="10" t="s">
@@ -2708,22 +2696,22 @@
         <v>54</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C60" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E60" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G60" s="9" t="s">
         <v>208</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>210</v>
       </c>
       <c r="H60" s="10" t="s">
         <v>15</v>
@@ -2735,22 +2723,22 @@
         <v>55</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C61" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E61" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="G61" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>214</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>15</v>
@@ -2762,19 +2750,19 @@
         <v>56</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C62" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D62" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F62" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>218</v>
       </c>
       <c r="G62" s="9" t="s">
         <v>72</v>
@@ -2789,22 +2777,22 @@
         <v>57</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C63" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E63" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="G63" s="9" t="s">
         <v>220</v>
-      </c>
-      <c r="F63" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>222</v>
       </c>
       <c r="H63" s="10" t="s">
         <v>15</v>
@@ -2816,22 +2804,22 @@
         <v>58</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C64" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E64" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="G64" s="9" t="s">
         <v>224</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>226</v>
       </c>
       <c r="H64" s="10" t="s">
         <v>15</v>
@@ -2843,22 +2831,22 @@
         <v>59</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C65" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F65" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="G65" s="9" t="s">
         <v>229</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="H65" s="10" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
chore: replace ACK circuit with TPS281C100 fault pin
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="232">
   <si>
     <t xml:space="preserve">S3Main PCS BOM</t>
   </si>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">Your Instructions / Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C2, C3, C7, C8, C11, C18, C29, C30, C32</t>
+    <t xml:space="preserve">C1,C2,C3,C7,C8,C11,C18,C29,C30,C31</t>
   </si>
   <si>
     <t xml:space="preserve">Samsung Electro-Mechanics</t>
@@ -152,7 +152,7 @@
     <t xml:space="preserve">SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">C4, C6, C19, C21, C22, C25, C26, C34</t>
+    <t xml:space="preserve">C4,C6,C19,C21,C22,C25,C26,C33</t>
   </si>
   <si>
     <t xml:space="preserve">Murata Electronics</t>
@@ -164,7 +164,7 @@
     <t xml:space="preserve">CAP CER 1000PF 100V C0G/NP0 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">C5, C35, C36</t>
+    <t xml:space="preserve">C5,C34,C35</t>
   </si>
   <si>
     <t xml:space="preserve">GCM1555C1H221JA16D</t>
@@ -173,7 +173,7 @@
     <t xml:space="preserve">CAP CER 220PF 50V C0G/NP0 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">C9, C10</t>
+    <t xml:space="preserve">C9,C10</t>
   </si>
   <si>
     <t xml:space="preserve">GCM1555C1H101JA16D</t>
@@ -182,7 +182,7 @@
     <t xml:space="preserve">CAP CER 100PF 50V C0G/NP0 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">C12, C20, C27</t>
+    <t xml:space="preserve">C12,C20,C27</t>
   </si>
   <si>
     <t xml:space="preserve">Cornell Dubilier Knowles</t>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">CAP CER 10UF 50V X7R 1206</t>
   </si>
   <si>
-    <t xml:space="preserve">C15, C16, C17, C23, C24</t>
+    <t xml:space="preserve">C15,C16,C17,C23,C24</t>
   </si>
   <si>
     <t xml:space="preserve">CL31B105KCHVPJE</t>
@@ -236,16 +236,7 @@
     <t xml:space="preserve">CAP CER 4.7UF 50V X7R 1206</t>
   </si>
   <si>
-    <t xml:space="preserve">C31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRT3195C2A103JA02D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 10000PF 100V C0G 1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C33, C37</t>
+    <t xml:space="preserve">C32,C36</t>
   </si>
   <si>
     <t xml:space="preserve">TDK Corporation</t>
@@ -257,7 +248,7 @@
     <t xml:space="preserve">CAP CER 47UF 6.3V X7S 1206</t>
   </si>
   <si>
-    <t xml:space="preserve">D1, D2, D3, D7, D8, D11, D13, D16, D17, D19</t>
+    <t xml:space="preserve">D1,D2,D3,D7,D8,D11,D13,D14,D15,D17</t>
   </si>
   <si>
     <t xml:space="preserve">onsemi</t>
@@ -344,22 +335,7 @@
     <t xml:space="preserve">TVS DIODE 30VWM 47.5VC ESC</t>
   </si>
   <si>
-    <t xml:space="preserve">D14, D15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micro Commercial Co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B5819W-TP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIODE SCHOTTKY 40V 1A SOD123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOD-123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D18</t>
+    <t xml:space="preserve">D16</t>
   </si>
   <si>
     <t xml:space="preserve">Diodes Incorporated</t>
@@ -440,7 +416,7 @@
     <t xml:space="preserve">0805</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1, Q6</t>
+    <t xml:space="preserve">Q1,Q6</t>
   </si>
   <si>
     <t xml:space="preserve">Rohm Semiconductor</t>
@@ -467,7 +443,7 @@
     <t xml:space="preserve">SOT-363</t>
   </si>
   <si>
-    <t xml:space="preserve">Q3, Q4, Q5, Q7, Q8</t>
+    <t xml:space="preserve">Q3,Q4,Q5,Q7,Q8</t>
   </si>
   <si>
     <t xml:space="preserve">Vishay Siliconix</t>
@@ -485,15 +461,6 @@
     <t xml:space="preserve">Q9</t>
   </si>
   <si>
-    <t xml:space="preserve">BSS138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSFET N-CH 50V 220MA SOT23-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q10</t>
-  </si>
-  <si>
     <t xml:space="preserve">ANBON SEMICONDUCTOR (INT'L) LIMITED</t>
   </si>
   <si>
@@ -506,7 +473,7 @@
     <t xml:space="preserve">SOT-23</t>
   </si>
   <si>
-    <t xml:space="preserve">R1, R8, R18, R20, R34, R35, R36, R43, R48, R50</t>
+    <t xml:space="preserve">R1,R8,R18,R20,R35,R36,R37,R44,R49</t>
   </si>
   <si>
     <t xml:space="preserve">YAGEO</t>
@@ -518,7 +485,7 @@
     <t xml:space="preserve">RES 10K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R2, R3, R4, R5</t>
+    <t xml:space="preserve">R2,R3,R4,R5</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0722KL</t>
@@ -527,7 +494,7 @@
     <t xml:space="preserve">RES 22K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R6, R7, R31, R49</t>
+    <t xml:space="preserve">R6,R7,R31</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-074K7L</t>
@@ -548,7 +515,7 @@
     <t xml:space="preserve">RES SMD 2.2 OHM 1% 1/2W 0805</t>
   </si>
   <si>
-    <t xml:space="preserve">R10, R11, R14, R32, R45, R51</t>
+    <t xml:space="preserve">R10,R11,R14,R32,R46</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-071KL</t>
@@ -557,7 +524,7 @@
     <t xml:space="preserve">RES 1K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R12, R13, R22, R26, R27</t>
+    <t xml:space="preserve">R12,R13,R22,R26,R27</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-073K3L</t>
@@ -566,7 +533,7 @@
     <t xml:space="preserve">RES 3.3K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R15, R16, R52, R53</t>
+    <t xml:space="preserve">R15,R16,R50,R51</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0733RL</t>
@@ -584,7 +551,7 @@
     <t xml:space="preserve">RES 220 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R19, R54</t>
+    <t xml:space="preserve">R19,R34</t>
   </si>
   <si>
     <t xml:space="preserve">DNP</t>
@@ -608,7 +575,7 @@
     <t xml:space="preserve">RES 562 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R24, R25</t>
+    <t xml:space="preserve">R24,R25</t>
   </si>
   <si>
     <t xml:space="preserve">R28</t>
@@ -620,7 +587,7 @@
     <t xml:space="preserve">RES 422 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R29, R30, R46, R47</t>
+    <t xml:space="preserve">R29,R30,R47,R48</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0747RL</t>
@@ -638,7 +605,7 @@
     <t xml:space="preserve">RES 180 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R37, R44</t>
+    <t xml:space="preserve">R38,R45</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0714K3L</t>
@@ -647,7 +614,7 @@
     <t xml:space="preserve">RES 14.3K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R38</t>
+    <t xml:space="preserve">R39</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-07470RL</t>
@@ -656,7 +623,7 @@
     <t xml:space="preserve">RES 470 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R39</t>
+    <t xml:space="preserve">R40</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0718K7L</t>
@@ -665,7 +632,7 @@
     <t xml:space="preserve">RES 18.7K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R40, R41</t>
+    <t xml:space="preserve">R41,R42</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-075K1L</t>
@@ -674,7 +641,7 @@
     <t xml:space="preserve">RES 5.1K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R42</t>
+    <t xml:space="preserve">R43</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0739KL</t>
@@ -683,7 +650,7 @@
     <t xml:space="preserve">RES 39K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R55</t>
+    <t xml:space="preserve">R52</t>
   </si>
   <si>
     <t xml:space="preserve">Panasonic Electronic Components</t>
@@ -1105,13 +1072,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>649800</xdr:colOff>
+      <xdr:colOff>649440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="图片 1" descr="pcbway-400x400.jpg"/>
+        <xdr:cNvPr id="1" name="图片 1" descr="pcbway-400x400.jpg"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1121,7 +1088,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="211680"/>
-          <a:ext cx="1360440" cy="359280"/>
+          <a:ext cx="1360080" cy="358920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1251,7 +1218,7 @@
   <dimension ref="A2:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N64" activeCellId="0" sqref="N64"/>
+      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1569,16 +1536,16 @@
         <v>44</v>
       </c>
       <c r="C16" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>34</v>
@@ -1593,22 +1560,22 @@
         <v>11</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>15</v>
@@ -1620,22 +1587,22 @@
         <v>12</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>15</v>
@@ -1647,13 +1614,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>58</v>
@@ -1680,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>61</v>
@@ -1707,16 +1674,16 @@
         <v>1</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="H21" s="10" t="s">
         <v>15</v>
@@ -1728,22 +1695,22 @@
         <v>16</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>15</v>
@@ -1755,22 +1722,22 @@
         <v>17</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C23" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>15</v>
@@ -1782,22 +1749,22 @@
         <v>18</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>15</v>
@@ -1809,25 +1776,23 @@
         <v>19</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C25" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="E25" s="7" t="n">
+        <v>1844210</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>84</v>
       </c>
+      <c r="G25" s="9"/>
       <c r="H25" s="10" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="I25" s="10"/>
     </row>
@@ -1836,23 +1801,21 @@
         <v>20</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C26" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="F26" s="8" t="s">
         <v>89</v>
       </c>
+      <c r="G26" s="9"/>
       <c r="H26" s="10" t="s">
         <v>15</v>
       </c>
@@ -1869,17 +1832,17 @@
         <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="7" t="n">
+        <v>1836189</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="E27" s="7" t="n">
-        <v>1844210</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I27" s="10"/>
     </row>
@@ -1888,19 +1851,19 @@
         <v>22</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="10" t="s">
@@ -1913,23 +1876,23 @@
         <v>23</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="7" t="n">
-        <v>1836189</v>
+        <v>97</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>99</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="10" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="I29" s="10"/>
     </row>
@@ -1944,15 +1907,17 @@
         <v>1</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="G30" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="G30" s="9"/>
       <c r="H30" s="10" t="s">
         <v>15</v>
       </c>
@@ -1966,7 +1931,7 @@
         <v>104</v>
       </c>
       <c r="C31" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>105</v>
@@ -1974,10 +1939,12 @@
       <c r="E31" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="G31" s="9"/>
+      <c r="G31" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="H31" s="10" t="s">
         <v>15</v>
       </c>
@@ -1988,22 +1955,22 @@
         <v>26</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C32" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F32" s="8" t="s">
         <v>110</v>
       </c>
+      <c r="F32" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="G32" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H32" s="10" t="s">
         <v>15</v>
@@ -2015,22 +1982,22 @@
         <v>27</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C33" s="6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="7" t="s">
         <v>115</v>
       </c>
+      <c r="F33" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="G33" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>15</v>
@@ -2042,22 +2009,22 @@
         <v>28</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C34" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>15</v>
@@ -2069,22 +2036,22 @@
         <v>29</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C35" s="6" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>125</v>
+        <v>14</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>15</v>
@@ -2096,22 +2063,22 @@
         <v>30</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C36" s="6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>15</v>
@@ -2123,13 +2090,13 @@
         <v>31</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C37" s="6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>131</v>
@@ -2138,7 +2105,7 @@
         <v>132</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="H37" s="10" t="s">
         <v>15</v>
@@ -2150,22 +2117,22 @@
         <v>32</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C38" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="D38" s="7" t="s">
+      <c r="E38" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>137</v>
-      </c>
       <c r="G38" s="9" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="H38" s="10" t="s">
         <v>15</v>
@@ -2177,19 +2144,19 @@
         <v>33</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C39" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>140</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>14</v>
@@ -2204,19 +2171,19 @@
         <v>34</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C40" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" s="7" t="s">
+      <c r="F40" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>14</v>
@@ -2231,22 +2198,22 @@
         <v>35</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>147</v>
-      </c>
       <c r="G41" s="9" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="H41" s="10" t="s">
         <v>15</v>
@@ -2258,19 +2225,19 @@
         <v>36</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="C42" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>14</v>
@@ -2285,25 +2252,19 @@
         <v>37</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C43" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="10" t="s">
+        <v>150</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="I43" s="10"/>
     </row>
@@ -2312,19 +2273,19 @@
         <v>38</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C44" s="6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>14</v>
@@ -2339,19 +2300,19 @@
         <v>39</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C45" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>14</v>
@@ -2366,7 +2327,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C46" s="6" t="n">
         <v>2</v>
@@ -2375,10 +2336,10 @@
       <c r="E46" s="7"/>
       <c r="F46" s="8"/>
       <c r="G46" s="10" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="I46" s="10"/>
     </row>
@@ -2387,19 +2348,19 @@
         <v>41</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C47" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="G47" s="9" t="s">
         <v>14</v>
@@ -2414,19 +2375,19 @@
         <v>42</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C48" s="6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>14</v>
@@ -2441,19 +2402,25 @@
         <v>43</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C49" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="10" t="s">
-        <v>161</v>
+        <v>1</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="I49" s="10"/>
     </row>
@@ -2462,19 +2429,19 @@
         <v>44</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C50" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F50" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="C50" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>14</v>
@@ -2489,19 +2456,19 @@
         <v>45</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C51" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F51" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="C51" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="G51" s="9" t="s">
         <v>14</v>
@@ -2516,19 +2483,19 @@
         <v>46</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C52" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>14</v>
@@ -2543,19 +2510,19 @@
         <v>47</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C53" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G53" s="9" t="s">
         <v>14</v>
@@ -2570,19 +2537,19 @@
         <v>48</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C54" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>14</v>
@@ -2597,19 +2564,19 @@
         <v>49</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C55" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="E55" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F55" s="8" t="s">
         <v>185</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>186</v>
       </c>
       <c r="G55" s="9" t="s">
         <v>14</v>
@@ -2624,22 +2591,22 @@
         <v>50</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C56" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="E56" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F56" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="G56" s="9" t="s">
         <v>189</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="H56" s="10" t="s">
         <v>15</v>
@@ -2657,16 +2624,16 @@
         <v>1</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>135</v>
+        <v>49</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F57" s="7" t="s">
         <v>192</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>14</v>
+        <v>193</v>
       </c>
       <c r="H57" s="10" t="s">
         <v>15</v>
@@ -2678,22 +2645,22 @@
         <v>52</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C58" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>14</v>
+        <v>198</v>
       </c>
       <c r="H58" s="10" t="s">
         <v>15</v>
@@ -2705,22 +2672,22 @@
         <v>53</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C59" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H59" s="10" t="s">
         <v>15</v>
@@ -2732,23 +2699,21 @@
         <v>54</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C60" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>204</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="G60" s="9"/>
       <c r="H60" s="10" t="s">
         <v>15</v>
       </c>
@@ -2759,22 +2724,22 @@
         <v>55</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C61" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>15</v>
@@ -2786,22 +2751,22 @@
         <v>56</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C62" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H62" s="10" t="s">
         <v>15</v>
@@ -2813,13 +2778,13 @@
         <v>57</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C63" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>216</v>
+        <v>78</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>217</v>
@@ -2827,7 +2792,9 @@
       <c r="F63" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="G63" s="9"/>
+      <c r="G63" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="H63" s="10" t="s">
         <v>15</v>
       </c>
@@ -2844,12 +2811,12 @@
         <v>1</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="12" t="s">
         <v>221</v>
       </c>
       <c r="G64" s="9" t="s">
@@ -2871,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>211</v>
+        <v>78</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>224</v>
@@ -2898,1133 +2865,1055 @@
         <v>1</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>86</v>
+        <v>228</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>75</v>
+        <v>231</v>
       </c>
       <c r="H66" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I66" s="10"/>
     </row>
-    <row r="67" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6" t="n">
-        <v>61</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="C67" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="H67" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I67" s="10"/>
-    </row>
-    <row r="68" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6" t="n">
-        <v>62</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C68" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="G68" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="H68" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I68" s="10"/>
-    </row>
-    <row r="69" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6" t="n">
-        <v>63</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C69" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="H69" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I69" s="10"/>
-    </row>
+    <row r="67" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="70" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
-      <c r="K74" s="11"/>
-      <c r="L74" s="11"/>
-      <c r="M74" s="11"/>
-      <c r="N74" s="11"/>
-      <c r="O74" s="11"/>
-      <c r="P74" s="11"/>
-      <c r="Q74" s="11"/>
-      <c r="R74" s="11"/>
-      <c r="S74" s="11"/>
-      <c r="T74" s="11"/>
-      <c r="U74" s="11"/>
-      <c r="V74" s="11"/>
-      <c r="W74" s="11"/>
-      <c r="X74" s="11"/>
-      <c r="Y74" s="11"/>
-      <c r="Z74" s="11"/>
-      <c r="AA74" s="11"/>
-      <c r="AB74" s="11"/>
-      <c r="AC74" s="11"/>
-      <c r="AD74" s="11"/>
-      <c r="AE74" s="11"/>
-      <c r="AF74" s="11"/>
-      <c r="AG74" s="11"/>
-      <c r="AH74" s="11"/>
-      <c r="AI74" s="11"/>
-      <c r="AJ74" s="11"/>
-      <c r="AK74" s="11"/>
-      <c r="AL74" s="11"/>
-      <c r="AM74" s="11"/>
-      <c r="AN74" s="11"/>
-      <c r="AO74" s="11"/>
-      <c r="AP74" s="11"/>
-      <c r="AQ74" s="11"/>
-      <c r="AR74" s="11"/>
-      <c r="AS74" s="11"/>
-      <c r="AT74" s="11"/>
-      <c r="AU74" s="11"/>
-      <c r="AV74" s="11"/>
-      <c r="AW74" s="11"/>
-      <c r="AX74" s="11"/>
-      <c r="AY74" s="11"/>
-      <c r="AZ74" s="11"/>
-      <c r="BA74" s="11"/>
-      <c r="BB74" s="11"/>
-      <c r="BC74" s="11"/>
-      <c r="BD74" s="11"/>
-      <c r="BE74" s="11"/>
-      <c r="BF74" s="11"/>
-      <c r="BG74" s="11"/>
-      <c r="BH74" s="11"/>
-      <c r="BI74" s="11"/>
-      <c r="BJ74" s="11"/>
-      <c r="BK74" s="11"/>
-      <c r="BL74" s="11"/>
-      <c r="BM74" s="11"/>
-      <c r="BN74" s="11"/>
-      <c r="BO74" s="11"/>
-      <c r="BP74" s="11"/>
-      <c r="BQ74" s="11"/>
-      <c r="BR74" s="11"/>
-      <c r="BS74" s="11"/>
-      <c r="BT74" s="11"/>
-      <c r="BU74" s="11"/>
-      <c r="BV74" s="11"/>
-      <c r="BW74" s="11"/>
-      <c r="BX74" s="11"/>
-      <c r="BY74" s="11"/>
-      <c r="BZ74" s="11"/>
-      <c r="CA74" s="11"/>
-      <c r="CB74" s="11"/>
-      <c r="CC74" s="11"/>
-      <c r="CD74" s="11"/>
-      <c r="CE74" s="11"/>
-      <c r="CF74" s="11"/>
-      <c r="CG74" s="11"/>
-      <c r="CH74" s="11"/>
-      <c r="CI74" s="11"/>
-      <c r="CJ74" s="11"/>
-      <c r="CK74" s="11"/>
-      <c r="CL74" s="11"/>
-      <c r="CM74" s="11"/>
-      <c r="CN74" s="11"/>
-      <c r="CO74" s="11"/>
-      <c r="CP74" s="11"/>
-      <c r="CQ74" s="11"/>
-      <c r="CR74" s="11"/>
-      <c r="CS74" s="11"/>
-      <c r="CT74" s="11"/>
-      <c r="CU74" s="11"/>
-      <c r="CV74" s="11"/>
-      <c r="CW74" s="11"/>
-      <c r="CX74" s="11"/>
-      <c r="CY74" s="11"/>
-      <c r="CZ74" s="11"/>
-      <c r="DA74" s="11"/>
-      <c r="DB74" s="11"/>
-      <c r="DC74" s="11"/>
-      <c r="DD74" s="11"/>
-      <c r="DE74" s="11"/>
-      <c r="DF74" s="11"/>
-      <c r="DG74" s="11"/>
-      <c r="DH74" s="11"/>
-      <c r="DI74" s="11"/>
-      <c r="DJ74" s="11"/>
-      <c r="DK74" s="11"/>
-      <c r="DL74" s="11"/>
-      <c r="DM74" s="11"/>
-      <c r="DN74" s="11"/>
-      <c r="DO74" s="11"/>
-      <c r="DP74" s="11"/>
-      <c r="DQ74" s="11"/>
-      <c r="DR74" s="11"/>
-      <c r="DS74" s="11"/>
-      <c r="DT74" s="11"/>
-      <c r="DU74" s="11"/>
-      <c r="DV74" s="11"/>
-      <c r="DW74" s="11"/>
-      <c r="DX74" s="11"/>
-      <c r="DY74" s="11"/>
-      <c r="DZ74" s="11"/>
-      <c r="EA74" s="11"/>
-      <c r="EB74" s="11"/>
-      <c r="EC74" s="11"/>
-      <c r="ED74" s="11"/>
-      <c r="EE74" s="11"/>
-      <c r="EF74" s="11"/>
-      <c r="EG74" s="11"/>
-      <c r="EH74" s="11"/>
-      <c r="EI74" s="11"/>
-      <c r="EJ74" s="11"/>
-      <c r="EK74" s="11"/>
-      <c r="EL74" s="11"/>
-      <c r="EM74" s="11"/>
-      <c r="EN74" s="11"/>
-      <c r="EO74" s="11"/>
-      <c r="EP74" s="11"/>
-      <c r="EQ74" s="11"/>
-      <c r="ER74" s="11"/>
-      <c r="ES74" s="11"/>
-      <c r="ET74" s="11"/>
-      <c r="EU74" s="11"/>
-      <c r="EV74" s="11"/>
-      <c r="EW74" s="11"/>
-      <c r="EX74" s="11"/>
-      <c r="EY74" s="11"/>
-      <c r="EZ74" s="11"/>
-      <c r="FA74" s="11"/>
-      <c r="FB74" s="11"/>
-      <c r="FC74" s="11"/>
-      <c r="FD74" s="11"/>
-      <c r="FE74" s="11"/>
-      <c r="FF74" s="11"/>
-      <c r="FG74" s="11"/>
-      <c r="FH74" s="11"/>
-      <c r="FI74" s="11"/>
-      <c r="FJ74" s="11"/>
-      <c r="FK74" s="11"/>
-      <c r="FL74" s="11"/>
-      <c r="FM74" s="11"/>
-      <c r="FN74" s="11"/>
-      <c r="FO74" s="11"/>
-      <c r="FP74" s="11"/>
-      <c r="FQ74" s="11"/>
-      <c r="FR74" s="11"/>
-      <c r="FS74" s="11"/>
-      <c r="FT74" s="11"/>
-      <c r="FU74" s="11"/>
-      <c r="FV74" s="11"/>
-      <c r="FW74" s="11"/>
-      <c r="FX74" s="11"/>
-      <c r="FY74" s="11"/>
-      <c r="FZ74" s="11"/>
-      <c r="GA74" s="11"/>
-      <c r="GB74" s="11"/>
-      <c r="GC74" s="11"/>
-      <c r="GD74" s="11"/>
-      <c r="GE74" s="11"/>
-      <c r="GF74" s="11"/>
-      <c r="GG74" s="11"/>
-      <c r="GH74" s="11"/>
-      <c r="GI74" s="11"/>
-      <c r="GJ74" s="11"/>
-      <c r="GK74" s="11"/>
-      <c r="GL74" s="11"/>
-      <c r="GM74" s="11"/>
-      <c r="GN74" s="11"/>
-      <c r="GO74" s="11"/>
-      <c r="GP74" s="11"/>
-      <c r="GQ74" s="11"/>
-      <c r="GR74" s="11"/>
-      <c r="GS74" s="11"/>
-      <c r="GT74" s="11"/>
-      <c r="GU74" s="11"/>
-      <c r="GV74" s="11"/>
-      <c r="GW74" s="11"/>
-      <c r="GX74" s="11"/>
-      <c r="GY74" s="11"/>
-      <c r="GZ74" s="11"/>
-      <c r="HA74" s="11"/>
-      <c r="HB74" s="11"/>
-      <c r="HC74" s="11"/>
-      <c r="HD74" s="11"/>
-      <c r="HE74" s="11"/>
-      <c r="HF74" s="11"/>
-      <c r="HG74" s="11"/>
-      <c r="HH74" s="11"/>
-      <c r="HI74" s="11"/>
-      <c r="HJ74" s="11"/>
-      <c r="HK74" s="11"/>
-      <c r="HL74" s="11"/>
-      <c r="HM74" s="11"/>
-      <c r="HN74" s="11"/>
-      <c r="HO74" s="11"/>
-      <c r="HP74" s="11"/>
-      <c r="HQ74" s="11"/>
-      <c r="HR74" s="11"/>
-      <c r="HS74" s="11"/>
-      <c r="HT74" s="11"/>
-      <c r="HU74" s="11"/>
-      <c r="HV74" s="11"/>
-      <c r="HW74" s="11"/>
-      <c r="HX74" s="11"/>
-      <c r="HY74" s="11"/>
-      <c r="HZ74" s="11"/>
-      <c r="IA74" s="11"/>
-      <c r="IB74" s="11"/>
-      <c r="IC74" s="11"/>
-      <c r="ID74" s="11"/>
-      <c r="IE74" s="11"/>
-      <c r="IF74" s="11"/>
-      <c r="IG74" s="11"/>
-      <c r="IH74" s="11"/>
-      <c r="II74" s="11"/>
-      <c r="IJ74" s="11"/>
-      <c r="IK74" s="11"/>
-      <c r="IL74" s="11"/>
-      <c r="IM74" s="11"/>
-      <c r="IN74" s="11"/>
-      <c r="IO74" s="11"/>
-      <c r="IP74" s="11"/>
-      <c r="IQ74" s="11"/>
-      <c r="IR74" s="11"/>
-      <c r="IS74" s="11"/>
-      <c r="IT74" s="11"/>
-      <c r="IU74" s="11"/>
-      <c r="IV74" s="11"/>
-      <c r="IW74" s="11"/>
-      <c r="IX74" s="11"/>
-      <c r="IY74" s="11"/>
-      <c r="IZ74" s="11"/>
-      <c r="JA74" s="11"/>
-      <c r="JB74" s="11"/>
-      <c r="JC74" s="11"/>
-      <c r="JD74" s="11"/>
-      <c r="JE74" s="11"/>
-      <c r="JF74" s="11"/>
-      <c r="JG74" s="11"/>
-      <c r="JH74" s="11"/>
-      <c r="JI74" s="11"/>
-      <c r="JJ74" s="11"/>
-      <c r="JK74" s="11"/>
-      <c r="JL74" s="11"/>
-      <c r="JM74" s="11"/>
-      <c r="JN74" s="11"/>
-      <c r="JO74" s="11"/>
-      <c r="JP74" s="11"/>
-      <c r="JQ74" s="11"/>
-      <c r="JR74" s="11"/>
-      <c r="JS74" s="11"/>
-      <c r="JT74" s="11"/>
-      <c r="JU74" s="11"/>
-      <c r="JV74" s="11"/>
-      <c r="JW74" s="11"/>
-      <c r="JX74" s="11"/>
-      <c r="JY74" s="11"/>
-      <c r="JZ74" s="11"/>
-      <c r="KA74" s="11"/>
-      <c r="KB74" s="11"/>
-      <c r="KC74" s="11"/>
-      <c r="KD74" s="11"/>
-      <c r="KE74" s="11"/>
-      <c r="KF74" s="11"/>
-      <c r="KG74" s="11"/>
-      <c r="KH74" s="11"/>
-      <c r="KI74" s="11"/>
-      <c r="KJ74" s="11"/>
-      <c r="KK74" s="11"/>
-      <c r="KL74" s="11"/>
-      <c r="KM74" s="11"/>
-      <c r="KN74" s="11"/>
-      <c r="KO74" s="11"/>
-      <c r="KP74" s="11"/>
-      <c r="KQ74" s="11"/>
-      <c r="KR74" s="11"/>
-      <c r="KS74" s="11"/>
-      <c r="KT74" s="11"/>
-      <c r="KU74" s="11"/>
-      <c r="KV74" s="11"/>
-      <c r="KW74" s="11"/>
-      <c r="KX74" s="11"/>
-      <c r="KY74" s="11"/>
-      <c r="KZ74" s="11"/>
-      <c r="LA74" s="11"/>
-      <c r="LB74" s="11"/>
-      <c r="LC74" s="11"/>
-      <c r="LD74" s="11"/>
-      <c r="LE74" s="11"/>
-      <c r="LF74" s="11"/>
-      <c r="LG74" s="11"/>
-      <c r="LH74" s="11"/>
-      <c r="LI74" s="11"/>
-      <c r="LJ74" s="11"/>
-      <c r="LK74" s="11"/>
-      <c r="LL74" s="11"/>
-      <c r="LM74" s="11"/>
-      <c r="LN74" s="11"/>
-      <c r="LO74" s="11"/>
-      <c r="LP74" s="11"/>
-      <c r="LQ74" s="11"/>
-      <c r="LR74" s="11"/>
-      <c r="LS74" s="11"/>
-      <c r="LT74" s="11"/>
-      <c r="LU74" s="11"/>
-      <c r="LV74" s="11"/>
-      <c r="LW74" s="11"/>
-      <c r="LX74" s="11"/>
-      <c r="LY74" s="11"/>
-      <c r="LZ74" s="11"/>
-      <c r="MA74" s="11"/>
-      <c r="MB74" s="11"/>
-      <c r="MC74" s="11"/>
-      <c r="MD74" s="11"/>
-      <c r="ME74" s="11"/>
-      <c r="MF74" s="11"/>
-      <c r="MG74" s="11"/>
-      <c r="MH74" s="11"/>
-      <c r="MI74" s="11"/>
-      <c r="MJ74" s="11"/>
-      <c r="MK74" s="11"/>
-      <c r="ML74" s="11"/>
-      <c r="MM74" s="11"/>
-      <c r="MN74" s="11"/>
-      <c r="MO74" s="11"/>
-      <c r="MP74" s="11"/>
-      <c r="MQ74" s="11"/>
-      <c r="MR74" s="11"/>
-      <c r="MS74" s="11"/>
-      <c r="MT74" s="11"/>
-      <c r="MU74" s="11"/>
-      <c r="MV74" s="11"/>
-      <c r="MW74" s="11"/>
-      <c r="MX74" s="11"/>
-      <c r="MY74" s="11"/>
-      <c r="MZ74" s="11"/>
-      <c r="NA74" s="11"/>
-      <c r="NB74" s="11"/>
-      <c r="NC74" s="11"/>
-      <c r="ND74" s="11"/>
-      <c r="NE74" s="11"/>
-      <c r="NF74" s="11"/>
-      <c r="NG74" s="11"/>
-      <c r="NH74" s="11"/>
-      <c r="NI74" s="11"/>
-      <c r="NJ74" s="11"/>
-      <c r="NK74" s="11"/>
-      <c r="NL74" s="11"/>
-      <c r="NM74" s="11"/>
-      <c r="NN74" s="11"/>
-      <c r="NO74" s="11"/>
-      <c r="NP74" s="11"/>
-      <c r="NQ74" s="11"/>
-      <c r="NR74" s="11"/>
-      <c r="NS74" s="11"/>
-      <c r="NT74" s="11"/>
-      <c r="NU74" s="11"/>
-      <c r="NV74" s="11"/>
-      <c r="NW74" s="11"/>
-      <c r="NX74" s="11"/>
-      <c r="NY74" s="11"/>
-      <c r="NZ74" s="11"/>
-      <c r="OA74" s="11"/>
-      <c r="OB74" s="11"/>
-      <c r="OC74" s="11"/>
-      <c r="OD74" s="11"/>
-      <c r="OE74" s="11"/>
-      <c r="OF74" s="11"/>
-      <c r="OG74" s="11"/>
-      <c r="OH74" s="11"/>
-      <c r="OI74" s="11"/>
-      <c r="OJ74" s="11"/>
-      <c r="OK74" s="11"/>
-      <c r="OL74" s="11"/>
-      <c r="OM74" s="11"/>
-      <c r="ON74" s="11"/>
-      <c r="OO74" s="11"/>
-      <c r="OP74" s="11"/>
-      <c r="OQ74" s="11"/>
-      <c r="OR74" s="11"/>
-      <c r="OS74" s="11"/>
-      <c r="OT74" s="11"/>
-      <c r="OU74" s="11"/>
-      <c r="OV74" s="11"/>
-      <c r="OW74" s="11"/>
-      <c r="OX74" s="11"/>
-      <c r="OY74" s="11"/>
-      <c r="OZ74" s="11"/>
-      <c r="PA74" s="11"/>
-      <c r="PB74" s="11"/>
-      <c r="PC74" s="11"/>
-      <c r="PD74" s="11"/>
-      <c r="PE74" s="11"/>
-      <c r="PF74" s="11"/>
-      <c r="PG74" s="11"/>
-      <c r="PH74" s="11"/>
-      <c r="PI74" s="11"/>
-      <c r="PJ74" s="11"/>
-      <c r="PK74" s="11"/>
-      <c r="PL74" s="11"/>
-      <c r="PM74" s="11"/>
-      <c r="PN74" s="11"/>
-      <c r="PO74" s="11"/>
-      <c r="PP74" s="11"/>
-      <c r="PQ74" s="11"/>
-      <c r="PR74" s="11"/>
-      <c r="PS74" s="11"/>
-      <c r="PT74" s="11"/>
-      <c r="PU74" s="11"/>
-      <c r="PV74" s="11"/>
-      <c r="PW74" s="11"/>
-      <c r="PX74" s="11"/>
-      <c r="PY74" s="11"/>
-      <c r="PZ74" s="11"/>
-      <c r="QA74" s="11"/>
-      <c r="QB74" s="11"/>
-      <c r="QC74" s="11"/>
-      <c r="QD74" s="11"/>
-      <c r="QE74" s="11"/>
-      <c r="QF74" s="11"/>
-      <c r="QG74" s="11"/>
-      <c r="QH74" s="11"/>
-      <c r="QI74" s="11"/>
-      <c r="QJ74" s="11"/>
-      <c r="QK74" s="11"/>
-      <c r="QL74" s="11"/>
-      <c r="QM74" s="11"/>
-      <c r="QN74" s="11"/>
-      <c r="QO74" s="11"/>
-      <c r="QP74" s="11"/>
-      <c r="QQ74" s="11"/>
-      <c r="QR74" s="11"/>
-      <c r="QS74" s="11"/>
-      <c r="QT74" s="11"/>
-      <c r="QU74" s="11"/>
-      <c r="QV74" s="11"/>
-      <c r="QW74" s="11"/>
-      <c r="QX74" s="11"/>
-      <c r="QY74" s="11"/>
-      <c r="QZ74" s="11"/>
-      <c r="RA74" s="11"/>
-      <c r="RB74" s="11"/>
-      <c r="RC74" s="11"/>
-      <c r="RD74" s="11"/>
-      <c r="RE74" s="11"/>
-      <c r="RF74" s="11"/>
-      <c r="RG74" s="11"/>
-      <c r="RH74" s="11"/>
-      <c r="RI74" s="11"/>
-      <c r="RJ74" s="11"/>
-      <c r="RK74" s="11"/>
-      <c r="RL74" s="11"/>
-      <c r="RM74" s="11"/>
-      <c r="RN74" s="11"/>
-      <c r="RO74" s="11"/>
-      <c r="RP74" s="11"/>
-      <c r="RQ74" s="11"/>
-      <c r="RR74" s="11"/>
-      <c r="RS74" s="11"/>
-      <c r="RT74" s="11"/>
-      <c r="RU74" s="11"/>
-      <c r="RV74" s="11"/>
-      <c r="RW74" s="11"/>
-      <c r="RX74" s="11"/>
-      <c r="RY74" s="11"/>
-      <c r="RZ74" s="11"/>
-      <c r="SA74" s="11"/>
-      <c r="SB74" s="11"/>
-      <c r="SC74" s="11"/>
-      <c r="SD74" s="11"/>
-      <c r="SE74" s="11"/>
-      <c r="SF74" s="11"/>
-      <c r="SG74" s="11"/>
-      <c r="SH74" s="11"/>
-      <c r="SI74" s="11"/>
-      <c r="SJ74" s="11"/>
-      <c r="SK74" s="11"/>
-      <c r="SL74" s="11"/>
-      <c r="SM74" s="11"/>
-      <c r="SN74" s="11"/>
-      <c r="SO74" s="11"/>
-      <c r="SP74" s="11"/>
-      <c r="SQ74" s="11"/>
-      <c r="SR74" s="11"/>
-      <c r="SS74" s="11"/>
-      <c r="ST74" s="11"/>
-      <c r="SU74" s="11"/>
-      <c r="SV74" s="11"/>
-      <c r="SW74" s="11"/>
-      <c r="SX74" s="11"/>
-      <c r="SY74" s="11"/>
-      <c r="SZ74" s="11"/>
-      <c r="TA74" s="11"/>
-      <c r="TB74" s="11"/>
-      <c r="TC74" s="11"/>
-      <c r="TD74" s="11"/>
-      <c r="TE74" s="11"/>
-      <c r="TF74" s="11"/>
-      <c r="TG74" s="11"/>
-      <c r="TH74" s="11"/>
-      <c r="TI74" s="11"/>
-      <c r="TJ74" s="11"/>
-      <c r="TK74" s="11"/>
-      <c r="TL74" s="11"/>
-      <c r="TM74" s="11"/>
-      <c r="TN74" s="11"/>
-      <c r="TO74" s="11"/>
-      <c r="TP74" s="11"/>
-      <c r="TQ74" s="11"/>
-      <c r="TR74" s="11"/>
-      <c r="TS74" s="11"/>
-      <c r="TT74" s="11"/>
-      <c r="TU74" s="11"/>
-      <c r="TV74" s="11"/>
-      <c r="TW74" s="11"/>
-      <c r="TX74" s="11"/>
-      <c r="TY74" s="11"/>
-      <c r="TZ74" s="11"/>
-      <c r="UA74" s="11"/>
-      <c r="UB74" s="11"/>
-      <c r="UC74" s="11"/>
-      <c r="UD74" s="11"/>
-      <c r="UE74" s="11"/>
-      <c r="UF74" s="11"/>
-      <c r="UG74" s="11"/>
-      <c r="UH74" s="11"/>
-      <c r="UI74" s="11"/>
-      <c r="UJ74" s="11"/>
-      <c r="UK74" s="11"/>
-      <c r="UL74" s="11"/>
-      <c r="UM74" s="11"/>
-      <c r="UN74" s="11"/>
-      <c r="UO74" s="11"/>
-      <c r="UP74" s="11"/>
-      <c r="UQ74" s="11"/>
-      <c r="UR74" s="11"/>
-      <c r="US74" s="11"/>
-      <c r="UT74" s="11"/>
-      <c r="UU74" s="11"/>
-      <c r="UV74" s="11"/>
-      <c r="UW74" s="11"/>
-      <c r="UX74" s="11"/>
-      <c r="UY74" s="11"/>
-      <c r="UZ74" s="11"/>
-      <c r="VA74" s="11"/>
-      <c r="VB74" s="11"/>
-      <c r="VC74" s="11"/>
-      <c r="VD74" s="11"/>
-      <c r="VE74" s="11"/>
-      <c r="VF74" s="11"/>
-      <c r="VG74" s="11"/>
-      <c r="VH74" s="11"/>
-      <c r="VI74" s="11"/>
-      <c r="VJ74" s="11"/>
-      <c r="VK74" s="11"/>
-      <c r="VL74" s="11"/>
-      <c r="VM74" s="11"/>
-      <c r="VN74" s="11"/>
-      <c r="VO74" s="11"/>
-      <c r="VP74" s="11"/>
-      <c r="VQ74" s="11"/>
-      <c r="VR74" s="11"/>
-      <c r="VS74" s="11"/>
-      <c r="VT74" s="11"/>
-      <c r="VU74" s="11"/>
-      <c r="VV74" s="11"/>
-      <c r="VW74" s="11"/>
-      <c r="VX74" s="11"/>
-      <c r="VY74" s="11"/>
-      <c r="VZ74" s="11"/>
-      <c r="WA74" s="11"/>
-      <c r="WB74" s="11"/>
-      <c r="WC74" s="11"/>
-      <c r="WD74" s="11"/>
-      <c r="WE74" s="11"/>
-      <c r="WF74" s="11"/>
-      <c r="WG74" s="11"/>
-      <c r="WH74" s="11"/>
-      <c r="WI74" s="11"/>
-      <c r="WJ74" s="11"/>
-      <c r="WK74" s="11"/>
-      <c r="WL74" s="11"/>
-      <c r="WM74" s="11"/>
-      <c r="WN74" s="11"/>
-      <c r="WO74" s="11"/>
-      <c r="WP74" s="11"/>
-      <c r="WQ74" s="11"/>
-      <c r="WR74" s="11"/>
-      <c r="WS74" s="11"/>
-      <c r="WT74" s="11"/>
-      <c r="WU74" s="11"/>
-      <c r="WV74" s="11"/>
-      <c r="WW74" s="11"/>
-      <c r="WX74" s="11"/>
-      <c r="WY74" s="11"/>
-      <c r="WZ74" s="11"/>
-      <c r="XA74" s="11"/>
-      <c r="XB74" s="11"/>
-      <c r="XC74" s="11"/>
-      <c r="XD74" s="11"/>
-      <c r="XE74" s="11"/>
-      <c r="XF74" s="11"/>
-      <c r="XG74" s="11"/>
-      <c r="XH74" s="11"/>
-      <c r="XI74" s="11"/>
-      <c r="XJ74" s="11"/>
-      <c r="XK74" s="11"/>
-      <c r="XL74" s="11"/>
-      <c r="XM74" s="11"/>
-      <c r="XN74" s="11"/>
-      <c r="XO74" s="11"/>
-      <c r="XP74" s="11"/>
-      <c r="XQ74" s="11"/>
-      <c r="XR74" s="11"/>
-      <c r="XS74" s="11"/>
-      <c r="XT74" s="11"/>
-      <c r="XU74" s="11"/>
-      <c r="XV74" s="11"/>
-      <c r="XW74" s="11"/>
-      <c r="XX74" s="11"/>
-      <c r="XY74" s="11"/>
-      <c r="XZ74" s="11"/>
-      <c r="YA74" s="11"/>
-      <c r="YB74" s="11"/>
-      <c r="YC74" s="11"/>
-      <c r="YD74" s="11"/>
-      <c r="YE74" s="11"/>
-      <c r="YF74" s="11"/>
-      <c r="YG74" s="11"/>
-      <c r="YH74" s="11"/>
-      <c r="YI74" s="11"/>
-      <c r="YJ74" s="11"/>
-      <c r="YK74" s="11"/>
-      <c r="YL74" s="11"/>
-      <c r="YM74" s="11"/>
-      <c r="YN74" s="11"/>
-      <c r="YO74" s="11"/>
-      <c r="YP74" s="11"/>
-      <c r="YQ74" s="11"/>
-      <c r="YR74" s="11"/>
-      <c r="YS74" s="11"/>
-      <c r="YT74" s="11"/>
-      <c r="YU74" s="11"/>
-      <c r="YV74" s="11"/>
-      <c r="YW74" s="11"/>
-      <c r="YX74" s="11"/>
-      <c r="YY74" s="11"/>
-      <c r="YZ74" s="11"/>
-      <c r="ZA74" s="11"/>
-      <c r="ZB74" s="11"/>
-      <c r="ZC74" s="11"/>
-      <c r="ZD74" s="11"/>
-      <c r="ZE74" s="11"/>
-      <c r="ZF74" s="11"/>
-      <c r="ZG74" s="11"/>
-      <c r="ZH74" s="11"/>
-      <c r="ZI74" s="11"/>
-      <c r="ZJ74" s="11"/>
-      <c r="ZK74" s="11"/>
-      <c r="ZL74" s="11"/>
-      <c r="ZM74" s="11"/>
-      <c r="ZN74" s="11"/>
-      <c r="ZO74" s="11"/>
-      <c r="ZP74" s="11"/>
-      <c r="ZQ74" s="11"/>
-      <c r="ZR74" s="11"/>
-      <c r="ZS74" s="11"/>
-      <c r="ZT74" s="11"/>
-      <c r="ZU74" s="11"/>
-      <c r="ZV74" s="11"/>
-      <c r="ZW74" s="11"/>
-      <c r="ZX74" s="11"/>
-      <c r="ZY74" s="11"/>
-      <c r="ZZ74" s="11"/>
-      <c r="AAA74" s="11"/>
-      <c r="AAB74" s="11"/>
-      <c r="AAC74" s="11"/>
-      <c r="AAD74" s="11"/>
-      <c r="AAE74" s="11"/>
-      <c r="AAF74" s="11"/>
-      <c r="AAG74" s="11"/>
-      <c r="AAH74" s="11"/>
-      <c r="AAI74" s="11"/>
-      <c r="AAJ74" s="11"/>
-      <c r="AAK74" s="11"/>
-      <c r="AAL74" s="11"/>
-      <c r="AAM74" s="11"/>
-      <c r="AAN74" s="11"/>
-      <c r="AAO74" s="11"/>
-      <c r="AAP74" s="11"/>
-      <c r="AAQ74" s="11"/>
-      <c r="AAR74" s="11"/>
-      <c r="AAS74" s="11"/>
-      <c r="AAT74" s="11"/>
-      <c r="AAU74" s="11"/>
-      <c r="AAV74" s="11"/>
-      <c r="AAW74" s="11"/>
-      <c r="AAX74" s="11"/>
-      <c r="AAY74" s="11"/>
-      <c r="AAZ74" s="11"/>
-      <c r="ABA74" s="11"/>
-      <c r="ABB74" s="11"/>
-      <c r="ABC74" s="11"/>
-      <c r="ABD74" s="11"/>
-      <c r="ABE74" s="11"/>
-      <c r="ABF74" s="11"/>
-      <c r="ABG74" s="11"/>
-      <c r="ABH74" s="11"/>
-      <c r="ABI74" s="11"/>
-      <c r="ABJ74" s="11"/>
-      <c r="ABK74" s="11"/>
-      <c r="ABL74" s="11"/>
-      <c r="ABM74" s="11"/>
-      <c r="ABN74" s="11"/>
-      <c r="ABO74" s="11"/>
-      <c r="ABP74" s="11"/>
-      <c r="ABQ74" s="11"/>
-      <c r="ABR74" s="11"/>
-      <c r="ABS74" s="11"/>
-      <c r="ABT74" s="11"/>
-      <c r="ABU74" s="11"/>
-      <c r="ABV74" s="11"/>
-      <c r="ABW74" s="11"/>
-      <c r="ABX74" s="11"/>
-      <c r="ABY74" s="11"/>
-      <c r="ABZ74" s="11"/>
-      <c r="ACA74" s="11"/>
-      <c r="ACB74" s="11"/>
-      <c r="ACC74" s="11"/>
-      <c r="ACD74" s="11"/>
-      <c r="ACE74" s="11"/>
-      <c r="ACF74" s="11"/>
-      <c r="ACG74" s="11"/>
-      <c r="ACH74" s="11"/>
-      <c r="ACI74" s="11"/>
-      <c r="ACJ74" s="11"/>
-      <c r="ACK74" s="11"/>
-      <c r="ACL74" s="11"/>
-      <c r="ACM74" s="11"/>
-      <c r="ACN74" s="11"/>
-      <c r="ACO74" s="11"/>
-      <c r="ACP74" s="11"/>
-      <c r="ACQ74" s="11"/>
-      <c r="ACR74" s="11"/>
-      <c r="ACS74" s="11"/>
-      <c r="ACT74" s="11"/>
-      <c r="ACU74" s="11"/>
-      <c r="ACV74" s="11"/>
-      <c r="ACW74" s="11"/>
-      <c r="ACX74" s="11"/>
-      <c r="ACY74" s="11"/>
-      <c r="ACZ74" s="11"/>
-      <c r="ADA74" s="11"/>
-      <c r="ADB74" s="11"/>
-      <c r="ADC74" s="11"/>
-      <c r="ADD74" s="11"/>
-      <c r="ADE74" s="11"/>
-      <c r="ADF74" s="11"/>
-      <c r="ADG74" s="11"/>
-      <c r="ADH74" s="11"/>
-      <c r="ADI74" s="11"/>
-      <c r="ADJ74" s="11"/>
-      <c r="ADK74" s="11"/>
-      <c r="ADL74" s="11"/>
-      <c r="ADM74" s="11"/>
-      <c r="ADN74" s="11"/>
-      <c r="ADO74" s="11"/>
-      <c r="ADP74" s="11"/>
-      <c r="ADQ74" s="11"/>
-      <c r="ADR74" s="11"/>
-      <c r="ADS74" s="11"/>
-      <c r="ADT74" s="11"/>
-      <c r="ADU74" s="11"/>
-      <c r="ADV74" s="11"/>
-      <c r="ADW74" s="11"/>
-      <c r="ADX74" s="11"/>
-      <c r="ADY74" s="11"/>
-      <c r="ADZ74" s="11"/>
-      <c r="AEA74" s="11"/>
-      <c r="AEB74" s="11"/>
-      <c r="AEC74" s="11"/>
-      <c r="AED74" s="11"/>
-      <c r="AEE74" s="11"/>
-      <c r="AEF74" s="11"/>
-      <c r="AEG74" s="11"/>
-      <c r="AEH74" s="11"/>
-      <c r="AEI74" s="11"/>
-      <c r="AEJ74" s="11"/>
-      <c r="AEK74" s="11"/>
-      <c r="AEL74" s="11"/>
-      <c r="AEM74" s="11"/>
-      <c r="AEN74" s="11"/>
-      <c r="AEO74" s="11"/>
-      <c r="AEP74" s="11"/>
-      <c r="AEQ74" s="11"/>
-      <c r="AER74" s="11"/>
-      <c r="AES74" s="11"/>
-      <c r="AET74" s="11"/>
-      <c r="AEU74" s="11"/>
-      <c r="AEV74" s="11"/>
-      <c r="AEW74" s="11"/>
-      <c r="AEX74" s="11"/>
-      <c r="AEY74" s="11"/>
-      <c r="AEZ74" s="11"/>
-      <c r="AFA74" s="11"/>
-      <c r="AFB74" s="11"/>
-      <c r="AFC74" s="11"/>
-      <c r="AFD74" s="11"/>
-      <c r="AFE74" s="11"/>
-      <c r="AFF74" s="11"/>
-      <c r="AFG74" s="11"/>
-      <c r="AFH74" s="11"/>
-      <c r="AFI74" s="11"/>
-      <c r="AFJ74" s="11"/>
-      <c r="AFK74" s="11"/>
-      <c r="AFL74" s="11"/>
-      <c r="AFM74" s="11"/>
-      <c r="AFN74" s="11"/>
-      <c r="AFO74" s="11"/>
-      <c r="AFP74" s="11"/>
-      <c r="AFQ74" s="11"/>
-      <c r="AFR74" s="11"/>
-      <c r="AFS74" s="11"/>
-      <c r="AFT74" s="11"/>
-      <c r="AFU74" s="11"/>
-      <c r="AFV74" s="11"/>
-      <c r="AFW74" s="11"/>
-      <c r="AFX74" s="11"/>
-      <c r="AFY74" s="11"/>
-      <c r="AFZ74" s="11"/>
-      <c r="AGA74" s="11"/>
-      <c r="AGB74" s="11"/>
-      <c r="AGC74" s="11"/>
-      <c r="AGD74" s="11"/>
-      <c r="AGE74" s="11"/>
-      <c r="AGF74" s="11"/>
-      <c r="AGG74" s="11"/>
-      <c r="AGH74" s="11"/>
-      <c r="AGI74" s="11"/>
-      <c r="AGJ74" s="11"/>
-      <c r="AGK74" s="11"/>
-      <c r="AGL74" s="11"/>
-      <c r="AGM74" s="11"/>
-      <c r="AGN74" s="11"/>
-      <c r="AGO74" s="11"/>
-      <c r="AGP74" s="11"/>
-      <c r="AGQ74" s="11"/>
-      <c r="AGR74" s="11"/>
-      <c r="AGS74" s="11"/>
-      <c r="AGT74" s="11"/>
-      <c r="AGU74" s="11"/>
-      <c r="AGV74" s="11"/>
-      <c r="AGW74" s="11"/>
-      <c r="AGX74" s="11"/>
-      <c r="AGY74" s="11"/>
-      <c r="AGZ74" s="11"/>
-      <c r="AHA74" s="11"/>
-      <c r="AHB74" s="11"/>
-      <c r="AHC74" s="11"/>
-      <c r="AHD74" s="11"/>
-      <c r="AHE74" s="11"/>
-      <c r="AHF74" s="11"/>
-      <c r="AHG74" s="11"/>
-      <c r="AHH74" s="11"/>
-      <c r="AHI74" s="11"/>
-      <c r="AHJ74" s="11"/>
-      <c r="AHK74" s="11"/>
-      <c r="AHL74" s="11"/>
-      <c r="AHM74" s="11"/>
-      <c r="AHN74" s="11"/>
-      <c r="AHO74" s="11"/>
-      <c r="AHP74" s="11"/>
-      <c r="AHQ74" s="11"/>
-      <c r="AHR74" s="11"/>
-      <c r="AHS74" s="11"/>
-      <c r="AHT74" s="11"/>
-      <c r="AHU74" s="11"/>
-      <c r="AHV74" s="11"/>
-      <c r="AHW74" s="11"/>
-      <c r="AHX74" s="11"/>
-      <c r="AHY74" s="11"/>
-      <c r="AHZ74" s="11"/>
-      <c r="AIA74" s="11"/>
-      <c r="AIB74" s="11"/>
-      <c r="AIC74" s="11"/>
-      <c r="AID74" s="11"/>
-      <c r="AIE74" s="11"/>
-      <c r="AIF74" s="11"/>
-      <c r="AIG74" s="11"/>
-      <c r="AIH74" s="11"/>
-      <c r="AII74" s="11"/>
-      <c r="AIJ74" s="11"/>
-      <c r="AIK74" s="11"/>
-      <c r="AIL74" s="11"/>
-      <c r="AIM74" s="11"/>
-      <c r="AIN74" s="11"/>
-      <c r="AIO74" s="11"/>
-      <c r="AIP74" s="11"/>
-      <c r="AIQ74" s="11"/>
-      <c r="AIR74" s="11"/>
-      <c r="AIS74" s="11"/>
-      <c r="AIT74" s="11"/>
-      <c r="AIU74" s="11"/>
-      <c r="AIV74" s="11"/>
-      <c r="AIW74" s="11"/>
-      <c r="AIX74" s="11"/>
-      <c r="AIY74" s="11"/>
-      <c r="AIZ74" s="11"/>
-      <c r="AJA74" s="11"/>
-      <c r="AJB74" s="11"/>
-      <c r="AJC74" s="11"/>
-      <c r="AJD74" s="11"/>
-      <c r="AJE74" s="11"/>
-      <c r="AJF74" s="11"/>
-      <c r="AJG74" s="11"/>
-      <c r="AJH74" s="11"/>
-      <c r="AJI74" s="11"/>
-      <c r="AJJ74" s="11"/>
-      <c r="AJK74" s="11"/>
-      <c r="AJL74" s="11"/>
-      <c r="AJM74" s="11"/>
-      <c r="AJN74" s="11"/>
-      <c r="AJO74" s="11"/>
-      <c r="AJP74" s="11"/>
-      <c r="AJQ74" s="11"/>
-      <c r="AJR74" s="11"/>
-      <c r="AJS74" s="11"/>
-      <c r="AJT74" s="11"/>
-      <c r="AJU74" s="11"/>
-      <c r="AJV74" s="11"/>
-      <c r="AJW74" s="11"/>
-      <c r="AJX74" s="11"/>
-      <c r="AJY74" s="11"/>
-      <c r="AJZ74" s="11"/>
-      <c r="AKA74" s="11"/>
-      <c r="AKB74" s="11"/>
-      <c r="AKC74" s="11"/>
-      <c r="AKD74" s="11"/>
-      <c r="AKE74" s="11"/>
-      <c r="AKF74" s="11"/>
-      <c r="AKG74" s="11"/>
-      <c r="AKH74" s="11"/>
-      <c r="AKI74" s="11"/>
-      <c r="AKJ74" s="11"/>
-      <c r="AKK74" s="11"/>
-      <c r="AKL74" s="11"/>
-      <c r="AKM74" s="11"/>
-      <c r="AKN74" s="11"/>
-      <c r="AKO74" s="11"/>
-      <c r="AKP74" s="11"/>
-      <c r="AKQ74" s="11"/>
-      <c r="AKR74" s="11"/>
-      <c r="AKS74" s="11"/>
-      <c r="AKT74" s="11"/>
-      <c r="AKU74" s="11"/>
-      <c r="AKV74" s="11"/>
-      <c r="AKW74" s="11"/>
-      <c r="AKX74" s="11"/>
-      <c r="AKY74" s="11"/>
-      <c r="AKZ74" s="11"/>
-      <c r="ALA74" s="11"/>
-      <c r="ALB74" s="11"/>
-      <c r="ALC74" s="11"/>
-      <c r="ALD74" s="11"/>
-      <c r="ALE74" s="11"/>
-      <c r="ALF74" s="11"/>
-      <c r="ALG74" s="11"/>
-      <c r="ALH74" s="11"/>
-      <c r="ALI74" s="11"/>
-      <c r="ALJ74" s="11"/>
-      <c r="ALK74" s="11"/>
-      <c r="ALL74" s="11"/>
-      <c r="ALM74" s="11"/>
-      <c r="ALN74" s="11"/>
-      <c r="ALO74" s="11"/>
-      <c r="ALP74" s="11"/>
-      <c r="ALQ74" s="11"/>
-      <c r="ALR74" s="11"/>
-      <c r="ALS74" s="11"/>
-      <c r="ALT74" s="11"/>
-      <c r="ALU74" s="11"/>
-      <c r="ALV74" s="11"/>
-      <c r="ALW74" s="11"/>
-      <c r="ALX74" s="11"/>
-      <c r="ALY74" s="11"/>
-      <c r="ALZ74" s="11"/>
-      <c r="AMA74" s="11"/>
-      <c r="AMB74" s="11"/>
-      <c r="AMC74" s="11"/>
-      <c r="AMD74" s="11"/>
-      <c r="AME74" s="11"/>
-      <c r="AMF74" s="11"/>
-      <c r="AMG74" s="11"/>
-      <c r="AMH74" s="11"/>
-      <c r="AMI74" s="11"/>
-      <c r="AMJ74" s="11"/>
-    </row>
+    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="11"/>
+      <c r="P71" s="11"/>
+      <c r="Q71" s="11"/>
+      <c r="R71" s="11"/>
+      <c r="S71" s="11"/>
+      <c r="T71" s="11"/>
+      <c r="U71" s="11"/>
+      <c r="V71" s="11"/>
+      <c r="W71" s="11"/>
+      <c r="X71" s="11"/>
+      <c r="Y71" s="11"/>
+      <c r="Z71" s="11"/>
+      <c r="AA71" s="11"/>
+      <c r="AB71" s="11"/>
+      <c r="AC71" s="11"/>
+      <c r="AD71" s="11"/>
+      <c r="AE71" s="11"/>
+      <c r="AF71" s="11"/>
+      <c r="AG71" s="11"/>
+      <c r="AH71" s="11"/>
+      <c r="AI71" s="11"/>
+      <c r="AJ71" s="11"/>
+      <c r="AK71" s="11"/>
+      <c r="AL71" s="11"/>
+      <c r="AM71" s="11"/>
+      <c r="AN71" s="11"/>
+      <c r="AO71" s="11"/>
+      <c r="AP71" s="11"/>
+      <c r="AQ71" s="11"/>
+      <c r="AR71" s="11"/>
+      <c r="AS71" s="11"/>
+      <c r="AT71" s="11"/>
+      <c r="AU71" s="11"/>
+      <c r="AV71" s="11"/>
+      <c r="AW71" s="11"/>
+      <c r="AX71" s="11"/>
+      <c r="AY71" s="11"/>
+      <c r="AZ71" s="11"/>
+      <c r="BA71" s="11"/>
+      <c r="BB71" s="11"/>
+      <c r="BC71" s="11"/>
+      <c r="BD71" s="11"/>
+      <c r="BE71" s="11"/>
+      <c r="BF71" s="11"/>
+      <c r="BG71" s="11"/>
+      <c r="BH71" s="11"/>
+      <c r="BI71" s="11"/>
+      <c r="BJ71" s="11"/>
+      <c r="BK71" s="11"/>
+      <c r="BL71" s="11"/>
+      <c r="BM71" s="11"/>
+      <c r="BN71" s="11"/>
+      <c r="BO71" s="11"/>
+      <c r="BP71" s="11"/>
+      <c r="BQ71" s="11"/>
+      <c r="BR71" s="11"/>
+      <c r="BS71" s="11"/>
+      <c r="BT71" s="11"/>
+      <c r="BU71" s="11"/>
+      <c r="BV71" s="11"/>
+      <c r="BW71" s="11"/>
+      <c r="BX71" s="11"/>
+      <c r="BY71" s="11"/>
+      <c r="BZ71" s="11"/>
+      <c r="CA71" s="11"/>
+      <c r="CB71" s="11"/>
+      <c r="CC71" s="11"/>
+      <c r="CD71" s="11"/>
+      <c r="CE71" s="11"/>
+      <c r="CF71" s="11"/>
+      <c r="CG71" s="11"/>
+      <c r="CH71" s="11"/>
+      <c r="CI71" s="11"/>
+      <c r="CJ71" s="11"/>
+      <c r="CK71" s="11"/>
+      <c r="CL71" s="11"/>
+      <c r="CM71" s="11"/>
+      <c r="CN71" s="11"/>
+      <c r="CO71" s="11"/>
+      <c r="CP71" s="11"/>
+      <c r="CQ71" s="11"/>
+      <c r="CR71" s="11"/>
+      <c r="CS71" s="11"/>
+      <c r="CT71" s="11"/>
+      <c r="CU71" s="11"/>
+      <c r="CV71" s="11"/>
+      <c r="CW71" s="11"/>
+      <c r="CX71" s="11"/>
+      <c r="CY71" s="11"/>
+      <c r="CZ71" s="11"/>
+      <c r="DA71" s="11"/>
+      <c r="DB71" s="11"/>
+      <c r="DC71" s="11"/>
+      <c r="DD71" s="11"/>
+      <c r="DE71" s="11"/>
+      <c r="DF71" s="11"/>
+      <c r="DG71" s="11"/>
+      <c r="DH71" s="11"/>
+      <c r="DI71" s="11"/>
+      <c r="DJ71" s="11"/>
+      <c r="DK71" s="11"/>
+      <c r="DL71" s="11"/>
+      <c r="DM71" s="11"/>
+      <c r="DN71" s="11"/>
+      <c r="DO71" s="11"/>
+      <c r="DP71" s="11"/>
+      <c r="DQ71" s="11"/>
+      <c r="DR71" s="11"/>
+      <c r="DS71" s="11"/>
+      <c r="DT71" s="11"/>
+      <c r="DU71" s="11"/>
+      <c r="DV71" s="11"/>
+      <c r="DW71" s="11"/>
+      <c r="DX71" s="11"/>
+      <c r="DY71" s="11"/>
+      <c r="DZ71" s="11"/>
+      <c r="EA71" s="11"/>
+      <c r="EB71" s="11"/>
+      <c r="EC71" s="11"/>
+      <c r="ED71" s="11"/>
+      <c r="EE71" s="11"/>
+      <c r="EF71" s="11"/>
+      <c r="EG71" s="11"/>
+      <c r="EH71" s="11"/>
+      <c r="EI71" s="11"/>
+      <c r="EJ71" s="11"/>
+      <c r="EK71" s="11"/>
+      <c r="EL71" s="11"/>
+      <c r="EM71" s="11"/>
+      <c r="EN71" s="11"/>
+      <c r="EO71" s="11"/>
+      <c r="EP71" s="11"/>
+      <c r="EQ71" s="11"/>
+      <c r="ER71" s="11"/>
+      <c r="ES71" s="11"/>
+      <c r="ET71" s="11"/>
+      <c r="EU71" s="11"/>
+      <c r="EV71" s="11"/>
+      <c r="EW71" s="11"/>
+      <c r="EX71" s="11"/>
+      <c r="EY71" s="11"/>
+      <c r="EZ71" s="11"/>
+      <c r="FA71" s="11"/>
+      <c r="FB71" s="11"/>
+      <c r="FC71" s="11"/>
+      <c r="FD71" s="11"/>
+      <c r="FE71" s="11"/>
+      <c r="FF71" s="11"/>
+      <c r="FG71" s="11"/>
+      <c r="FH71" s="11"/>
+      <c r="FI71" s="11"/>
+      <c r="FJ71" s="11"/>
+      <c r="FK71" s="11"/>
+      <c r="FL71" s="11"/>
+      <c r="FM71" s="11"/>
+      <c r="FN71" s="11"/>
+      <c r="FO71" s="11"/>
+      <c r="FP71" s="11"/>
+      <c r="FQ71" s="11"/>
+      <c r="FR71" s="11"/>
+      <c r="FS71" s="11"/>
+      <c r="FT71" s="11"/>
+      <c r="FU71" s="11"/>
+      <c r="FV71" s="11"/>
+      <c r="FW71" s="11"/>
+      <c r="FX71" s="11"/>
+      <c r="FY71" s="11"/>
+      <c r="FZ71" s="11"/>
+      <c r="GA71" s="11"/>
+      <c r="GB71" s="11"/>
+      <c r="GC71" s="11"/>
+      <c r="GD71" s="11"/>
+      <c r="GE71" s="11"/>
+      <c r="GF71" s="11"/>
+      <c r="GG71" s="11"/>
+      <c r="GH71" s="11"/>
+      <c r="GI71" s="11"/>
+      <c r="GJ71" s="11"/>
+      <c r="GK71" s="11"/>
+      <c r="GL71" s="11"/>
+      <c r="GM71" s="11"/>
+      <c r="GN71" s="11"/>
+      <c r="GO71" s="11"/>
+      <c r="GP71" s="11"/>
+      <c r="GQ71" s="11"/>
+      <c r="GR71" s="11"/>
+      <c r="GS71" s="11"/>
+      <c r="GT71" s="11"/>
+      <c r="GU71" s="11"/>
+      <c r="GV71" s="11"/>
+      <c r="GW71" s="11"/>
+      <c r="GX71" s="11"/>
+      <c r="GY71" s="11"/>
+      <c r="GZ71" s="11"/>
+      <c r="HA71" s="11"/>
+      <c r="HB71" s="11"/>
+      <c r="HC71" s="11"/>
+      <c r="HD71" s="11"/>
+      <c r="HE71" s="11"/>
+      <c r="HF71" s="11"/>
+      <c r="HG71" s="11"/>
+      <c r="HH71" s="11"/>
+      <c r="HI71" s="11"/>
+      <c r="HJ71" s="11"/>
+      <c r="HK71" s="11"/>
+      <c r="HL71" s="11"/>
+      <c r="HM71" s="11"/>
+      <c r="HN71" s="11"/>
+      <c r="HO71" s="11"/>
+      <c r="HP71" s="11"/>
+      <c r="HQ71" s="11"/>
+      <c r="HR71" s="11"/>
+      <c r="HS71" s="11"/>
+      <c r="HT71" s="11"/>
+      <c r="HU71" s="11"/>
+      <c r="HV71" s="11"/>
+      <c r="HW71" s="11"/>
+      <c r="HX71" s="11"/>
+      <c r="HY71" s="11"/>
+      <c r="HZ71" s="11"/>
+      <c r="IA71" s="11"/>
+      <c r="IB71" s="11"/>
+      <c r="IC71" s="11"/>
+      <c r="ID71" s="11"/>
+      <c r="IE71" s="11"/>
+      <c r="IF71" s="11"/>
+      <c r="IG71" s="11"/>
+      <c r="IH71" s="11"/>
+      <c r="II71" s="11"/>
+      <c r="IJ71" s="11"/>
+      <c r="IK71" s="11"/>
+      <c r="IL71" s="11"/>
+      <c r="IM71" s="11"/>
+      <c r="IN71" s="11"/>
+      <c r="IO71" s="11"/>
+      <c r="IP71" s="11"/>
+      <c r="IQ71" s="11"/>
+      <c r="IR71" s="11"/>
+      <c r="IS71" s="11"/>
+      <c r="IT71" s="11"/>
+      <c r="IU71" s="11"/>
+      <c r="IV71" s="11"/>
+      <c r="IW71" s="11"/>
+      <c r="IX71" s="11"/>
+      <c r="IY71" s="11"/>
+      <c r="IZ71" s="11"/>
+      <c r="JA71" s="11"/>
+      <c r="JB71" s="11"/>
+      <c r="JC71" s="11"/>
+      <c r="JD71" s="11"/>
+      <c r="JE71" s="11"/>
+      <c r="JF71" s="11"/>
+      <c r="JG71" s="11"/>
+      <c r="JH71" s="11"/>
+      <c r="JI71" s="11"/>
+      <c r="JJ71" s="11"/>
+      <c r="JK71" s="11"/>
+      <c r="JL71" s="11"/>
+      <c r="JM71" s="11"/>
+      <c r="JN71" s="11"/>
+      <c r="JO71" s="11"/>
+      <c r="JP71" s="11"/>
+      <c r="JQ71" s="11"/>
+      <c r="JR71" s="11"/>
+      <c r="JS71" s="11"/>
+      <c r="JT71" s="11"/>
+      <c r="JU71" s="11"/>
+      <c r="JV71" s="11"/>
+      <c r="JW71" s="11"/>
+      <c r="JX71" s="11"/>
+      <c r="JY71" s="11"/>
+      <c r="JZ71" s="11"/>
+      <c r="KA71" s="11"/>
+      <c r="KB71" s="11"/>
+      <c r="KC71" s="11"/>
+      <c r="KD71" s="11"/>
+      <c r="KE71" s="11"/>
+      <c r="KF71" s="11"/>
+      <c r="KG71" s="11"/>
+      <c r="KH71" s="11"/>
+      <c r="KI71" s="11"/>
+      <c r="KJ71" s="11"/>
+      <c r="KK71" s="11"/>
+      <c r="KL71" s="11"/>
+      <c r="KM71" s="11"/>
+      <c r="KN71" s="11"/>
+      <c r="KO71" s="11"/>
+      <c r="KP71" s="11"/>
+      <c r="KQ71" s="11"/>
+      <c r="KR71" s="11"/>
+      <c r="KS71" s="11"/>
+      <c r="KT71" s="11"/>
+      <c r="KU71" s="11"/>
+      <c r="KV71" s="11"/>
+      <c r="KW71" s="11"/>
+      <c r="KX71" s="11"/>
+      <c r="KY71" s="11"/>
+      <c r="KZ71" s="11"/>
+      <c r="LA71" s="11"/>
+      <c r="LB71" s="11"/>
+      <c r="LC71" s="11"/>
+      <c r="LD71" s="11"/>
+      <c r="LE71" s="11"/>
+      <c r="LF71" s="11"/>
+      <c r="LG71" s="11"/>
+      <c r="LH71" s="11"/>
+      <c r="LI71" s="11"/>
+      <c r="LJ71" s="11"/>
+      <c r="LK71" s="11"/>
+      <c r="LL71" s="11"/>
+      <c r="LM71" s="11"/>
+      <c r="LN71" s="11"/>
+      <c r="LO71" s="11"/>
+      <c r="LP71" s="11"/>
+      <c r="LQ71" s="11"/>
+      <c r="LR71" s="11"/>
+      <c r="LS71" s="11"/>
+      <c r="LT71" s="11"/>
+      <c r="LU71" s="11"/>
+      <c r="LV71" s="11"/>
+      <c r="LW71" s="11"/>
+      <c r="LX71" s="11"/>
+      <c r="LY71" s="11"/>
+      <c r="LZ71" s="11"/>
+      <c r="MA71" s="11"/>
+      <c r="MB71" s="11"/>
+      <c r="MC71" s="11"/>
+      <c r="MD71" s="11"/>
+      <c r="ME71" s="11"/>
+      <c r="MF71" s="11"/>
+      <c r="MG71" s="11"/>
+      <c r="MH71" s="11"/>
+      <c r="MI71" s="11"/>
+      <c r="MJ71" s="11"/>
+      <c r="MK71" s="11"/>
+      <c r="ML71" s="11"/>
+      <c r="MM71" s="11"/>
+      <c r="MN71" s="11"/>
+      <c r="MO71" s="11"/>
+      <c r="MP71" s="11"/>
+      <c r="MQ71" s="11"/>
+      <c r="MR71" s="11"/>
+      <c r="MS71" s="11"/>
+      <c r="MT71" s="11"/>
+      <c r="MU71" s="11"/>
+      <c r="MV71" s="11"/>
+      <c r="MW71" s="11"/>
+      <c r="MX71" s="11"/>
+      <c r="MY71" s="11"/>
+      <c r="MZ71" s="11"/>
+      <c r="NA71" s="11"/>
+      <c r="NB71" s="11"/>
+      <c r="NC71" s="11"/>
+      <c r="ND71" s="11"/>
+      <c r="NE71" s="11"/>
+      <c r="NF71" s="11"/>
+      <c r="NG71" s="11"/>
+      <c r="NH71" s="11"/>
+      <c r="NI71" s="11"/>
+      <c r="NJ71" s="11"/>
+      <c r="NK71" s="11"/>
+      <c r="NL71" s="11"/>
+      <c r="NM71" s="11"/>
+      <c r="NN71" s="11"/>
+      <c r="NO71" s="11"/>
+      <c r="NP71" s="11"/>
+      <c r="NQ71" s="11"/>
+      <c r="NR71" s="11"/>
+      <c r="NS71" s="11"/>
+      <c r="NT71" s="11"/>
+      <c r="NU71" s="11"/>
+      <c r="NV71" s="11"/>
+      <c r="NW71" s="11"/>
+      <c r="NX71" s="11"/>
+      <c r="NY71" s="11"/>
+      <c r="NZ71" s="11"/>
+      <c r="OA71" s="11"/>
+      <c r="OB71" s="11"/>
+      <c r="OC71" s="11"/>
+      <c r="OD71" s="11"/>
+      <c r="OE71" s="11"/>
+      <c r="OF71" s="11"/>
+      <c r="OG71" s="11"/>
+      <c r="OH71" s="11"/>
+      <c r="OI71" s="11"/>
+      <c r="OJ71" s="11"/>
+      <c r="OK71" s="11"/>
+      <c r="OL71" s="11"/>
+      <c r="OM71" s="11"/>
+      <c r="ON71" s="11"/>
+      <c r="OO71" s="11"/>
+      <c r="OP71" s="11"/>
+      <c r="OQ71" s="11"/>
+      <c r="OR71" s="11"/>
+      <c r="OS71" s="11"/>
+      <c r="OT71" s="11"/>
+      <c r="OU71" s="11"/>
+      <c r="OV71" s="11"/>
+      <c r="OW71" s="11"/>
+      <c r="OX71" s="11"/>
+      <c r="OY71" s="11"/>
+      <c r="OZ71" s="11"/>
+      <c r="PA71" s="11"/>
+      <c r="PB71" s="11"/>
+      <c r="PC71" s="11"/>
+      <c r="PD71" s="11"/>
+      <c r="PE71" s="11"/>
+      <c r="PF71" s="11"/>
+      <c r="PG71" s="11"/>
+      <c r="PH71" s="11"/>
+      <c r="PI71" s="11"/>
+      <c r="PJ71" s="11"/>
+      <c r="PK71" s="11"/>
+      <c r="PL71" s="11"/>
+      <c r="PM71" s="11"/>
+      <c r="PN71" s="11"/>
+      <c r="PO71" s="11"/>
+      <c r="PP71" s="11"/>
+      <c r="PQ71" s="11"/>
+      <c r="PR71" s="11"/>
+      <c r="PS71" s="11"/>
+      <c r="PT71" s="11"/>
+      <c r="PU71" s="11"/>
+      <c r="PV71" s="11"/>
+      <c r="PW71" s="11"/>
+      <c r="PX71" s="11"/>
+      <c r="PY71" s="11"/>
+      <c r="PZ71" s="11"/>
+      <c r="QA71" s="11"/>
+      <c r="QB71" s="11"/>
+      <c r="QC71" s="11"/>
+      <c r="QD71" s="11"/>
+      <c r="QE71" s="11"/>
+      <c r="QF71" s="11"/>
+      <c r="QG71" s="11"/>
+      <c r="QH71" s="11"/>
+      <c r="QI71" s="11"/>
+      <c r="QJ71" s="11"/>
+      <c r="QK71" s="11"/>
+      <c r="QL71" s="11"/>
+      <c r="QM71" s="11"/>
+      <c r="QN71" s="11"/>
+      <c r="QO71" s="11"/>
+      <c r="QP71" s="11"/>
+      <c r="QQ71" s="11"/>
+      <c r="QR71" s="11"/>
+      <c r="QS71" s="11"/>
+      <c r="QT71" s="11"/>
+      <c r="QU71" s="11"/>
+      <c r="QV71" s="11"/>
+      <c r="QW71" s="11"/>
+      <c r="QX71" s="11"/>
+      <c r="QY71" s="11"/>
+      <c r="QZ71" s="11"/>
+      <c r="RA71" s="11"/>
+      <c r="RB71" s="11"/>
+      <c r="RC71" s="11"/>
+      <c r="RD71" s="11"/>
+      <c r="RE71" s="11"/>
+      <c r="RF71" s="11"/>
+      <c r="RG71" s="11"/>
+      <c r="RH71" s="11"/>
+      <c r="RI71" s="11"/>
+      <c r="RJ71" s="11"/>
+      <c r="RK71" s="11"/>
+      <c r="RL71" s="11"/>
+      <c r="RM71" s="11"/>
+      <c r="RN71" s="11"/>
+      <c r="RO71" s="11"/>
+      <c r="RP71" s="11"/>
+      <c r="RQ71" s="11"/>
+      <c r="RR71" s="11"/>
+      <c r="RS71" s="11"/>
+      <c r="RT71" s="11"/>
+      <c r="RU71" s="11"/>
+      <c r="RV71" s="11"/>
+      <c r="RW71" s="11"/>
+      <c r="RX71" s="11"/>
+      <c r="RY71" s="11"/>
+      <c r="RZ71" s="11"/>
+      <c r="SA71" s="11"/>
+      <c r="SB71" s="11"/>
+      <c r="SC71" s="11"/>
+      <c r="SD71" s="11"/>
+      <c r="SE71" s="11"/>
+      <c r="SF71" s="11"/>
+      <c r="SG71" s="11"/>
+      <c r="SH71" s="11"/>
+      <c r="SI71" s="11"/>
+      <c r="SJ71" s="11"/>
+      <c r="SK71" s="11"/>
+      <c r="SL71" s="11"/>
+      <c r="SM71" s="11"/>
+      <c r="SN71" s="11"/>
+      <c r="SO71" s="11"/>
+      <c r="SP71" s="11"/>
+      <c r="SQ71" s="11"/>
+      <c r="SR71" s="11"/>
+      <c r="SS71" s="11"/>
+      <c r="ST71" s="11"/>
+      <c r="SU71" s="11"/>
+      <c r="SV71" s="11"/>
+      <c r="SW71" s="11"/>
+      <c r="SX71" s="11"/>
+      <c r="SY71" s="11"/>
+      <c r="SZ71" s="11"/>
+      <c r="TA71" s="11"/>
+      <c r="TB71" s="11"/>
+      <c r="TC71" s="11"/>
+      <c r="TD71" s="11"/>
+      <c r="TE71" s="11"/>
+      <c r="TF71" s="11"/>
+      <c r="TG71" s="11"/>
+      <c r="TH71" s="11"/>
+      <c r="TI71" s="11"/>
+      <c r="TJ71" s="11"/>
+      <c r="TK71" s="11"/>
+      <c r="TL71" s="11"/>
+      <c r="TM71" s="11"/>
+      <c r="TN71" s="11"/>
+      <c r="TO71" s="11"/>
+      <c r="TP71" s="11"/>
+      <c r="TQ71" s="11"/>
+      <c r="TR71" s="11"/>
+      <c r="TS71" s="11"/>
+      <c r="TT71" s="11"/>
+      <c r="TU71" s="11"/>
+      <c r="TV71" s="11"/>
+      <c r="TW71" s="11"/>
+      <c r="TX71" s="11"/>
+      <c r="TY71" s="11"/>
+      <c r="TZ71" s="11"/>
+      <c r="UA71" s="11"/>
+      <c r="UB71" s="11"/>
+      <c r="UC71" s="11"/>
+      <c r="UD71" s="11"/>
+      <c r="UE71" s="11"/>
+      <c r="UF71" s="11"/>
+      <c r="UG71" s="11"/>
+      <c r="UH71" s="11"/>
+      <c r="UI71" s="11"/>
+      <c r="UJ71" s="11"/>
+      <c r="UK71" s="11"/>
+      <c r="UL71" s="11"/>
+      <c r="UM71" s="11"/>
+      <c r="UN71" s="11"/>
+      <c r="UO71" s="11"/>
+      <c r="UP71" s="11"/>
+      <c r="UQ71" s="11"/>
+      <c r="UR71" s="11"/>
+      <c r="US71" s="11"/>
+      <c r="UT71" s="11"/>
+      <c r="UU71" s="11"/>
+      <c r="UV71" s="11"/>
+      <c r="UW71" s="11"/>
+      <c r="UX71" s="11"/>
+      <c r="UY71" s="11"/>
+      <c r="UZ71" s="11"/>
+      <c r="VA71" s="11"/>
+      <c r="VB71" s="11"/>
+      <c r="VC71" s="11"/>
+      <c r="VD71" s="11"/>
+      <c r="VE71" s="11"/>
+      <c r="VF71" s="11"/>
+      <c r="VG71" s="11"/>
+      <c r="VH71" s="11"/>
+      <c r="VI71" s="11"/>
+      <c r="VJ71" s="11"/>
+      <c r="VK71" s="11"/>
+      <c r="VL71" s="11"/>
+      <c r="VM71" s="11"/>
+      <c r="VN71" s="11"/>
+      <c r="VO71" s="11"/>
+      <c r="VP71" s="11"/>
+      <c r="VQ71" s="11"/>
+      <c r="VR71" s="11"/>
+      <c r="VS71" s="11"/>
+      <c r="VT71" s="11"/>
+      <c r="VU71" s="11"/>
+      <c r="VV71" s="11"/>
+      <c r="VW71" s="11"/>
+      <c r="VX71" s="11"/>
+      <c r="VY71" s="11"/>
+      <c r="VZ71" s="11"/>
+      <c r="WA71" s="11"/>
+      <c r="WB71" s="11"/>
+      <c r="WC71" s="11"/>
+      <c r="WD71" s="11"/>
+      <c r="WE71" s="11"/>
+      <c r="WF71" s="11"/>
+      <c r="WG71" s="11"/>
+      <c r="WH71" s="11"/>
+      <c r="WI71" s="11"/>
+      <c r="WJ71" s="11"/>
+      <c r="WK71" s="11"/>
+      <c r="WL71" s="11"/>
+      <c r="WM71" s="11"/>
+      <c r="WN71" s="11"/>
+      <c r="WO71" s="11"/>
+      <c r="WP71" s="11"/>
+      <c r="WQ71" s="11"/>
+      <c r="WR71" s="11"/>
+      <c r="WS71" s="11"/>
+      <c r="WT71" s="11"/>
+      <c r="WU71" s="11"/>
+      <c r="WV71" s="11"/>
+      <c r="WW71" s="11"/>
+      <c r="WX71" s="11"/>
+      <c r="WY71" s="11"/>
+      <c r="WZ71" s="11"/>
+      <c r="XA71" s="11"/>
+      <c r="XB71" s="11"/>
+      <c r="XC71" s="11"/>
+      <c r="XD71" s="11"/>
+      <c r="XE71" s="11"/>
+      <c r="XF71" s="11"/>
+      <c r="XG71" s="11"/>
+      <c r="XH71" s="11"/>
+      <c r="XI71" s="11"/>
+      <c r="XJ71" s="11"/>
+      <c r="XK71" s="11"/>
+      <c r="XL71" s="11"/>
+      <c r="XM71" s="11"/>
+      <c r="XN71" s="11"/>
+      <c r="XO71" s="11"/>
+      <c r="XP71" s="11"/>
+      <c r="XQ71" s="11"/>
+      <c r="XR71" s="11"/>
+      <c r="XS71" s="11"/>
+      <c r="XT71" s="11"/>
+      <c r="XU71" s="11"/>
+      <c r="XV71" s="11"/>
+      <c r="XW71" s="11"/>
+      <c r="XX71" s="11"/>
+      <c r="XY71" s="11"/>
+      <c r="XZ71" s="11"/>
+      <c r="YA71" s="11"/>
+      <c r="YB71" s="11"/>
+      <c r="YC71" s="11"/>
+      <c r="YD71" s="11"/>
+      <c r="YE71" s="11"/>
+      <c r="YF71" s="11"/>
+      <c r="YG71" s="11"/>
+      <c r="YH71" s="11"/>
+      <c r="YI71" s="11"/>
+      <c r="YJ71" s="11"/>
+      <c r="YK71" s="11"/>
+      <c r="YL71" s="11"/>
+      <c r="YM71" s="11"/>
+      <c r="YN71" s="11"/>
+      <c r="YO71" s="11"/>
+      <c r="YP71" s="11"/>
+      <c r="YQ71" s="11"/>
+      <c r="YR71" s="11"/>
+      <c r="YS71" s="11"/>
+      <c r="YT71" s="11"/>
+      <c r="YU71" s="11"/>
+      <c r="YV71" s="11"/>
+      <c r="YW71" s="11"/>
+      <c r="YX71" s="11"/>
+      <c r="YY71" s="11"/>
+      <c r="YZ71" s="11"/>
+      <c r="ZA71" s="11"/>
+      <c r="ZB71" s="11"/>
+      <c r="ZC71" s="11"/>
+      <c r="ZD71" s="11"/>
+      <c r="ZE71" s="11"/>
+      <c r="ZF71" s="11"/>
+      <c r="ZG71" s="11"/>
+      <c r="ZH71" s="11"/>
+      <c r="ZI71" s="11"/>
+      <c r="ZJ71" s="11"/>
+      <c r="ZK71" s="11"/>
+      <c r="ZL71" s="11"/>
+      <c r="ZM71" s="11"/>
+      <c r="ZN71" s="11"/>
+      <c r="ZO71" s="11"/>
+      <c r="ZP71" s="11"/>
+      <c r="ZQ71" s="11"/>
+      <c r="ZR71" s="11"/>
+      <c r="ZS71" s="11"/>
+      <c r="ZT71" s="11"/>
+      <c r="ZU71" s="11"/>
+      <c r="ZV71" s="11"/>
+      <c r="ZW71" s="11"/>
+      <c r="ZX71" s="11"/>
+      <c r="ZY71" s="11"/>
+      <c r="ZZ71" s="11"/>
+      <c r="AAA71" s="11"/>
+      <c r="AAB71" s="11"/>
+      <c r="AAC71" s="11"/>
+      <c r="AAD71" s="11"/>
+      <c r="AAE71" s="11"/>
+      <c r="AAF71" s="11"/>
+      <c r="AAG71" s="11"/>
+      <c r="AAH71" s="11"/>
+      <c r="AAI71" s="11"/>
+      <c r="AAJ71" s="11"/>
+      <c r="AAK71" s="11"/>
+      <c r="AAL71" s="11"/>
+      <c r="AAM71" s="11"/>
+      <c r="AAN71" s="11"/>
+      <c r="AAO71" s="11"/>
+      <c r="AAP71" s="11"/>
+      <c r="AAQ71" s="11"/>
+      <c r="AAR71" s="11"/>
+      <c r="AAS71" s="11"/>
+      <c r="AAT71" s="11"/>
+      <c r="AAU71" s="11"/>
+      <c r="AAV71" s="11"/>
+      <c r="AAW71" s="11"/>
+      <c r="AAX71" s="11"/>
+      <c r="AAY71" s="11"/>
+      <c r="AAZ71" s="11"/>
+      <c r="ABA71" s="11"/>
+      <c r="ABB71" s="11"/>
+      <c r="ABC71" s="11"/>
+      <c r="ABD71" s="11"/>
+      <c r="ABE71" s="11"/>
+      <c r="ABF71" s="11"/>
+      <c r="ABG71" s="11"/>
+      <c r="ABH71" s="11"/>
+      <c r="ABI71" s="11"/>
+      <c r="ABJ71" s="11"/>
+      <c r="ABK71" s="11"/>
+      <c r="ABL71" s="11"/>
+      <c r="ABM71" s="11"/>
+      <c r="ABN71" s="11"/>
+      <c r="ABO71" s="11"/>
+      <c r="ABP71" s="11"/>
+      <c r="ABQ71" s="11"/>
+      <c r="ABR71" s="11"/>
+      <c r="ABS71" s="11"/>
+      <c r="ABT71" s="11"/>
+      <c r="ABU71" s="11"/>
+      <c r="ABV71" s="11"/>
+      <c r="ABW71" s="11"/>
+      <c r="ABX71" s="11"/>
+      <c r="ABY71" s="11"/>
+      <c r="ABZ71" s="11"/>
+      <c r="ACA71" s="11"/>
+      <c r="ACB71" s="11"/>
+      <c r="ACC71" s="11"/>
+      <c r="ACD71" s="11"/>
+      <c r="ACE71" s="11"/>
+      <c r="ACF71" s="11"/>
+      <c r="ACG71" s="11"/>
+      <c r="ACH71" s="11"/>
+      <c r="ACI71" s="11"/>
+      <c r="ACJ71" s="11"/>
+      <c r="ACK71" s="11"/>
+      <c r="ACL71" s="11"/>
+      <c r="ACM71" s="11"/>
+      <c r="ACN71" s="11"/>
+      <c r="ACO71" s="11"/>
+      <c r="ACP71" s="11"/>
+      <c r="ACQ71" s="11"/>
+      <c r="ACR71" s="11"/>
+      <c r="ACS71" s="11"/>
+      <c r="ACT71" s="11"/>
+      <c r="ACU71" s="11"/>
+      <c r="ACV71" s="11"/>
+      <c r="ACW71" s="11"/>
+      <c r="ACX71" s="11"/>
+      <c r="ACY71" s="11"/>
+      <c r="ACZ71" s="11"/>
+      <c r="ADA71" s="11"/>
+      <c r="ADB71" s="11"/>
+      <c r="ADC71" s="11"/>
+      <c r="ADD71" s="11"/>
+      <c r="ADE71" s="11"/>
+      <c r="ADF71" s="11"/>
+      <c r="ADG71" s="11"/>
+      <c r="ADH71" s="11"/>
+      <c r="ADI71" s="11"/>
+      <c r="ADJ71" s="11"/>
+      <c r="ADK71" s="11"/>
+      <c r="ADL71" s="11"/>
+      <c r="ADM71" s="11"/>
+      <c r="ADN71" s="11"/>
+      <c r="ADO71" s="11"/>
+      <c r="ADP71" s="11"/>
+      <c r="ADQ71" s="11"/>
+      <c r="ADR71" s="11"/>
+      <c r="ADS71" s="11"/>
+      <c r="ADT71" s="11"/>
+      <c r="ADU71" s="11"/>
+      <c r="ADV71" s="11"/>
+      <c r="ADW71" s="11"/>
+      <c r="ADX71" s="11"/>
+      <c r="ADY71" s="11"/>
+      <c r="ADZ71" s="11"/>
+      <c r="AEA71" s="11"/>
+      <c r="AEB71" s="11"/>
+      <c r="AEC71" s="11"/>
+      <c r="AED71" s="11"/>
+      <c r="AEE71" s="11"/>
+      <c r="AEF71" s="11"/>
+      <c r="AEG71" s="11"/>
+      <c r="AEH71" s="11"/>
+      <c r="AEI71" s="11"/>
+      <c r="AEJ71" s="11"/>
+      <c r="AEK71" s="11"/>
+      <c r="AEL71" s="11"/>
+      <c r="AEM71" s="11"/>
+      <c r="AEN71" s="11"/>
+      <c r="AEO71" s="11"/>
+      <c r="AEP71" s="11"/>
+      <c r="AEQ71" s="11"/>
+      <c r="AER71" s="11"/>
+      <c r="AES71" s="11"/>
+      <c r="AET71" s="11"/>
+      <c r="AEU71" s="11"/>
+      <c r="AEV71" s="11"/>
+      <c r="AEW71" s="11"/>
+      <c r="AEX71" s="11"/>
+      <c r="AEY71" s="11"/>
+      <c r="AEZ71" s="11"/>
+      <c r="AFA71" s="11"/>
+      <c r="AFB71" s="11"/>
+      <c r="AFC71" s="11"/>
+      <c r="AFD71" s="11"/>
+      <c r="AFE71" s="11"/>
+      <c r="AFF71" s="11"/>
+      <c r="AFG71" s="11"/>
+      <c r="AFH71" s="11"/>
+      <c r="AFI71" s="11"/>
+      <c r="AFJ71" s="11"/>
+      <c r="AFK71" s="11"/>
+      <c r="AFL71" s="11"/>
+      <c r="AFM71" s="11"/>
+      <c r="AFN71" s="11"/>
+      <c r="AFO71" s="11"/>
+      <c r="AFP71" s="11"/>
+      <c r="AFQ71" s="11"/>
+      <c r="AFR71" s="11"/>
+      <c r="AFS71" s="11"/>
+      <c r="AFT71" s="11"/>
+      <c r="AFU71" s="11"/>
+      <c r="AFV71" s="11"/>
+      <c r="AFW71" s="11"/>
+      <c r="AFX71" s="11"/>
+      <c r="AFY71" s="11"/>
+      <c r="AFZ71" s="11"/>
+      <c r="AGA71" s="11"/>
+      <c r="AGB71" s="11"/>
+      <c r="AGC71" s="11"/>
+      <c r="AGD71" s="11"/>
+      <c r="AGE71" s="11"/>
+      <c r="AGF71" s="11"/>
+      <c r="AGG71" s="11"/>
+      <c r="AGH71" s="11"/>
+      <c r="AGI71" s="11"/>
+      <c r="AGJ71" s="11"/>
+      <c r="AGK71" s="11"/>
+      <c r="AGL71" s="11"/>
+      <c r="AGM71" s="11"/>
+      <c r="AGN71" s="11"/>
+      <c r="AGO71" s="11"/>
+      <c r="AGP71" s="11"/>
+      <c r="AGQ71" s="11"/>
+      <c r="AGR71" s="11"/>
+      <c r="AGS71" s="11"/>
+      <c r="AGT71" s="11"/>
+      <c r="AGU71" s="11"/>
+      <c r="AGV71" s="11"/>
+      <c r="AGW71" s="11"/>
+      <c r="AGX71" s="11"/>
+      <c r="AGY71" s="11"/>
+      <c r="AGZ71" s="11"/>
+      <c r="AHA71" s="11"/>
+      <c r="AHB71" s="11"/>
+      <c r="AHC71" s="11"/>
+      <c r="AHD71" s="11"/>
+      <c r="AHE71" s="11"/>
+      <c r="AHF71" s="11"/>
+      <c r="AHG71" s="11"/>
+      <c r="AHH71" s="11"/>
+      <c r="AHI71" s="11"/>
+      <c r="AHJ71" s="11"/>
+      <c r="AHK71" s="11"/>
+      <c r="AHL71" s="11"/>
+      <c r="AHM71" s="11"/>
+      <c r="AHN71" s="11"/>
+      <c r="AHO71" s="11"/>
+      <c r="AHP71" s="11"/>
+      <c r="AHQ71" s="11"/>
+      <c r="AHR71" s="11"/>
+      <c r="AHS71" s="11"/>
+      <c r="AHT71" s="11"/>
+      <c r="AHU71" s="11"/>
+      <c r="AHV71" s="11"/>
+      <c r="AHW71" s="11"/>
+      <c r="AHX71" s="11"/>
+      <c r="AHY71" s="11"/>
+      <c r="AHZ71" s="11"/>
+      <c r="AIA71" s="11"/>
+      <c r="AIB71" s="11"/>
+      <c r="AIC71" s="11"/>
+      <c r="AID71" s="11"/>
+      <c r="AIE71" s="11"/>
+      <c r="AIF71" s="11"/>
+      <c r="AIG71" s="11"/>
+      <c r="AIH71" s="11"/>
+      <c r="AII71" s="11"/>
+      <c r="AIJ71" s="11"/>
+      <c r="AIK71" s="11"/>
+      <c r="AIL71" s="11"/>
+      <c r="AIM71" s="11"/>
+      <c r="AIN71" s="11"/>
+      <c r="AIO71" s="11"/>
+      <c r="AIP71" s="11"/>
+      <c r="AIQ71" s="11"/>
+      <c r="AIR71" s="11"/>
+      <c r="AIS71" s="11"/>
+      <c r="AIT71" s="11"/>
+      <c r="AIU71" s="11"/>
+      <c r="AIV71" s="11"/>
+      <c r="AIW71" s="11"/>
+      <c r="AIX71" s="11"/>
+      <c r="AIY71" s="11"/>
+      <c r="AIZ71" s="11"/>
+      <c r="AJA71" s="11"/>
+      <c r="AJB71" s="11"/>
+      <c r="AJC71" s="11"/>
+      <c r="AJD71" s="11"/>
+      <c r="AJE71" s="11"/>
+      <c r="AJF71" s="11"/>
+      <c r="AJG71" s="11"/>
+      <c r="AJH71" s="11"/>
+      <c r="AJI71" s="11"/>
+      <c r="AJJ71" s="11"/>
+      <c r="AJK71" s="11"/>
+      <c r="AJL71" s="11"/>
+      <c r="AJM71" s="11"/>
+      <c r="AJN71" s="11"/>
+      <c r="AJO71" s="11"/>
+      <c r="AJP71" s="11"/>
+      <c r="AJQ71" s="11"/>
+      <c r="AJR71" s="11"/>
+      <c r="AJS71" s="11"/>
+      <c r="AJT71" s="11"/>
+      <c r="AJU71" s="11"/>
+      <c r="AJV71" s="11"/>
+      <c r="AJW71" s="11"/>
+      <c r="AJX71" s="11"/>
+      <c r="AJY71" s="11"/>
+      <c r="AJZ71" s="11"/>
+      <c r="AKA71" s="11"/>
+      <c r="AKB71" s="11"/>
+      <c r="AKC71" s="11"/>
+      <c r="AKD71" s="11"/>
+      <c r="AKE71" s="11"/>
+      <c r="AKF71" s="11"/>
+      <c r="AKG71" s="11"/>
+      <c r="AKH71" s="11"/>
+      <c r="AKI71" s="11"/>
+      <c r="AKJ71" s="11"/>
+      <c r="AKK71" s="11"/>
+      <c r="AKL71" s="11"/>
+      <c r="AKM71" s="11"/>
+      <c r="AKN71" s="11"/>
+      <c r="AKO71" s="11"/>
+      <c r="AKP71" s="11"/>
+      <c r="AKQ71" s="11"/>
+      <c r="AKR71" s="11"/>
+      <c r="AKS71" s="11"/>
+      <c r="AKT71" s="11"/>
+      <c r="AKU71" s="11"/>
+      <c r="AKV71" s="11"/>
+      <c r="AKW71" s="11"/>
+      <c r="AKX71" s="11"/>
+      <c r="AKY71" s="11"/>
+      <c r="AKZ71" s="11"/>
+      <c r="ALA71" s="11"/>
+      <c r="ALB71" s="11"/>
+      <c r="ALC71" s="11"/>
+      <c r="ALD71" s="11"/>
+      <c r="ALE71" s="11"/>
+      <c r="ALF71" s="11"/>
+      <c r="ALG71" s="11"/>
+      <c r="ALH71" s="11"/>
+      <c r="ALI71" s="11"/>
+      <c r="ALJ71" s="11"/>
+      <c r="ALK71" s="11"/>
+      <c r="ALL71" s="11"/>
+      <c r="ALM71" s="11"/>
+      <c r="ALN71" s="11"/>
+      <c r="ALO71" s="11"/>
+      <c r="ALP71" s="11"/>
+      <c r="ALQ71" s="11"/>
+      <c r="ALR71" s="11"/>
+      <c r="ALS71" s="11"/>
+      <c r="ALT71" s="11"/>
+      <c r="ALU71" s="11"/>
+      <c r="ALV71" s="11"/>
+      <c r="ALW71" s="11"/>
+      <c r="ALX71" s="11"/>
+      <c r="ALY71" s="11"/>
+      <c r="ALZ71" s="11"/>
+      <c r="AMA71" s="11"/>
+      <c r="AMB71" s="11"/>
+      <c r="AMC71" s="11"/>
+      <c r="AMD71" s="11"/>
+      <c r="AME71" s="11"/>
+      <c r="AMF71" s="11"/>
+      <c r="AMG71" s="11"/>
+      <c r="AMH71" s="11"/>
+      <c r="AMI71" s="11"/>
+      <c r="AMJ71" s="11"/>
+    </row>
+    <row r="1048415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
chore: replace ACK circuit with TPS28C100 fault pin
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="232">
   <si>
     <t xml:space="preserve">S3Main PCS BOM</t>
   </si>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">Your Instructions / Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C2, C3, C7, C8, C11, C18, C29, C30, C32</t>
+    <t xml:space="preserve">C1,C2,C3,C7,C8,C11,C18,C29,C30,C31</t>
   </si>
   <si>
     <t xml:space="preserve">Samsung Electro-Mechanics</t>
@@ -152,7 +152,7 @@
     <t xml:space="preserve">SMD</t>
   </si>
   <si>
-    <t xml:space="preserve">C4, C6, C19, C21, C22, C25, C26, C34</t>
+    <t xml:space="preserve">C4,C6,C19,C21,C22,C25,C26,C33</t>
   </si>
   <si>
     <t xml:space="preserve">Murata Electronics</t>
@@ -164,7 +164,7 @@
     <t xml:space="preserve">CAP CER 1000PF 100V C0G/NP0 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">C5, C35, C36</t>
+    <t xml:space="preserve">C5,C34,C35</t>
   </si>
   <si>
     <t xml:space="preserve">GCM1555C1H221JA16D</t>
@@ -173,7 +173,7 @@
     <t xml:space="preserve">CAP CER 220PF 50V C0G/NP0 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">C9, C10</t>
+    <t xml:space="preserve">C9,C10</t>
   </si>
   <si>
     <t xml:space="preserve">GCM1555C1H101JA16D</t>
@@ -182,7 +182,7 @@
     <t xml:space="preserve">CAP CER 100PF 50V C0G/NP0 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">C12, C20, C27</t>
+    <t xml:space="preserve">C12,C20,C27</t>
   </si>
   <si>
     <t xml:space="preserve">Cornell Dubilier Knowles</t>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">CAP CER 10UF 50V X7R 1206</t>
   </si>
   <si>
-    <t xml:space="preserve">C15, C16, C17, C23, C24</t>
+    <t xml:space="preserve">C15,C16,C17,C23,C24</t>
   </si>
   <si>
     <t xml:space="preserve">CL31B105KCHVPJE</t>
@@ -236,16 +236,7 @@
     <t xml:space="preserve">CAP CER 4.7UF 50V X7R 1206</t>
   </si>
   <si>
-    <t xml:space="preserve">C31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRT3195C2A103JA02D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 10000PF 100V C0G 1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C33, C37</t>
+    <t xml:space="preserve">C32,C36</t>
   </si>
   <si>
     <t xml:space="preserve">TDK Corporation</t>
@@ -257,7 +248,7 @@
     <t xml:space="preserve">CAP CER 47UF 6.3V X7S 1206</t>
   </si>
   <si>
-    <t xml:space="preserve">D1, D2, D3, D7, D8, D11, D13, D16, D17, D19</t>
+    <t xml:space="preserve">D1,D2,D3,D7,D8,D11,D13,D14,D15,D17</t>
   </si>
   <si>
     <t xml:space="preserve">onsemi</t>
@@ -344,22 +335,7 @@
     <t xml:space="preserve">TVS DIODE 30VWM 47.5VC ESC</t>
   </si>
   <si>
-    <t xml:space="preserve">D14, D15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micro Commercial Co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B5819W-TP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIODE SCHOTTKY 40V 1A SOD123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOD-123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D18</t>
+    <t xml:space="preserve">D16</t>
   </si>
   <si>
     <t xml:space="preserve">Diodes Incorporated</t>
@@ -440,7 +416,7 @@
     <t xml:space="preserve">0805</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1, Q6</t>
+    <t xml:space="preserve">Q1,Q6</t>
   </si>
   <si>
     <t xml:space="preserve">Rohm Semiconductor</t>
@@ -467,7 +443,7 @@
     <t xml:space="preserve">SOT-363</t>
   </si>
   <si>
-    <t xml:space="preserve">Q3, Q4, Q5, Q7, Q8</t>
+    <t xml:space="preserve">Q3,Q4,Q5,Q7,Q8</t>
   </si>
   <si>
     <t xml:space="preserve">Vishay Siliconix</t>
@@ -485,15 +461,6 @@
     <t xml:space="preserve">Q9</t>
   </si>
   <si>
-    <t xml:space="preserve">BSS138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOSFET N-CH 50V 220MA SOT23-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q10</t>
-  </si>
-  <si>
     <t xml:space="preserve">ANBON SEMICONDUCTOR (INT'L) LIMITED</t>
   </si>
   <si>
@@ -506,7 +473,7 @@
     <t xml:space="preserve">SOT-23</t>
   </si>
   <si>
-    <t xml:space="preserve">R1, R8, R18, R20, R34, R35, R36, R43, R48, R50</t>
+    <t xml:space="preserve">R1,R8,R18,R20,R35,R36,R37,R44,R49</t>
   </si>
   <si>
     <t xml:space="preserve">YAGEO</t>
@@ -518,7 +485,7 @@
     <t xml:space="preserve">RES 10K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R2, R3, R4, R5</t>
+    <t xml:space="preserve">R2,R3,R4,R5</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0722KL</t>
@@ -527,7 +494,7 @@
     <t xml:space="preserve">RES 22K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R6, R7, R31, R49</t>
+    <t xml:space="preserve">R6,R7,R31</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-074K7L</t>
@@ -548,7 +515,7 @@
     <t xml:space="preserve">RES SMD 2.2 OHM 1% 1/2W 0805</t>
   </si>
   <si>
-    <t xml:space="preserve">R10, R11, R14, R32, R45, R51</t>
+    <t xml:space="preserve">R10,R11,R14,R32,R46</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-071KL</t>
@@ -557,7 +524,7 @@
     <t xml:space="preserve">RES 1K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R12, R13, R22, R26, R27</t>
+    <t xml:space="preserve">R12,R13,R22,R26,R27</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-073K3L</t>
@@ -566,7 +533,7 @@
     <t xml:space="preserve">RES 3.3K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R15, R16, R52, R53</t>
+    <t xml:space="preserve">R15,R16,R50,R51</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0733RL</t>
@@ -584,7 +551,7 @@
     <t xml:space="preserve">RES 220 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R19, R54</t>
+    <t xml:space="preserve">R19,R34</t>
   </si>
   <si>
     <t xml:space="preserve">DNP</t>
@@ -608,7 +575,7 @@
     <t xml:space="preserve">RES 562 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R24, R25</t>
+    <t xml:space="preserve">R24,R25</t>
   </si>
   <si>
     <t xml:space="preserve">R28</t>
@@ -620,7 +587,7 @@
     <t xml:space="preserve">RES 422 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R29, R30, R46, R47</t>
+    <t xml:space="preserve">R29,R30,R47,R48</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0747RL</t>
@@ -638,7 +605,7 @@
     <t xml:space="preserve">RES 180 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R37, R44</t>
+    <t xml:space="preserve">R38,R45</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0714K3L</t>
@@ -647,7 +614,7 @@
     <t xml:space="preserve">RES 14.3K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R38</t>
+    <t xml:space="preserve">R39</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-07470RL</t>
@@ -656,7 +623,7 @@
     <t xml:space="preserve">RES 470 OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R39</t>
+    <t xml:space="preserve">R40</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0718K7L</t>
@@ -665,7 +632,7 @@
     <t xml:space="preserve">RES 18.7K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R40, R41</t>
+    <t xml:space="preserve">R41,R42</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-075K1L</t>
@@ -674,7 +641,7 @@
     <t xml:space="preserve">RES 5.1K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R42</t>
+    <t xml:space="preserve">R43</t>
   </si>
   <si>
     <t xml:space="preserve">RC0402FR-0739KL</t>
@@ -683,7 +650,7 @@
     <t xml:space="preserve">RES 39K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">R55</t>
+    <t xml:space="preserve">R52</t>
   </si>
   <si>
     <t xml:space="preserve">Panasonic Electronic Components</t>
@@ -1105,13 +1072,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>649800</xdr:colOff>
+      <xdr:colOff>649440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="图片 1" descr="pcbway-400x400.jpg"/>
+        <xdr:cNvPr id="1" name="图片 1" descr="pcbway-400x400.jpg"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1121,7 +1088,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9360" y="211680"/>
-          <a:ext cx="1360440" cy="359280"/>
+          <a:ext cx="1360080" cy="358920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1251,7 +1218,7 @@
   <dimension ref="A2:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N64" activeCellId="0" sqref="N64"/>
+      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1569,16 +1536,16 @@
         <v>44</v>
       </c>
       <c r="C16" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>34</v>
@@ -1593,22 +1560,22 @@
         <v>11</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="H17" s="10" t="s">
         <v>15</v>
@@ -1620,22 +1587,22 @@
         <v>12</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>15</v>
@@ -1647,13 +1614,13 @@
         <v>13</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>58</v>
@@ -1680,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>61</v>
@@ -1707,16 +1674,16 @@
         <v>1</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="H21" s="10" t="s">
         <v>15</v>
@@ -1728,22 +1695,22 @@
         <v>16</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>15</v>
@@ -1755,22 +1722,22 @@
         <v>17</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C23" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>15</v>
@@ -1782,22 +1749,22 @@
         <v>18</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>15</v>
@@ -1809,25 +1776,23 @@
         <v>19</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C25" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="E25" s="7" t="n">
+        <v>1844210</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>84</v>
       </c>
+      <c r="G25" s="9"/>
       <c r="H25" s="10" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="I25" s="10"/>
     </row>
@@ -1836,23 +1801,21 @@
         <v>20</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C26" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="F26" s="8" t="s">
         <v>89</v>
       </c>
+      <c r="G26" s="9"/>
       <c r="H26" s="10" t="s">
         <v>15</v>
       </c>
@@ -1869,17 +1832,17 @@
         <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="7" t="n">
+        <v>1836189</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="E27" s="7" t="n">
-        <v>1844210</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I27" s="10"/>
     </row>
@@ -1888,19 +1851,19 @@
         <v>22</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="10" t="s">
@@ -1913,23 +1876,23 @@
         <v>23</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="7" t="n">
-        <v>1836189</v>
+        <v>97</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>99</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="10" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="I29" s="10"/>
     </row>
@@ -1944,15 +1907,17 @@
         <v>1</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="G30" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="G30" s="9"/>
       <c r="H30" s="10" t="s">
         <v>15</v>
       </c>
@@ -1966,7 +1931,7 @@
         <v>104</v>
       </c>
       <c r="C31" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>105</v>
@@ -1974,10 +1939,12 @@
       <c r="E31" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="G31" s="9"/>
+      <c r="G31" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="H31" s="10" t="s">
         <v>15</v>
       </c>
@@ -1988,22 +1955,22 @@
         <v>26</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C32" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F32" s="8" t="s">
         <v>110</v>
       </c>
+      <c r="F32" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="G32" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H32" s="10" t="s">
         <v>15</v>
@@ -2015,22 +1982,22 @@
         <v>27</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C33" s="6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="7" t="s">
         <v>115</v>
       </c>
+      <c r="F33" s="8" t="s">
+        <v>116</v>
+      </c>
       <c r="G33" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>15</v>
@@ -2042,22 +2009,22 @@
         <v>28</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C34" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>15</v>
@@ -2069,22 +2036,22 @@
         <v>29</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C35" s="6" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>125</v>
+        <v>14</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>15</v>
@@ -2096,22 +2063,22 @@
         <v>30</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C36" s="6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>15</v>
@@ -2123,13 +2090,13 @@
         <v>31</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C37" s="6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>131</v>
@@ -2138,7 +2105,7 @@
         <v>132</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="H37" s="10" t="s">
         <v>15</v>
@@ -2150,22 +2117,22 @@
         <v>32</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C38" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="D38" s="7" t="s">
+      <c r="E38" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>137</v>
-      </c>
       <c r="G38" s="9" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="H38" s="10" t="s">
         <v>15</v>
@@ -2177,19 +2144,19 @@
         <v>33</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C39" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>140</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>14</v>
@@ -2204,19 +2171,19 @@
         <v>34</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C40" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" s="7" t="s">
+      <c r="F40" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>14</v>
@@ -2231,22 +2198,22 @@
         <v>35</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>147</v>
-      </c>
       <c r="G41" s="9" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="H41" s="10" t="s">
         <v>15</v>
@@ -2258,19 +2225,19 @@
         <v>36</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="C42" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>14</v>
@@ -2285,25 +2252,19 @@
         <v>37</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C43" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="10" t="s">
+        <v>150</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="I43" s="10"/>
     </row>
@@ -2312,19 +2273,19 @@
         <v>38</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C44" s="6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>14</v>
@@ -2339,19 +2300,19 @@
         <v>39</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C45" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>14</v>
@@ -2366,7 +2327,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C46" s="6" t="n">
         <v>2</v>
@@ -2375,10 +2336,10 @@
       <c r="E46" s="7"/>
       <c r="F46" s="8"/>
       <c r="G46" s="10" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="I46" s="10"/>
     </row>
@@ -2387,19 +2348,19 @@
         <v>41</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C47" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="G47" s="9" t="s">
         <v>14</v>
@@ -2414,19 +2375,19 @@
         <v>42</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C48" s="6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>14</v>
@@ -2441,19 +2402,25 @@
         <v>43</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C49" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="10" t="s">
-        <v>161</v>
+        <v>1</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="I49" s="10"/>
     </row>
@@ -2462,19 +2429,19 @@
         <v>44</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C50" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F50" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="C50" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>171</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>14</v>
@@ -2489,19 +2456,19 @@
         <v>45</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C51" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F51" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="C51" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="G51" s="9" t="s">
         <v>14</v>
@@ -2516,19 +2483,19 @@
         <v>46</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C52" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>14</v>
@@ -2543,19 +2510,19 @@
         <v>47</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C53" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G53" s="9" t="s">
         <v>14</v>
@@ -2570,19 +2537,19 @@
         <v>48</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C54" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>14</v>
@@ -2597,19 +2564,19 @@
         <v>49</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C55" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="E55" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F55" s="8" t="s">
         <v>185</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>186</v>
       </c>
       <c r="G55" s="9" t="s">
         <v>14</v>
@@ -2624,22 +2591,22 @@
         <v>50</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C56" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="E56" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F56" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="G56" s="9" t="s">
         <v>189</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="H56" s="10" t="s">
         <v>15</v>
@@ -2657,16 +2624,16 @@
         <v>1</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>135</v>
+        <v>49</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F57" s="7" t="s">
         <v>192</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>14</v>
+        <v>193</v>
       </c>
       <c r="H57" s="10" t="s">
         <v>15</v>
@@ -2678,22 +2645,22 @@
         <v>52</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C58" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>14</v>
+        <v>198</v>
       </c>
       <c r="H58" s="10" t="s">
         <v>15</v>
@@ -2705,22 +2672,22 @@
         <v>53</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C59" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H59" s="10" t="s">
         <v>15</v>
@@ -2732,23 +2699,21 @@
         <v>54</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C60" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>52</v>
+        <v>205</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>204</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="G60" s="9"/>
       <c r="H60" s="10" t="s">
         <v>15</v>
       </c>
@@ -2759,22 +2724,22 @@
         <v>55</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C61" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>15</v>
@@ -2786,22 +2751,22 @@
         <v>56</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C62" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H62" s="10" t="s">
         <v>15</v>
@@ -2813,13 +2778,13 @@
         <v>57</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C63" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>216</v>
+        <v>78</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>217</v>
@@ -2827,7 +2792,9 @@
       <c r="F63" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="G63" s="9"/>
+      <c r="G63" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="H63" s="10" t="s">
         <v>15</v>
       </c>
@@ -2844,12 +2811,12 @@
         <v>1</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="12" t="s">
         <v>221</v>
       </c>
       <c r="G64" s="9" t="s">
@@ -2871,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>211</v>
+        <v>78</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>224</v>
@@ -2898,1133 +2865,1055 @@
         <v>1</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>86</v>
+        <v>228</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>75</v>
+        <v>231</v>
       </c>
       <c r="H66" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I66" s="10"/>
     </row>
-    <row r="67" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6" t="n">
-        <v>61</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="C67" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="H67" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I67" s="10"/>
-    </row>
-    <row r="68" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6" t="n">
-        <v>62</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C68" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="G68" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="H68" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I68" s="10"/>
-    </row>
-    <row r="69" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6" t="n">
-        <v>63</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="C69" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="H69" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I69" s="10"/>
-    </row>
+    <row r="67" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="70" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" s="11" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
-      <c r="K74" s="11"/>
-      <c r="L74" s="11"/>
-      <c r="M74" s="11"/>
-      <c r="N74" s="11"/>
-      <c r="O74" s="11"/>
-      <c r="P74" s="11"/>
-      <c r="Q74" s="11"/>
-      <c r="R74" s="11"/>
-      <c r="S74" s="11"/>
-      <c r="T74" s="11"/>
-      <c r="U74" s="11"/>
-      <c r="V74" s="11"/>
-      <c r="W74" s="11"/>
-      <c r="X74" s="11"/>
-      <c r="Y74" s="11"/>
-      <c r="Z74" s="11"/>
-      <c r="AA74" s="11"/>
-      <c r="AB74" s="11"/>
-      <c r="AC74" s="11"/>
-      <c r="AD74" s="11"/>
-      <c r="AE74" s="11"/>
-      <c r="AF74" s="11"/>
-      <c r="AG74" s="11"/>
-      <c r="AH74" s="11"/>
-      <c r="AI74" s="11"/>
-      <c r="AJ74" s="11"/>
-      <c r="AK74" s="11"/>
-      <c r="AL74" s="11"/>
-      <c r="AM74" s="11"/>
-      <c r="AN74" s="11"/>
-      <c r="AO74" s="11"/>
-      <c r="AP74" s="11"/>
-      <c r="AQ74" s="11"/>
-      <c r="AR74" s="11"/>
-      <c r="AS74" s="11"/>
-      <c r="AT74" s="11"/>
-      <c r="AU74" s="11"/>
-      <c r="AV74" s="11"/>
-      <c r="AW74" s="11"/>
-      <c r="AX74" s="11"/>
-      <c r="AY74" s="11"/>
-      <c r="AZ74" s="11"/>
-      <c r="BA74" s="11"/>
-      <c r="BB74" s="11"/>
-      <c r="BC74" s="11"/>
-      <c r="BD74" s="11"/>
-      <c r="BE74" s="11"/>
-      <c r="BF74" s="11"/>
-      <c r="BG74" s="11"/>
-      <c r="BH74" s="11"/>
-      <c r="BI74" s="11"/>
-      <c r="BJ74" s="11"/>
-      <c r="BK74" s="11"/>
-      <c r="BL74" s="11"/>
-      <c r="BM74" s="11"/>
-      <c r="BN74" s="11"/>
-      <c r="BO74" s="11"/>
-      <c r="BP74" s="11"/>
-      <c r="BQ74" s="11"/>
-      <c r="BR74" s="11"/>
-      <c r="BS74" s="11"/>
-      <c r="BT74" s="11"/>
-      <c r="BU74" s="11"/>
-      <c r="BV74" s="11"/>
-      <c r="BW74" s="11"/>
-      <c r="BX74" s="11"/>
-      <c r="BY74" s="11"/>
-      <c r="BZ74" s="11"/>
-      <c r="CA74" s="11"/>
-      <c r="CB74" s="11"/>
-      <c r="CC74" s="11"/>
-      <c r="CD74" s="11"/>
-      <c r="CE74" s="11"/>
-      <c r="CF74" s="11"/>
-      <c r="CG74" s="11"/>
-      <c r="CH74" s="11"/>
-      <c r="CI74" s="11"/>
-      <c r="CJ74" s="11"/>
-      <c r="CK74" s="11"/>
-      <c r="CL74" s="11"/>
-      <c r="CM74" s="11"/>
-      <c r="CN74" s="11"/>
-      <c r="CO74" s="11"/>
-      <c r="CP74" s="11"/>
-      <c r="CQ74" s="11"/>
-      <c r="CR74" s="11"/>
-      <c r="CS74" s="11"/>
-      <c r="CT74" s="11"/>
-      <c r="CU74" s="11"/>
-      <c r="CV74" s="11"/>
-      <c r="CW74" s="11"/>
-      <c r="CX74" s="11"/>
-      <c r="CY74" s="11"/>
-      <c r="CZ74" s="11"/>
-      <c r="DA74" s="11"/>
-      <c r="DB74" s="11"/>
-      <c r="DC74" s="11"/>
-      <c r="DD74" s="11"/>
-      <c r="DE74" s="11"/>
-      <c r="DF74" s="11"/>
-      <c r="DG74" s="11"/>
-      <c r="DH74" s="11"/>
-      <c r="DI74" s="11"/>
-      <c r="DJ74" s="11"/>
-      <c r="DK74" s="11"/>
-      <c r="DL74" s="11"/>
-      <c r="DM74" s="11"/>
-      <c r="DN74" s="11"/>
-      <c r="DO74" s="11"/>
-      <c r="DP74" s="11"/>
-      <c r="DQ74" s="11"/>
-      <c r="DR74" s="11"/>
-      <c r="DS74" s="11"/>
-      <c r="DT74" s="11"/>
-      <c r="DU74" s="11"/>
-      <c r="DV74" s="11"/>
-      <c r="DW74" s="11"/>
-      <c r="DX74" s="11"/>
-      <c r="DY74" s="11"/>
-      <c r="DZ74" s="11"/>
-      <c r="EA74" s="11"/>
-      <c r="EB74" s="11"/>
-      <c r="EC74" s="11"/>
-      <c r="ED74" s="11"/>
-      <c r="EE74" s="11"/>
-      <c r="EF74" s="11"/>
-      <c r="EG74" s="11"/>
-      <c r="EH74" s="11"/>
-      <c r="EI74" s="11"/>
-      <c r="EJ74" s="11"/>
-      <c r="EK74" s="11"/>
-      <c r="EL74" s="11"/>
-      <c r="EM74" s="11"/>
-      <c r="EN74" s="11"/>
-      <c r="EO74" s="11"/>
-      <c r="EP74" s="11"/>
-      <c r="EQ74" s="11"/>
-      <c r="ER74" s="11"/>
-      <c r="ES74" s="11"/>
-      <c r="ET74" s="11"/>
-      <c r="EU74" s="11"/>
-      <c r="EV74" s="11"/>
-      <c r="EW74" s="11"/>
-      <c r="EX74" s="11"/>
-      <c r="EY74" s="11"/>
-      <c r="EZ74" s="11"/>
-      <c r="FA74" s="11"/>
-      <c r="FB74" s="11"/>
-      <c r="FC74" s="11"/>
-      <c r="FD74" s="11"/>
-      <c r="FE74" s="11"/>
-      <c r="FF74" s="11"/>
-      <c r="FG74" s="11"/>
-      <c r="FH74" s="11"/>
-      <c r="FI74" s="11"/>
-      <c r="FJ74" s="11"/>
-      <c r="FK74" s="11"/>
-      <c r="FL74" s="11"/>
-      <c r="FM74" s="11"/>
-      <c r="FN74" s="11"/>
-      <c r="FO74" s="11"/>
-      <c r="FP74" s="11"/>
-      <c r="FQ74" s="11"/>
-      <c r="FR74" s="11"/>
-      <c r="FS74" s="11"/>
-      <c r="FT74" s="11"/>
-      <c r="FU74" s="11"/>
-      <c r="FV74" s="11"/>
-      <c r="FW74" s="11"/>
-      <c r="FX74" s="11"/>
-      <c r="FY74" s="11"/>
-      <c r="FZ74" s="11"/>
-      <c r="GA74" s="11"/>
-      <c r="GB74" s="11"/>
-      <c r="GC74" s="11"/>
-      <c r="GD74" s="11"/>
-      <c r="GE74" s="11"/>
-      <c r="GF74" s="11"/>
-      <c r="GG74" s="11"/>
-      <c r="GH74" s="11"/>
-      <c r="GI74" s="11"/>
-      <c r="GJ74" s="11"/>
-      <c r="GK74" s="11"/>
-      <c r="GL74" s="11"/>
-      <c r="GM74" s="11"/>
-      <c r="GN74" s="11"/>
-      <c r="GO74" s="11"/>
-      <c r="GP74" s="11"/>
-      <c r="GQ74" s="11"/>
-      <c r="GR74" s="11"/>
-      <c r="GS74" s="11"/>
-      <c r="GT74" s="11"/>
-      <c r="GU74" s="11"/>
-      <c r="GV74" s="11"/>
-      <c r="GW74" s="11"/>
-      <c r="GX74" s="11"/>
-      <c r="GY74" s="11"/>
-      <c r="GZ74" s="11"/>
-      <c r="HA74" s="11"/>
-      <c r="HB74" s="11"/>
-      <c r="HC74" s="11"/>
-      <c r="HD74" s="11"/>
-      <c r="HE74" s="11"/>
-      <c r="HF74" s="11"/>
-      <c r="HG74" s="11"/>
-      <c r="HH74" s="11"/>
-      <c r="HI74" s="11"/>
-      <c r="HJ74" s="11"/>
-      <c r="HK74" s="11"/>
-      <c r="HL74" s="11"/>
-      <c r="HM74" s="11"/>
-      <c r="HN74" s="11"/>
-      <c r="HO74" s="11"/>
-      <c r="HP74" s="11"/>
-      <c r="HQ74" s="11"/>
-      <c r="HR74" s="11"/>
-      <c r="HS74" s="11"/>
-      <c r="HT74" s="11"/>
-      <c r="HU74" s="11"/>
-      <c r="HV74" s="11"/>
-      <c r="HW74" s="11"/>
-      <c r="HX74" s="11"/>
-      <c r="HY74" s="11"/>
-      <c r="HZ74" s="11"/>
-      <c r="IA74" s="11"/>
-      <c r="IB74" s="11"/>
-      <c r="IC74" s="11"/>
-      <c r="ID74" s="11"/>
-      <c r="IE74" s="11"/>
-      <c r="IF74" s="11"/>
-      <c r="IG74" s="11"/>
-      <c r="IH74" s="11"/>
-      <c r="II74" s="11"/>
-      <c r="IJ74" s="11"/>
-      <c r="IK74" s="11"/>
-      <c r="IL74" s="11"/>
-      <c r="IM74" s="11"/>
-      <c r="IN74" s="11"/>
-      <c r="IO74" s="11"/>
-      <c r="IP74" s="11"/>
-      <c r="IQ74" s="11"/>
-      <c r="IR74" s="11"/>
-      <c r="IS74" s="11"/>
-      <c r="IT74" s="11"/>
-      <c r="IU74" s="11"/>
-      <c r="IV74" s="11"/>
-      <c r="IW74" s="11"/>
-      <c r="IX74" s="11"/>
-      <c r="IY74" s="11"/>
-      <c r="IZ74" s="11"/>
-      <c r="JA74" s="11"/>
-      <c r="JB74" s="11"/>
-      <c r="JC74" s="11"/>
-      <c r="JD74" s="11"/>
-      <c r="JE74" s="11"/>
-      <c r="JF74" s="11"/>
-      <c r="JG74" s="11"/>
-      <c r="JH74" s="11"/>
-      <c r="JI74" s="11"/>
-      <c r="JJ74" s="11"/>
-      <c r="JK74" s="11"/>
-      <c r="JL74" s="11"/>
-      <c r="JM74" s="11"/>
-      <c r="JN74" s="11"/>
-      <c r="JO74" s="11"/>
-      <c r="JP74" s="11"/>
-      <c r="JQ74" s="11"/>
-      <c r="JR74" s="11"/>
-      <c r="JS74" s="11"/>
-      <c r="JT74" s="11"/>
-      <c r="JU74" s="11"/>
-      <c r="JV74" s="11"/>
-      <c r="JW74" s="11"/>
-      <c r="JX74" s="11"/>
-      <c r="JY74" s="11"/>
-      <c r="JZ74" s="11"/>
-      <c r="KA74" s="11"/>
-      <c r="KB74" s="11"/>
-      <c r="KC74" s="11"/>
-      <c r="KD74" s="11"/>
-      <c r="KE74" s="11"/>
-      <c r="KF74" s="11"/>
-      <c r="KG74" s="11"/>
-      <c r="KH74" s="11"/>
-      <c r="KI74" s="11"/>
-      <c r="KJ74" s="11"/>
-      <c r="KK74" s="11"/>
-      <c r="KL74" s="11"/>
-      <c r="KM74" s="11"/>
-      <c r="KN74" s="11"/>
-      <c r="KO74" s="11"/>
-      <c r="KP74" s="11"/>
-      <c r="KQ74" s="11"/>
-      <c r="KR74" s="11"/>
-      <c r="KS74" s="11"/>
-      <c r="KT74" s="11"/>
-      <c r="KU74" s="11"/>
-      <c r="KV74" s="11"/>
-      <c r="KW74" s="11"/>
-      <c r="KX74" s="11"/>
-      <c r="KY74" s="11"/>
-      <c r="KZ74" s="11"/>
-      <c r="LA74" s="11"/>
-      <c r="LB74" s="11"/>
-      <c r="LC74" s="11"/>
-      <c r="LD74" s="11"/>
-      <c r="LE74" s="11"/>
-      <c r="LF74" s="11"/>
-      <c r="LG74" s="11"/>
-      <c r="LH74" s="11"/>
-      <c r="LI74" s="11"/>
-      <c r="LJ74" s="11"/>
-      <c r="LK74" s="11"/>
-      <c r="LL74" s="11"/>
-      <c r="LM74" s="11"/>
-      <c r="LN74" s="11"/>
-      <c r="LO74" s="11"/>
-      <c r="LP74" s="11"/>
-      <c r="LQ74" s="11"/>
-      <c r="LR74" s="11"/>
-      <c r="LS74" s="11"/>
-      <c r="LT74" s="11"/>
-      <c r="LU74" s="11"/>
-      <c r="LV74" s="11"/>
-      <c r="LW74" s="11"/>
-      <c r="LX74" s="11"/>
-      <c r="LY74" s="11"/>
-      <c r="LZ74" s="11"/>
-      <c r="MA74" s="11"/>
-      <c r="MB74" s="11"/>
-      <c r="MC74" s="11"/>
-      <c r="MD74" s="11"/>
-      <c r="ME74" s="11"/>
-      <c r="MF74" s="11"/>
-      <c r="MG74" s="11"/>
-      <c r="MH74" s="11"/>
-      <c r="MI74" s="11"/>
-      <c r="MJ74" s="11"/>
-      <c r="MK74" s="11"/>
-      <c r="ML74" s="11"/>
-      <c r="MM74" s="11"/>
-      <c r="MN74" s="11"/>
-      <c r="MO74" s="11"/>
-      <c r="MP74" s="11"/>
-      <c r="MQ74" s="11"/>
-      <c r="MR74" s="11"/>
-      <c r="MS74" s="11"/>
-      <c r="MT74" s="11"/>
-      <c r="MU74" s="11"/>
-      <c r="MV74" s="11"/>
-      <c r="MW74" s="11"/>
-      <c r="MX74" s="11"/>
-      <c r="MY74" s="11"/>
-      <c r="MZ74" s="11"/>
-      <c r="NA74" s="11"/>
-      <c r="NB74" s="11"/>
-      <c r="NC74" s="11"/>
-      <c r="ND74" s="11"/>
-      <c r="NE74" s="11"/>
-      <c r="NF74" s="11"/>
-      <c r="NG74" s="11"/>
-      <c r="NH74" s="11"/>
-      <c r="NI74" s="11"/>
-      <c r="NJ74" s="11"/>
-      <c r="NK74" s="11"/>
-      <c r="NL74" s="11"/>
-      <c r="NM74" s="11"/>
-      <c r="NN74" s="11"/>
-      <c r="NO74" s="11"/>
-      <c r="NP74" s="11"/>
-      <c r="NQ74" s="11"/>
-      <c r="NR74" s="11"/>
-      <c r="NS74" s="11"/>
-      <c r="NT74" s="11"/>
-      <c r="NU74" s="11"/>
-      <c r="NV74" s="11"/>
-      <c r="NW74" s="11"/>
-      <c r="NX74" s="11"/>
-      <c r="NY74" s="11"/>
-      <c r="NZ74" s="11"/>
-      <c r="OA74" s="11"/>
-      <c r="OB74" s="11"/>
-      <c r="OC74" s="11"/>
-      <c r="OD74" s="11"/>
-      <c r="OE74" s="11"/>
-      <c r="OF74" s="11"/>
-      <c r="OG74" s="11"/>
-      <c r="OH74" s="11"/>
-      <c r="OI74" s="11"/>
-      <c r="OJ74" s="11"/>
-      <c r="OK74" s="11"/>
-      <c r="OL74" s="11"/>
-      <c r="OM74" s="11"/>
-      <c r="ON74" s="11"/>
-      <c r="OO74" s="11"/>
-      <c r="OP74" s="11"/>
-      <c r="OQ74" s="11"/>
-      <c r="OR74" s="11"/>
-      <c r="OS74" s="11"/>
-      <c r="OT74" s="11"/>
-      <c r="OU74" s="11"/>
-      <c r="OV74" s="11"/>
-      <c r="OW74" s="11"/>
-      <c r="OX74" s="11"/>
-      <c r="OY74" s="11"/>
-      <c r="OZ74" s="11"/>
-      <c r="PA74" s="11"/>
-      <c r="PB74" s="11"/>
-      <c r="PC74" s="11"/>
-      <c r="PD74" s="11"/>
-      <c r="PE74" s="11"/>
-      <c r="PF74" s="11"/>
-      <c r="PG74" s="11"/>
-      <c r="PH74" s="11"/>
-      <c r="PI74" s="11"/>
-      <c r="PJ74" s="11"/>
-      <c r="PK74" s="11"/>
-      <c r="PL74" s="11"/>
-      <c r="PM74" s="11"/>
-      <c r="PN74" s="11"/>
-      <c r="PO74" s="11"/>
-      <c r="PP74" s="11"/>
-      <c r="PQ74" s="11"/>
-      <c r="PR74" s="11"/>
-      <c r="PS74" s="11"/>
-      <c r="PT74" s="11"/>
-      <c r="PU74" s="11"/>
-      <c r="PV74" s="11"/>
-      <c r="PW74" s="11"/>
-      <c r="PX74" s="11"/>
-      <c r="PY74" s="11"/>
-      <c r="PZ74" s="11"/>
-      <c r="QA74" s="11"/>
-      <c r="QB74" s="11"/>
-      <c r="QC74" s="11"/>
-      <c r="QD74" s="11"/>
-      <c r="QE74" s="11"/>
-      <c r="QF74" s="11"/>
-      <c r="QG74" s="11"/>
-      <c r="QH74" s="11"/>
-      <c r="QI74" s="11"/>
-      <c r="QJ74" s="11"/>
-      <c r="QK74" s="11"/>
-      <c r="QL74" s="11"/>
-      <c r="QM74" s="11"/>
-      <c r="QN74" s="11"/>
-      <c r="QO74" s="11"/>
-      <c r="QP74" s="11"/>
-      <c r="QQ74" s="11"/>
-      <c r="QR74" s="11"/>
-      <c r="QS74" s="11"/>
-      <c r="QT74" s="11"/>
-      <c r="QU74" s="11"/>
-      <c r="QV74" s="11"/>
-      <c r="QW74" s="11"/>
-      <c r="QX74" s="11"/>
-      <c r="QY74" s="11"/>
-      <c r="QZ74" s="11"/>
-      <c r="RA74" s="11"/>
-      <c r="RB74" s="11"/>
-      <c r="RC74" s="11"/>
-      <c r="RD74" s="11"/>
-      <c r="RE74" s="11"/>
-      <c r="RF74" s="11"/>
-      <c r="RG74" s="11"/>
-      <c r="RH74" s="11"/>
-      <c r="RI74" s="11"/>
-      <c r="RJ74" s="11"/>
-      <c r="RK74" s="11"/>
-      <c r="RL74" s="11"/>
-      <c r="RM74" s="11"/>
-      <c r="RN74" s="11"/>
-      <c r="RO74" s="11"/>
-      <c r="RP74" s="11"/>
-      <c r="RQ74" s="11"/>
-      <c r="RR74" s="11"/>
-      <c r="RS74" s="11"/>
-      <c r="RT74" s="11"/>
-      <c r="RU74" s="11"/>
-      <c r="RV74" s="11"/>
-      <c r="RW74" s="11"/>
-      <c r="RX74" s="11"/>
-      <c r="RY74" s="11"/>
-      <c r="RZ74" s="11"/>
-      <c r="SA74" s="11"/>
-      <c r="SB74" s="11"/>
-      <c r="SC74" s="11"/>
-      <c r="SD74" s="11"/>
-      <c r="SE74" s="11"/>
-      <c r="SF74" s="11"/>
-      <c r="SG74" s="11"/>
-      <c r="SH74" s="11"/>
-      <c r="SI74" s="11"/>
-      <c r="SJ74" s="11"/>
-      <c r="SK74" s="11"/>
-      <c r="SL74" s="11"/>
-      <c r="SM74" s="11"/>
-      <c r="SN74" s="11"/>
-      <c r="SO74" s="11"/>
-      <c r="SP74" s="11"/>
-      <c r="SQ74" s="11"/>
-      <c r="SR74" s="11"/>
-      <c r="SS74" s="11"/>
-      <c r="ST74" s="11"/>
-      <c r="SU74" s="11"/>
-      <c r="SV74" s="11"/>
-      <c r="SW74" s="11"/>
-      <c r="SX74" s="11"/>
-      <c r="SY74" s="11"/>
-      <c r="SZ74" s="11"/>
-      <c r="TA74" s="11"/>
-      <c r="TB74" s="11"/>
-      <c r="TC74" s="11"/>
-      <c r="TD74" s="11"/>
-      <c r="TE74" s="11"/>
-      <c r="TF74" s="11"/>
-      <c r="TG74" s="11"/>
-      <c r="TH74" s="11"/>
-      <c r="TI74" s="11"/>
-      <c r="TJ74" s="11"/>
-      <c r="TK74" s="11"/>
-      <c r="TL74" s="11"/>
-      <c r="TM74" s="11"/>
-      <c r="TN74" s="11"/>
-      <c r="TO74" s="11"/>
-      <c r="TP74" s="11"/>
-      <c r="TQ74" s="11"/>
-      <c r="TR74" s="11"/>
-      <c r="TS74" s="11"/>
-      <c r="TT74" s="11"/>
-      <c r="TU74" s="11"/>
-      <c r="TV74" s="11"/>
-      <c r="TW74" s="11"/>
-      <c r="TX74" s="11"/>
-      <c r="TY74" s="11"/>
-      <c r="TZ74" s="11"/>
-      <c r="UA74" s="11"/>
-      <c r="UB74" s="11"/>
-      <c r="UC74" s="11"/>
-      <c r="UD74" s="11"/>
-      <c r="UE74" s="11"/>
-      <c r="UF74" s="11"/>
-      <c r="UG74" s="11"/>
-      <c r="UH74" s="11"/>
-      <c r="UI74" s="11"/>
-      <c r="UJ74" s="11"/>
-      <c r="UK74" s="11"/>
-      <c r="UL74" s="11"/>
-      <c r="UM74" s="11"/>
-      <c r="UN74" s="11"/>
-      <c r="UO74" s="11"/>
-      <c r="UP74" s="11"/>
-      <c r="UQ74" s="11"/>
-      <c r="UR74" s="11"/>
-      <c r="US74" s="11"/>
-      <c r="UT74" s="11"/>
-      <c r="UU74" s="11"/>
-      <c r="UV74" s="11"/>
-      <c r="UW74" s="11"/>
-      <c r="UX74" s="11"/>
-      <c r="UY74" s="11"/>
-      <c r="UZ74" s="11"/>
-      <c r="VA74" s="11"/>
-      <c r="VB74" s="11"/>
-      <c r="VC74" s="11"/>
-      <c r="VD74" s="11"/>
-      <c r="VE74" s="11"/>
-      <c r="VF74" s="11"/>
-      <c r="VG74" s="11"/>
-      <c r="VH74" s="11"/>
-      <c r="VI74" s="11"/>
-      <c r="VJ74" s="11"/>
-      <c r="VK74" s="11"/>
-      <c r="VL74" s="11"/>
-      <c r="VM74" s="11"/>
-      <c r="VN74" s="11"/>
-      <c r="VO74" s="11"/>
-      <c r="VP74" s="11"/>
-      <c r="VQ74" s="11"/>
-      <c r="VR74" s="11"/>
-      <c r="VS74" s="11"/>
-      <c r="VT74" s="11"/>
-      <c r="VU74" s="11"/>
-      <c r="VV74" s="11"/>
-      <c r="VW74" s="11"/>
-      <c r="VX74" s="11"/>
-      <c r="VY74" s="11"/>
-      <c r="VZ74" s="11"/>
-      <c r="WA74" s="11"/>
-      <c r="WB74" s="11"/>
-      <c r="WC74" s="11"/>
-      <c r="WD74" s="11"/>
-      <c r="WE74" s="11"/>
-      <c r="WF74" s="11"/>
-      <c r="WG74" s="11"/>
-      <c r="WH74" s="11"/>
-      <c r="WI74" s="11"/>
-      <c r="WJ74" s="11"/>
-      <c r="WK74" s="11"/>
-      <c r="WL74" s="11"/>
-      <c r="WM74" s="11"/>
-      <c r="WN74" s="11"/>
-      <c r="WO74" s="11"/>
-      <c r="WP74" s="11"/>
-      <c r="WQ74" s="11"/>
-      <c r="WR74" s="11"/>
-      <c r="WS74" s="11"/>
-      <c r="WT74" s="11"/>
-      <c r="WU74" s="11"/>
-      <c r="WV74" s="11"/>
-      <c r="WW74" s="11"/>
-      <c r="WX74" s="11"/>
-      <c r="WY74" s="11"/>
-      <c r="WZ74" s="11"/>
-      <c r="XA74" s="11"/>
-      <c r="XB74" s="11"/>
-      <c r="XC74" s="11"/>
-      <c r="XD74" s="11"/>
-      <c r="XE74" s="11"/>
-      <c r="XF74" s="11"/>
-      <c r="XG74" s="11"/>
-      <c r="XH74" s="11"/>
-      <c r="XI74" s="11"/>
-      <c r="XJ74" s="11"/>
-      <c r="XK74" s="11"/>
-      <c r="XL74" s="11"/>
-      <c r="XM74" s="11"/>
-      <c r="XN74" s="11"/>
-      <c r="XO74" s="11"/>
-      <c r="XP74" s="11"/>
-      <c r="XQ74" s="11"/>
-      <c r="XR74" s="11"/>
-      <c r="XS74" s="11"/>
-      <c r="XT74" s="11"/>
-      <c r="XU74" s="11"/>
-      <c r="XV74" s="11"/>
-      <c r="XW74" s="11"/>
-      <c r="XX74" s="11"/>
-      <c r="XY74" s="11"/>
-      <c r="XZ74" s="11"/>
-      <c r="YA74" s="11"/>
-      <c r="YB74" s="11"/>
-      <c r="YC74" s="11"/>
-      <c r="YD74" s="11"/>
-      <c r="YE74" s="11"/>
-      <c r="YF74" s="11"/>
-      <c r="YG74" s="11"/>
-      <c r="YH74" s="11"/>
-      <c r="YI74" s="11"/>
-      <c r="YJ74" s="11"/>
-      <c r="YK74" s="11"/>
-      <c r="YL74" s="11"/>
-      <c r="YM74" s="11"/>
-      <c r="YN74" s="11"/>
-      <c r="YO74" s="11"/>
-      <c r="YP74" s="11"/>
-      <c r="YQ74" s="11"/>
-      <c r="YR74" s="11"/>
-      <c r="YS74" s="11"/>
-      <c r="YT74" s="11"/>
-      <c r="YU74" s="11"/>
-      <c r="YV74" s="11"/>
-      <c r="YW74" s="11"/>
-      <c r="YX74" s="11"/>
-      <c r="YY74" s="11"/>
-      <c r="YZ74" s="11"/>
-      <c r="ZA74" s="11"/>
-      <c r="ZB74" s="11"/>
-      <c r="ZC74" s="11"/>
-      <c r="ZD74" s="11"/>
-      <c r="ZE74" s="11"/>
-      <c r="ZF74" s="11"/>
-      <c r="ZG74" s="11"/>
-      <c r="ZH74" s="11"/>
-      <c r="ZI74" s="11"/>
-      <c r="ZJ74" s="11"/>
-      <c r="ZK74" s="11"/>
-      <c r="ZL74" s="11"/>
-      <c r="ZM74" s="11"/>
-      <c r="ZN74" s="11"/>
-      <c r="ZO74" s="11"/>
-      <c r="ZP74" s="11"/>
-      <c r="ZQ74" s="11"/>
-      <c r="ZR74" s="11"/>
-      <c r="ZS74" s="11"/>
-      <c r="ZT74" s="11"/>
-      <c r="ZU74" s="11"/>
-      <c r="ZV74" s="11"/>
-      <c r="ZW74" s="11"/>
-      <c r="ZX74" s="11"/>
-      <c r="ZY74" s="11"/>
-      <c r="ZZ74" s="11"/>
-      <c r="AAA74" s="11"/>
-      <c r="AAB74" s="11"/>
-      <c r="AAC74" s="11"/>
-      <c r="AAD74" s="11"/>
-      <c r="AAE74" s="11"/>
-      <c r="AAF74" s="11"/>
-      <c r="AAG74" s="11"/>
-      <c r="AAH74" s="11"/>
-      <c r="AAI74" s="11"/>
-      <c r="AAJ74" s="11"/>
-      <c r="AAK74" s="11"/>
-      <c r="AAL74" s="11"/>
-      <c r="AAM74" s="11"/>
-      <c r="AAN74" s="11"/>
-      <c r="AAO74" s="11"/>
-      <c r="AAP74" s="11"/>
-      <c r="AAQ74" s="11"/>
-      <c r="AAR74" s="11"/>
-      <c r="AAS74" s="11"/>
-      <c r="AAT74" s="11"/>
-      <c r="AAU74" s="11"/>
-      <c r="AAV74" s="11"/>
-      <c r="AAW74" s="11"/>
-      <c r="AAX74" s="11"/>
-      <c r="AAY74" s="11"/>
-      <c r="AAZ74" s="11"/>
-      <c r="ABA74" s="11"/>
-      <c r="ABB74" s="11"/>
-      <c r="ABC74" s="11"/>
-      <c r="ABD74" s="11"/>
-      <c r="ABE74" s="11"/>
-      <c r="ABF74" s="11"/>
-      <c r="ABG74" s="11"/>
-      <c r="ABH74" s="11"/>
-      <c r="ABI74" s="11"/>
-      <c r="ABJ74" s="11"/>
-      <c r="ABK74" s="11"/>
-      <c r="ABL74" s="11"/>
-      <c r="ABM74" s="11"/>
-      <c r="ABN74" s="11"/>
-      <c r="ABO74" s="11"/>
-      <c r="ABP74" s="11"/>
-      <c r="ABQ74" s="11"/>
-      <c r="ABR74" s="11"/>
-      <c r="ABS74" s="11"/>
-      <c r="ABT74" s="11"/>
-      <c r="ABU74" s="11"/>
-      <c r="ABV74" s="11"/>
-      <c r="ABW74" s="11"/>
-      <c r="ABX74" s="11"/>
-      <c r="ABY74" s="11"/>
-      <c r="ABZ74" s="11"/>
-      <c r="ACA74" s="11"/>
-      <c r="ACB74" s="11"/>
-      <c r="ACC74" s="11"/>
-      <c r="ACD74" s="11"/>
-      <c r="ACE74" s="11"/>
-      <c r="ACF74" s="11"/>
-      <c r="ACG74" s="11"/>
-      <c r="ACH74" s="11"/>
-      <c r="ACI74" s="11"/>
-      <c r="ACJ74" s="11"/>
-      <c r="ACK74" s="11"/>
-      <c r="ACL74" s="11"/>
-      <c r="ACM74" s="11"/>
-      <c r="ACN74" s="11"/>
-      <c r="ACO74" s="11"/>
-      <c r="ACP74" s="11"/>
-      <c r="ACQ74" s="11"/>
-      <c r="ACR74" s="11"/>
-      <c r="ACS74" s="11"/>
-      <c r="ACT74" s="11"/>
-      <c r="ACU74" s="11"/>
-      <c r="ACV74" s="11"/>
-      <c r="ACW74" s="11"/>
-      <c r="ACX74" s="11"/>
-      <c r="ACY74" s="11"/>
-      <c r="ACZ74" s="11"/>
-      <c r="ADA74" s="11"/>
-      <c r="ADB74" s="11"/>
-      <c r="ADC74" s="11"/>
-      <c r="ADD74" s="11"/>
-      <c r="ADE74" s="11"/>
-      <c r="ADF74" s="11"/>
-      <c r="ADG74" s="11"/>
-      <c r="ADH74" s="11"/>
-      <c r="ADI74" s="11"/>
-      <c r="ADJ74" s="11"/>
-      <c r="ADK74" s="11"/>
-      <c r="ADL74" s="11"/>
-      <c r="ADM74" s="11"/>
-      <c r="ADN74" s="11"/>
-      <c r="ADO74" s="11"/>
-      <c r="ADP74" s="11"/>
-      <c r="ADQ74" s="11"/>
-      <c r="ADR74" s="11"/>
-      <c r="ADS74" s="11"/>
-      <c r="ADT74" s="11"/>
-      <c r="ADU74" s="11"/>
-      <c r="ADV74" s="11"/>
-      <c r="ADW74" s="11"/>
-      <c r="ADX74" s="11"/>
-      <c r="ADY74" s="11"/>
-      <c r="ADZ74" s="11"/>
-      <c r="AEA74" s="11"/>
-      <c r="AEB74" s="11"/>
-      <c r="AEC74" s="11"/>
-      <c r="AED74" s="11"/>
-      <c r="AEE74" s="11"/>
-      <c r="AEF74" s="11"/>
-      <c r="AEG74" s="11"/>
-      <c r="AEH74" s="11"/>
-      <c r="AEI74" s="11"/>
-      <c r="AEJ74" s="11"/>
-      <c r="AEK74" s="11"/>
-      <c r="AEL74" s="11"/>
-      <c r="AEM74" s="11"/>
-      <c r="AEN74" s="11"/>
-      <c r="AEO74" s="11"/>
-      <c r="AEP74" s="11"/>
-      <c r="AEQ74" s="11"/>
-      <c r="AER74" s="11"/>
-      <c r="AES74" s="11"/>
-      <c r="AET74" s="11"/>
-      <c r="AEU74" s="11"/>
-      <c r="AEV74" s="11"/>
-      <c r="AEW74" s="11"/>
-      <c r="AEX74" s="11"/>
-      <c r="AEY74" s="11"/>
-      <c r="AEZ74" s="11"/>
-      <c r="AFA74" s="11"/>
-      <c r="AFB74" s="11"/>
-      <c r="AFC74" s="11"/>
-      <c r="AFD74" s="11"/>
-      <c r="AFE74" s="11"/>
-      <c r="AFF74" s="11"/>
-      <c r="AFG74" s="11"/>
-      <c r="AFH74" s="11"/>
-      <c r="AFI74" s="11"/>
-      <c r="AFJ74" s="11"/>
-      <c r="AFK74" s="11"/>
-      <c r="AFL74" s="11"/>
-      <c r="AFM74" s="11"/>
-      <c r="AFN74" s="11"/>
-      <c r="AFO74" s="11"/>
-      <c r="AFP74" s="11"/>
-      <c r="AFQ74" s="11"/>
-      <c r="AFR74" s="11"/>
-      <c r="AFS74" s="11"/>
-      <c r="AFT74" s="11"/>
-      <c r="AFU74" s="11"/>
-      <c r="AFV74" s="11"/>
-      <c r="AFW74" s="11"/>
-      <c r="AFX74" s="11"/>
-      <c r="AFY74" s="11"/>
-      <c r="AFZ74" s="11"/>
-      <c r="AGA74" s="11"/>
-      <c r="AGB74" s="11"/>
-      <c r="AGC74" s="11"/>
-      <c r="AGD74" s="11"/>
-      <c r="AGE74" s="11"/>
-      <c r="AGF74" s="11"/>
-      <c r="AGG74" s="11"/>
-      <c r="AGH74" s="11"/>
-      <c r="AGI74" s="11"/>
-      <c r="AGJ74" s="11"/>
-      <c r="AGK74" s="11"/>
-      <c r="AGL74" s="11"/>
-      <c r="AGM74" s="11"/>
-      <c r="AGN74" s="11"/>
-      <c r="AGO74" s="11"/>
-      <c r="AGP74" s="11"/>
-      <c r="AGQ74" s="11"/>
-      <c r="AGR74" s="11"/>
-      <c r="AGS74" s="11"/>
-      <c r="AGT74" s="11"/>
-      <c r="AGU74" s="11"/>
-      <c r="AGV74" s="11"/>
-      <c r="AGW74" s="11"/>
-      <c r="AGX74" s="11"/>
-      <c r="AGY74" s="11"/>
-      <c r="AGZ74" s="11"/>
-      <c r="AHA74" s="11"/>
-      <c r="AHB74" s="11"/>
-      <c r="AHC74" s="11"/>
-      <c r="AHD74" s="11"/>
-      <c r="AHE74" s="11"/>
-      <c r="AHF74" s="11"/>
-      <c r="AHG74" s="11"/>
-      <c r="AHH74" s="11"/>
-      <c r="AHI74" s="11"/>
-      <c r="AHJ74" s="11"/>
-      <c r="AHK74" s="11"/>
-      <c r="AHL74" s="11"/>
-      <c r="AHM74" s="11"/>
-      <c r="AHN74" s="11"/>
-      <c r="AHO74" s="11"/>
-      <c r="AHP74" s="11"/>
-      <c r="AHQ74" s="11"/>
-      <c r="AHR74" s="11"/>
-      <c r="AHS74" s="11"/>
-      <c r="AHT74" s="11"/>
-      <c r="AHU74" s="11"/>
-      <c r="AHV74" s="11"/>
-      <c r="AHW74" s="11"/>
-      <c r="AHX74" s="11"/>
-      <c r="AHY74" s="11"/>
-      <c r="AHZ74" s="11"/>
-      <c r="AIA74" s="11"/>
-      <c r="AIB74" s="11"/>
-      <c r="AIC74" s="11"/>
-      <c r="AID74" s="11"/>
-      <c r="AIE74" s="11"/>
-      <c r="AIF74" s="11"/>
-      <c r="AIG74" s="11"/>
-      <c r="AIH74" s="11"/>
-      <c r="AII74" s="11"/>
-      <c r="AIJ74" s="11"/>
-      <c r="AIK74" s="11"/>
-      <c r="AIL74" s="11"/>
-      <c r="AIM74" s="11"/>
-      <c r="AIN74" s="11"/>
-      <c r="AIO74" s="11"/>
-      <c r="AIP74" s="11"/>
-      <c r="AIQ74" s="11"/>
-      <c r="AIR74" s="11"/>
-      <c r="AIS74" s="11"/>
-      <c r="AIT74" s="11"/>
-      <c r="AIU74" s="11"/>
-      <c r="AIV74" s="11"/>
-      <c r="AIW74" s="11"/>
-      <c r="AIX74" s="11"/>
-      <c r="AIY74" s="11"/>
-      <c r="AIZ74" s="11"/>
-      <c r="AJA74" s="11"/>
-      <c r="AJB74" s="11"/>
-      <c r="AJC74" s="11"/>
-      <c r="AJD74" s="11"/>
-      <c r="AJE74" s="11"/>
-      <c r="AJF74" s="11"/>
-      <c r="AJG74" s="11"/>
-      <c r="AJH74" s="11"/>
-      <c r="AJI74" s="11"/>
-      <c r="AJJ74" s="11"/>
-      <c r="AJK74" s="11"/>
-      <c r="AJL74" s="11"/>
-      <c r="AJM74" s="11"/>
-      <c r="AJN74" s="11"/>
-      <c r="AJO74" s="11"/>
-      <c r="AJP74" s="11"/>
-      <c r="AJQ74" s="11"/>
-      <c r="AJR74" s="11"/>
-      <c r="AJS74" s="11"/>
-      <c r="AJT74" s="11"/>
-      <c r="AJU74" s="11"/>
-      <c r="AJV74" s="11"/>
-      <c r="AJW74" s="11"/>
-      <c r="AJX74" s="11"/>
-      <c r="AJY74" s="11"/>
-      <c r="AJZ74" s="11"/>
-      <c r="AKA74" s="11"/>
-      <c r="AKB74" s="11"/>
-      <c r="AKC74" s="11"/>
-      <c r="AKD74" s="11"/>
-      <c r="AKE74" s="11"/>
-      <c r="AKF74" s="11"/>
-      <c r="AKG74" s="11"/>
-      <c r="AKH74" s="11"/>
-      <c r="AKI74" s="11"/>
-      <c r="AKJ74" s="11"/>
-      <c r="AKK74" s="11"/>
-      <c r="AKL74" s="11"/>
-      <c r="AKM74" s="11"/>
-      <c r="AKN74" s="11"/>
-      <c r="AKO74" s="11"/>
-      <c r="AKP74" s="11"/>
-      <c r="AKQ74" s="11"/>
-      <c r="AKR74" s="11"/>
-      <c r="AKS74" s="11"/>
-      <c r="AKT74" s="11"/>
-      <c r="AKU74" s="11"/>
-      <c r="AKV74" s="11"/>
-      <c r="AKW74" s="11"/>
-      <c r="AKX74" s="11"/>
-      <c r="AKY74" s="11"/>
-      <c r="AKZ74" s="11"/>
-      <c r="ALA74" s="11"/>
-      <c r="ALB74" s="11"/>
-      <c r="ALC74" s="11"/>
-      <c r="ALD74" s="11"/>
-      <c r="ALE74" s="11"/>
-      <c r="ALF74" s="11"/>
-      <c r="ALG74" s="11"/>
-      <c r="ALH74" s="11"/>
-      <c r="ALI74" s="11"/>
-      <c r="ALJ74" s="11"/>
-      <c r="ALK74" s="11"/>
-      <c r="ALL74" s="11"/>
-      <c r="ALM74" s="11"/>
-      <c r="ALN74" s="11"/>
-      <c r="ALO74" s="11"/>
-      <c r="ALP74" s="11"/>
-      <c r="ALQ74" s="11"/>
-      <c r="ALR74" s="11"/>
-      <c r="ALS74" s="11"/>
-      <c r="ALT74" s="11"/>
-      <c r="ALU74" s="11"/>
-      <c r="ALV74" s="11"/>
-      <c r="ALW74" s="11"/>
-      <c r="ALX74" s="11"/>
-      <c r="ALY74" s="11"/>
-      <c r="ALZ74" s="11"/>
-      <c r="AMA74" s="11"/>
-      <c r="AMB74" s="11"/>
-      <c r="AMC74" s="11"/>
-      <c r="AMD74" s="11"/>
-      <c r="AME74" s="11"/>
-      <c r="AMF74" s="11"/>
-      <c r="AMG74" s="11"/>
-      <c r="AMH74" s="11"/>
-      <c r="AMI74" s="11"/>
-      <c r="AMJ74" s="11"/>
-    </row>
+    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="11"/>
+      <c r="P71" s="11"/>
+      <c r="Q71" s="11"/>
+      <c r="R71" s="11"/>
+      <c r="S71" s="11"/>
+      <c r="T71" s="11"/>
+      <c r="U71" s="11"/>
+      <c r="V71" s="11"/>
+      <c r="W71" s="11"/>
+      <c r="X71" s="11"/>
+      <c r="Y71" s="11"/>
+      <c r="Z71" s="11"/>
+      <c r="AA71" s="11"/>
+      <c r="AB71" s="11"/>
+      <c r="AC71" s="11"/>
+      <c r="AD71" s="11"/>
+      <c r="AE71" s="11"/>
+      <c r="AF71" s="11"/>
+      <c r="AG71" s="11"/>
+      <c r="AH71" s="11"/>
+      <c r="AI71" s="11"/>
+      <c r="AJ71" s="11"/>
+      <c r="AK71" s="11"/>
+      <c r="AL71" s="11"/>
+      <c r="AM71" s="11"/>
+      <c r="AN71" s="11"/>
+      <c r="AO71" s="11"/>
+      <c r="AP71" s="11"/>
+      <c r="AQ71" s="11"/>
+      <c r="AR71" s="11"/>
+      <c r="AS71" s="11"/>
+      <c r="AT71" s="11"/>
+      <c r="AU71" s="11"/>
+      <c r="AV71" s="11"/>
+      <c r="AW71" s="11"/>
+      <c r="AX71" s="11"/>
+      <c r="AY71" s="11"/>
+      <c r="AZ71" s="11"/>
+      <c r="BA71" s="11"/>
+      <c r="BB71" s="11"/>
+      <c r="BC71" s="11"/>
+      <c r="BD71" s="11"/>
+      <c r="BE71" s="11"/>
+      <c r="BF71" s="11"/>
+      <c r="BG71" s="11"/>
+      <c r="BH71" s="11"/>
+      <c r="BI71" s="11"/>
+      <c r="BJ71" s="11"/>
+      <c r="BK71" s="11"/>
+      <c r="BL71" s="11"/>
+      <c r="BM71" s="11"/>
+      <c r="BN71" s="11"/>
+      <c r="BO71" s="11"/>
+      <c r="BP71" s="11"/>
+      <c r="BQ71" s="11"/>
+      <c r="BR71" s="11"/>
+      <c r="BS71" s="11"/>
+      <c r="BT71" s="11"/>
+      <c r="BU71" s="11"/>
+      <c r="BV71" s="11"/>
+      <c r="BW71" s="11"/>
+      <c r="BX71" s="11"/>
+      <c r="BY71" s="11"/>
+      <c r="BZ71" s="11"/>
+      <c r="CA71" s="11"/>
+      <c r="CB71" s="11"/>
+      <c r="CC71" s="11"/>
+      <c r="CD71" s="11"/>
+      <c r="CE71" s="11"/>
+      <c r="CF71" s="11"/>
+      <c r="CG71" s="11"/>
+      <c r="CH71" s="11"/>
+      <c r="CI71" s="11"/>
+      <c r="CJ71" s="11"/>
+      <c r="CK71" s="11"/>
+      <c r="CL71" s="11"/>
+      <c r="CM71" s="11"/>
+      <c r="CN71" s="11"/>
+      <c r="CO71" s="11"/>
+      <c r="CP71" s="11"/>
+      <c r="CQ71" s="11"/>
+      <c r="CR71" s="11"/>
+      <c r="CS71" s="11"/>
+      <c r="CT71" s="11"/>
+      <c r="CU71" s="11"/>
+      <c r="CV71" s="11"/>
+      <c r="CW71" s="11"/>
+      <c r="CX71" s="11"/>
+      <c r="CY71" s="11"/>
+      <c r="CZ71" s="11"/>
+      <c r="DA71" s="11"/>
+      <c r="DB71" s="11"/>
+      <c r="DC71" s="11"/>
+      <c r="DD71" s="11"/>
+      <c r="DE71" s="11"/>
+      <c r="DF71" s="11"/>
+      <c r="DG71" s="11"/>
+      <c r="DH71" s="11"/>
+      <c r="DI71" s="11"/>
+      <c r="DJ71" s="11"/>
+      <c r="DK71" s="11"/>
+      <c r="DL71" s="11"/>
+      <c r="DM71" s="11"/>
+      <c r="DN71" s="11"/>
+      <c r="DO71" s="11"/>
+      <c r="DP71" s="11"/>
+      <c r="DQ71" s="11"/>
+      <c r="DR71" s="11"/>
+      <c r="DS71" s="11"/>
+      <c r="DT71" s="11"/>
+      <c r="DU71" s="11"/>
+      <c r="DV71" s="11"/>
+      <c r="DW71" s="11"/>
+      <c r="DX71" s="11"/>
+      <c r="DY71" s="11"/>
+      <c r="DZ71" s="11"/>
+      <c r="EA71" s="11"/>
+      <c r="EB71" s="11"/>
+      <c r="EC71" s="11"/>
+      <c r="ED71" s="11"/>
+      <c r="EE71" s="11"/>
+      <c r="EF71" s="11"/>
+      <c r="EG71" s="11"/>
+      <c r="EH71" s="11"/>
+      <c r="EI71" s="11"/>
+      <c r="EJ71" s="11"/>
+      <c r="EK71" s="11"/>
+      <c r="EL71" s="11"/>
+      <c r="EM71" s="11"/>
+      <c r="EN71" s="11"/>
+      <c r="EO71" s="11"/>
+      <c r="EP71" s="11"/>
+      <c r="EQ71" s="11"/>
+      <c r="ER71" s="11"/>
+      <c r="ES71" s="11"/>
+      <c r="ET71" s="11"/>
+      <c r="EU71" s="11"/>
+      <c r="EV71" s="11"/>
+      <c r="EW71" s="11"/>
+      <c r="EX71" s="11"/>
+      <c r="EY71" s="11"/>
+      <c r="EZ71" s="11"/>
+      <c r="FA71" s="11"/>
+      <c r="FB71" s="11"/>
+      <c r="FC71" s="11"/>
+      <c r="FD71" s="11"/>
+      <c r="FE71" s="11"/>
+      <c r="FF71" s="11"/>
+      <c r="FG71" s="11"/>
+      <c r="FH71" s="11"/>
+      <c r="FI71" s="11"/>
+      <c r="FJ71" s="11"/>
+      <c r="FK71" s="11"/>
+      <c r="FL71" s="11"/>
+      <c r="FM71" s="11"/>
+      <c r="FN71" s="11"/>
+      <c r="FO71" s="11"/>
+      <c r="FP71" s="11"/>
+      <c r="FQ71" s="11"/>
+      <c r="FR71" s="11"/>
+      <c r="FS71" s="11"/>
+      <c r="FT71" s="11"/>
+      <c r="FU71" s="11"/>
+      <c r="FV71" s="11"/>
+      <c r="FW71" s="11"/>
+      <c r="FX71" s="11"/>
+      <c r="FY71" s="11"/>
+      <c r="FZ71" s="11"/>
+      <c r="GA71" s="11"/>
+      <c r="GB71" s="11"/>
+      <c r="GC71" s="11"/>
+      <c r="GD71" s="11"/>
+      <c r="GE71" s="11"/>
+      <c r="GF71" s="11"/>
+      <c r="GG71" s="11"/>
+      <c r="GH71" s="11"/>
+      <c r="GI71" s="11"/>
+      <c r="GJ71" s="11"/>
+      <c r="GK71" s="11"/>
+      <c r="GL71" s="11"/>
+      <c r="GM71" s="11"/>
+      <c r="GN71" s="11"/>
+      <c r="GO71" s="11"/>
+      <c r="GP71" s="11"/>
+      <c r="GQ71" s="11"/>
+      <c r="GR71" s="11"/>
+      <c r="GS71" s="11"/>
+      <c r="GT71" s="11"/>
+      <c r="GU71" s="11"/>
+      <c r="GV71" s="11"/>
+      <c r="GW71" s="11"/>
+      <c r="GX71" s="11"/>
+      <c r="GY71" s="11"/>
+      <c r="GZ71" s="11"/>
+      <c r="HA71" s="11"/>
+      <c r="HB71" s="11"/>
+      <c r="HC71" s="11"/>
+      <c r="HD71" s="11"/>
+      <c r="HE71" s="11"/>
+      <c r="HF71" s="11"/>
+      <c r="HG71" s="11"/>
+      <c r="HH71" s="11"/>
+      <c r="HI71" s="11"/>
+      <c r="HJ71" s="11"/>
+      <c r="HK71" s="11"/>
+      <c r="HL71" s="11"/>
+      <c r="HM71" s="11"/>
+      <c r="HN71" s="11"/>
+      <c r="HO71" s="11"/>
+      <c r="HP71" s="11"/>
+      <c r="HQ71" s="11"/>
+      <c r="HR71" s="11"/>
+      <c r="HS71" s="11"/>
+      <c r="HT71" s="11"/>
+      <c r="HU71" s="11"/>
+      <c r="HV71" s="11"/>
+      <c r="HW71" s="11"/>
+      <c r="HX71" s="11"/>
+      <c r="HY71" s="11"/>
+      <c r="HZ71" s="11"/>
+      <c r="IA71" s="11"/>
+      <c r="IB71" s="11"/>
+      <c r="IC71" s="11"/>
+      <c r="ID71" s="11"/>
+      <c r="IE71" s="11"/>
+      <c r="IF71" s="11"/>
+      <c r="IG71" s="11"/>
+      <c r="IH71" s="11"/>
+      <c r="II71" s="11"/>
+      <c r="IJ71" s="11"/>
+      <c r="IK71" s="11"/>
+      <c r="IL71" s="11"/>
+      <c r="IM71" s="11"/>
+      <c r="IN71" s="11"/>
+      <c r="IO71" s="11"/>
+      <c r="IP71" s="11"/>
+      <c r="IQ71" s="11"/>
+      <c r="IR71" s="11"/>
+      <c r="IS71" s="11"/>
+      <c r="IT71" s="11"/>
+      <c r="IU71" s="11"/>
+      <c r="IV71" s="11"/>
+      <c r="IW71" s="11"/>
+      <c r="IX71" s="11"/>
+      <c r="IY71" s="11"/>
+      <c r="IZ71" s="11"/>
+      <c r="JA71" s="11"/>
+      <c r="JB71" s="11"/>
+      <c r="JC71" s="11"/>
+      <c r="JD71" s="11"/>
+      <c r="JE71" s="11"/>
+      <c r="JF71" s="11"/>
+      <c r="JG71" s="11"/>
+      <c r="JH71" s="11"/>
+      <c r="JI71" s="11"/>
+      <c r="JJ71" s="11"/>
+      <c r="JK71" s="11"/>
+      <c r="JL71" s="11"/>
+      <c r="JM71" s="11"/>
+      <c r="JN71" s="11"/>
+      <c r="JO71" s="11"/>
+      <c r="JP71" s="11"/>
+      <c r="JQ71" s="11"/>
+      <c r="JR71" s="11"/>
+      <c r="JS71" s="11"/>
+      <c r="JT71" s="11"/>
+      <c r="JU71" s="11"/>
+      <c r="JV71" s="11"/>
+      <c r="JW71" s="11"/>
+      <c r="JX71" s="11"/>
+      <c r="JY71" s="11"/>
+      <c r="JZ71" s="11"/>
+      <c r="KA71" s="11"/>
+      <c r="KB71" s="11"/>
+      <c r="KC71" s="11"/>
+      <c r="KD71" s="11"/>
+      <c r="KE71" s="11"/>
+      <c r="KF71" s="11"/>
+      <c r="KG71" s="11"/>
+      <c r="KH71" s="11"/>
+      <c r="KI71" s="11"/>
+      <c r="KJ71" s="11"/>
+      <c r="KK71" s="11"/>
+      <c r="KL71" s="11"/>
+      <c r="KM71" s="11"/>
+      <c r="KN71" s="11"/>
+      <c r="KO71" s="11"/>
+      <c r="KP71" s="11"/>
+      <c r="KQ71" s="11"/>
+      <c r="KR71" s="11"/>
+      <c r="KS71" s="11"/>
+      <c r="KT71" s="11"/>
+      <c r="KU71" s="11"/>
+      <c r="KV71" s="11"/>
+      <c r="KW71" s="11"/>
+      <c r="KX71" s="11"/>
+      <c r="KY71" s="11"/>
+      <c r="KZ71" s="11"/>
+      <c r="LA71" s="11"/>
+      <c r="LB71" s="11"/>
+      <c r="LC71" s="11"/>
+      <c r="LD71" s="11"/>
+      <c r="LE71" s="11"/>
+      <c r="LF71" s="11"/>
+      <c r="LG71" s="11"/>
+      <c r="LH71" s="11"/>
+      <c r="LI71" s="11"/>
+      <c r="LJ71" s="11"/>
+      <c r="LK71" s="11"/>
+      <c r="LL71" s="11"/>
+      <c r="LM71" s="11"/>
+      <c r="LN71" s="11"/>
+      <c r="LO71" s="11"/>
+      <c r="LP71" s="11"/>
+      <c r="LQ71" s="11"/>
+      <c r="LR71" s="11"/>
+      <c r="LS71" s="11"/>
+      <c r="LT71" s="11"/>
+      <c r="LU71" s="11"/>
+      <c r="LV71" s="11"/>
+      <c r="LW71" s="11"/>
+      <c r="LX71" s="11"/>
+      <c r="LY71" s="11"/>
+      <c r="LZ71" s="11"/>
+      <c r="MA71" s="11"/>
+      <c r="MB71" s="11"/>
+      <c r="MC71" s="11"/>
+      <c r="MD71" s="11"/>
+      <c r="ME71" s="11"/>
+      <c r="MF71" s="11"/>
+      <c r="MG71" s="11"/>
+      <c r="MH71" s="11"/>
+      <c r="MI71" s="11"/>
+      <c r="MJ71" s="11"/>
+      <c r="MK71" s="11"/>
+      <c r="ML71" s="11"/>
+      <c r="MM71" s="11"/>
+      <c r="MN71" s="11"/>
+      <c r="MO71" s="11"/>
+      <c r="MP71" s="11"/>
+      <c r="MQ71" s="11"/>
+      <c r="MR71" s="11"/>
+      <c r="MS71" s="11"/>
+      <c r="MT71" s="11"/>
+      <c r="MU71" s="11"/>
+      <c r="MV71" s="11"/>
+      <c r="MW71" s="11"/>
+      <c r="MX71" s="11"/>
+      <c r="MY71" s="11"/>
+      <c r="MZ71" s="11"/>
+      <c r="NA71" s="11"/>
+      <c r="NB71" s="11"/>
+      <c r="NC71" s="11"/>
+      <c r="ND71" s="11"/>
+      <c r="NE71" s="11"/>
+      <c r="NF71" s="11"/>
+      <c r="NG71" s="11"/>
+      <c r="NH71" s="11"/>
+      <c r="NI71" s="11"/>
+      <c r="NJ71" s="11"/>
+      <c r="NK71" s="11"/>
+      <c r="NL71" s="11"/>
+      <c r="NM71" s="11"/>
+      <c r="NN71" s="11"/>
+      <c r="NO71" s="11"/>
+      <c r="NP71" s="11"/>
+      <c r="NQ71" s="11"/>
+      <c r="NR71" s="11"/>
+      <c r="NS71" s="11"/>
+      <c r="NT71" s="11"/>
+      <c r="NU71" s="11"/>
+      <c r="NV71" s="11"/>
+      <c r="NW71" s="11"/>
+      <c r="NX71" s="11"/>
+      <c r="NY71" s="11"/>
+      <c r="NZ71" s="11"/>
+      <c r="OA71" s="11"/>
+      <c r="OB71" s="11"/>
+      <c r="OC71" s="11"/>
+      <c r="OD71" s="11"/>
+      <c r="OE71" s="11"/>
+      <c r="OF71" s="11"/>
+      <c r="OG71" s="11"/>
+      <c r="OH71" s="11"/>
+      <c r="OI71" s="11"/>
+      <c r="OJ71" s="11"/>
+      <c r="OK71" s="11"/>
+      <c r="OL71" s="11"/>
+      <c r="OM71" s="11"/>
+      <c r="ON71" s="11"/>
+      <c r="OO71" s="11"/>
+      <c r="OP71" s="11"/>
+      <c r="OQ71" s="11"/>
+      <c r="OR71" s="11"/>
+      <c r="OS71" s="11"/>
+      <c r="OT71" s="11"/>
+      <c r="OU71" s="11"/>
+      <c r="OV71" s="11"/>
+      <c r="OW71" s="11"/>
+      <c r="OX71" s="11"/>
+      <c r="OY71" s="11"/>
+      <c r="OZ71" s="11"/>
+      <c r="PA71" s="11"/>
+      <c r="PB71" s="11"/>
+      <c r="PC71" s="11"/>
+      <c r="PD71" s="11"/>
+      <c r="PE71" s="11"/>
+      <c r="PF71" s="11"/>
+      <c r="PG71" s="11"/>
+      <c r="PH71" s="11"/>
+      <c r="PI71" s="11"/>
+      <c r="PJ71" s="11"/>
+      <c r="PK71" s="11"/>
+      <c r="PL71" s="11"/>
+      <c r="PM71" s="11"/>
+      <c r="PN71" s="11"/>
+      <c r="PO71" s="11"/>
+      <c r="PP71" s="11"/>
+      <c r="PQ71" s="11"/>
+      <c r="PR71" s="11"/>
+      <c r="PS71" s="11"/>
+      <c r="PT71" s="11"/>
+      <c r="PU71" s="11"/>
+      <c r="PV71" s="11"/>
+      <c r="PW71" s="11"/>
+      <c r="PX71" s="11"/>
+      <c r="PY71" s="11"/>
+      <c r="PZ71" s="11"/>
+      <c r="QA71" s="11"/>
+      <c r="QB71" s="11"/>
+      <c r="QC71" s="11"/>
+      <c r="QD71" s="11"/>
+      <c r="QE71" s="11"/>
+      <c r="QF71" s="11"/>
+      <c r="QG71" s="11"/>
+      <c r="QH71" s="11"/>
+      <c r="QI71" s="11"/>
+      <c r="QJ71" s="11"/>
+      <c r="QK71" s="11"/>
+      <c r="QL71" s="11"/>
+      <c r="QM71" s="11"/>
+      <c r="QN71" s="11"/>
+      <c r="QO71" s="11"/>
+      <c r="QP71" s="11"/>
+      <c r="QQ71" s="11"/>
+      <c r="QR71" s="11"/>
+      <c r="QS71" s="11"/>
+      <c r="QT71" s="11"/>
+      <c r="QU71" s="11"/>
+      <c r="QV71" s="11"/>
+      <c r="QW71" s="11"/>
+      <c r="QX71" s="11"/>
+      <c r="QY71" s="11"/>
+      <c r="QZ71" s="11"/>
+      <c r="RA71" s="11"/>
+      <c r="RB71" s="11"/>
+      <c r="RC71" s="11"/>
+      <c r="RD71" s="11"/>
+      <c r="RE71" s="11"/>
+      <c r="RF71" s="11"/>
+      <c r="RG71" s="11"/>
+      <c r="RH71" s="11"/>
+      <c r="RI71" s="11"/>
+      <c r="RJ71" s="11"/>
+      <c r="RK71" s="11"/>
+      <c r="RL71" s="11"/>
+      <c r="RM71" s="11"/>
+      <c r="RN71" s="11"/>
+      <c r="RO71" s="11"/>
+      <c r="RP71" s="11"/>
+      <c r="RQ71" s="11"/>
+      <c r="RR71" s="11"/>
+      <c r="RS71" s="11"/>
+      <c r="RT71" s="11"/>
+      <c r="RU71" s="11"/>
+      <c r="RV71" s="11"/>
+      <c r="RW71" s="11"/>
+      <c r="RX71" s="11"/>
+      <c r="RY71" s="11"/>
+      <c r="RZ71" s="11"/>
+      <c r="SA71" s="11"/>
+      <c r="SB71" s="11"/>
+      <c r="SC71" s="11"/>
+      <c r="SD71" s="11"/>
+      <c r="SE71" s="11"/>
+      <c r="SF71" s="11"/>
+      <c r="SG71" s="11"/>
+      <c r="SH71" s="11"/>
+      <c r="SI71" s="11"/>
+      <c r="SJ71" s="11"/>
+      <c r="SK71" s="11"/>
+      <c r="SL71" s="11"/>
+      <c r="SM71" s="11"/>
+      <c r="SN71" s="11"/>
+      <c r="SO71" s="11"/>
+      <c r="SP71" s="11"/>
+      <c r="SQ71" s="11"/>
+      <c r="SR71" s="11"/>
+      <c r="SS71" s="11"/>
+      <c r="ST71" s="11"/>
+      <c r="SU71" s="11"/>
+      <c r="SV71" s="11"/>
+      <c r="SW71" s="11"/>
+      <c r="SX71" s="11"/>
+      <c r="SY71" s="11"/>
+      <c r="SZ71" s="11"/>
+      <c r="TA71" s="11"/>
+      <c r="TB71" s="11"/>
+      <c r="TC71" s="11"/>
+      <c r="TD71" s="11"/>
+      <c r="TE71" s="11"/>
+      <c r="TF71" s="11"/>
+      <c r="TG71" s="11"/>
+      <c r="TH71" s="11"/>
+      <c r="TI71" s="11"/>
+      <c r="TJ71" s="11"/>
+      <c r="TK71" s="11"/>
+      <c r="TL71" s="11"/>
+      <c r="TM71" s="11"/>
+      <c r="TN71" s="11"/>
+      <c r="TO71" s="11"/>
+      <c r="TP71" s="11"/>
+      <c r="TQ71" s="11"/>
+      <c r="TR71" s="11"/>
+      <c r="TS71" s="11"/>
+      <c r="TT71" s="11"/>
+      <c r="TU71" s="11"/>
+      <c r="TV71" s="11"/>
+      <c r="TW71" s="11"/>
+      <c r="TX71" s="11"/>
+      <c r="TY71" s="11"/>
+      <c r="TZ71" s="11"/>
+      <c r="UA71" s="11"/>
+      <c r="UB71" s="11"/>
+      <c r="UC71" s="11"/>
+      <c r="UD71" s="11"/>
+      <c r="UE71" s="11"/>
+      <c r="UF71" s="11"/>
+      <c r="UG71" s="11"/>
+      <c r="UH71" s="11"/>
+      <c r="UI71" s="11"/>
+      <c r="UJ71" s="11"/>
+      <c r="UK71" s="11"/>
+      <c r="UL71" s="11"/>
+      <c r="UM71" s="11"/>
+      <c r="UN71" s="11"/>
+      <c r="UO71" s="11"/>
+      <c r="UP71" s="11"/>
+      <c r="UQ71" s="11"/>
+      <c r="UR71" s="11"/>
+      <c r="US71" s="11"/>
+      <c r="UT71" s="11"/>
+      <c r="UU71" s="11"/>
+      <c r="UV71" s="11"/>
+      <c r="UW71" s="11"/>
+      <c r="UX71" s="11"/>
+      <c r="UY71" s="11"/>
+      <c r="UZ71" s="11"/>
+      <c r="VA71" s="11"/>
+      <c r="VB71" s="11"/>
+      <c r="VC71" s="11"/>
+      <c r="VD71" s="11"/>
+      <c r="VE71" s="11"/>
+      <c r="VF71" s="11"/>
+      <c r="VG71" s="11"/>
+      <c r="VH71" s="11"/>
+      <c r="VI71" s="11"/>
+      <c r="VJ71" s="11"/>
+      <c r="VK71" s="11"/>
+      <c r="VL71" s="11"/>
+      <c r="VM71" s="11"/>
+      <c r="VN71" s="11"/>
+      <c r="VO71" s="11"/>
+      <c r="VP71" s="11"/>
+      <c r="VQ71" s="11"/>
+      <c r="VR71" s="11"/>
+      <c r="VS71" s="11"/>
+      <c r="VT71" s="11"/>
+      <c r="VU71" s="11"/>
+      <c r="VV71" s="11"/>
+      <c r="VW71" s="11"/>
+      <c r="VX71" s="11"/>
+      <c r="VY71" s="11"/>
+      <c r="VZ71" s="11"/>
+      <c r="WA71" s="11"/>
+      <c r="WB71" s="11"/>
+      <c r="WC71" s="11"/>
+      <c r="WD71" s="11"/>
+      <c r="WE71" s="11"/>
+      <c r="WF71" s="11"/>
+      <c r="WG71" s="11"/>
+      <c r="WH71" s="11"/>
+      <c r="WI71" s="11"/>
+      <c r="WJ71" s="11"/>
+      <c r="WK71" s="11"/>
+      <c r="WL71" s="11"/>
+      <c r="WM71" s="11"/>
+      <c r="WN71" s="11"/>
+      <c r="WO71" s="11"/>
+      <c r="WP71" s="11"/>
+      <c r="WQ71" s="11"/>
+      <c r="WR71" s="11"/>
+      <c r="WS71" s="11"/>
+      <c r="WT71" s="11"/>
+      <c r="WU71" s="11"/>
+      <c r="WV71" s="11"/>
+      <c r="WW71" s="11"/>
+      <c r="WX71" s="11"/>
+      <c r="WY71" s="11"/>
+      <c r="WZ71" s="11"/>
+      <c r="XA71" s="11"/>
+      <c r="XB71" s="11"/>
+      <c r="XC71" s="11"/>
+      <c r="XD71" s="11"/>
+      <c r="XE71" s="11"/>
+      <c r="XF71" s="11"/>
+      <c r="XG71" s="11"/>
+      <c r="XH71" s="11"/>
+      <c r="XI71" s="11"/>
+      <c r="XJ71" s="11"/>
+      <c r="XK71" s="11"/>
+      <c r="XL71" s="11"/>
+      <c r="XM71" s="11"/>
+      <c r="XN71" s="11"/>
+      <c r="XO71" s="11"/>
+      <c r="XP71" s="11"/>
+      <c r="XQ71" s="11"/>
+      <c r="XR71" s="11"/>
+      <c r="XS71" s="11"/>
+      <c r="XT71" s="11"/>
+      <c r="XU71" s="11"/>
+      <c r="XV71" s="11"/>
+      <c r="XW71" s="11"/>
+      <c r="XX71" s="11"/>
+      <c r="XY71" s="11"/>
+      <c r="XZ71" s="11"/>
+      <c r="YA71" s="11"/>
+      <c r="YB71" s="11"/>
+      <c r="YC71" s="11"/>
+      <c r="YD71" s="11"/>
+      <c r="YE71" s="11"/>
+      <c r="YF71" s="11"/>
+      <c r="YG71" s="11"/>
+      <c r="YH71" s="11"/>
+      <c r="YI71" s="11"/>
+      <c r="YJ71" s="11"/>
+      <c r="YK71" s="11"/>
+      <c r="YL71" s="11"/>
+      <c r="YM71" s="11"/>
+      <c r="YN71" s="11"/>
+      <c r="YO71" s="11"/>
+      <c r="YP71" s="11"/>
+      <c r="YQ71" s="11"/>
+      <c r="YR71" s="11"/>
+      <c r="YS71" s="11"/>
+      <c r="YT71" s="11"/>
+      <c r="YU71" s="11"/>
+      <c r="YV71" s="11"/>
+      <c r="YW71" s="11"/>
+      <c r="YX71" s="11"/>
+      <c r="YY71" s="11"/>
+      <c r="YZ71" s="11"/>
+      <c r="ZA71" s="11"/>
+      <c r="ZB71" s="11"/>
+      <c r="ZC71" s="11"/>
+      <c r="ZD71" s="11"/>
+      <c r="ZE71" s="11"/>
+      <c r="ZF71" s="11"/>
+      <c r="ZG71" s="11"/>
+      <c r="ZH71" s="11"/>
+      <c r="ZI71" s="11"/>
+      <c r="ZJ71" s="11"/>
+      <c r="ZK71" s="11"/>
+      <c r="ZL71" s="11"/>
+      <c r="ZM71" s="11"/>
+      <c r="ZN71" s="11"/>
+      <c r="ZO71" s="11"/>
+      <c r="ZP71" s="11"/>
+      <c r="ZQ71" s="11"/>
+      <c r="ZR71" s="11"/>
+      <c r="ZS71" s="11"/>
+      <c r="ZT71" s="11"/>
+      <c r="ZU71" s="11"/>
+      <c r="ZV71" s="11"/>
+      <c r="ZW71" s="11"/>
+      <c r="ZX71" s="11"/>
+      <c r="ZY71" s="11"/>
+      <c r="ZZ71" s="11"/>
+      <c r="AAA71" s="11"/>
+      <c r="AAB71" s="11"/>
+      <c r="AAC71" s="11"/>
+      <c r="AAD71" s="11"/>
+      <c r="AAE71" s="11"/>
+      <c r="AAF71" s="11"/>
+      <c r="AAG71" s="11"/>
+      <c r="AAH71" s="11"/>
+      <c r="AAI71" s="11"/>
+      <c r="AAJ71" s="11"/>
+      <c r="AAK71" s="11"/>
+      <c r="AAL71" s="11"/>
+      <c r="AAM71" s="11"/>
+      <c r="AAN71" s="11"/>
+      <c r="AAO71" s="11"/>
+      <c r="AAP71" s="11"/>
+      <c r="AAQ71" s="11"/>
+      <c r="AAR71" s="11"/>
+      <c r="AAS71" s="11"/>
+      <c r="AAT71" s="11"/>
+      <c r="AAU71" s="11"/>
+      <c r="AAV71" s="11"/>
+      <c r="AAW71" s="11"/>
+      <c r="AAX71" s="11"/>
+      <c r="AAY71" s="11"/>
+      <c r="AAZ71" s="11"/>
+      <c r="ABA71" s="11"/>
+      <c r="ABB71" s="11"/>
+      <c r="ABC71" s="11"/>
+      <c r="ABD71" s="11"/>
+      <c r="ABE71" s="11"/>
+      <c r="ABF71" s="11"/>
+      <c r="ABG71" s="11"/>
+      <c r="ABH71" s="11"/>
+      <c r="ABI71" s="11"/>
+      <c r="ABJ71" s="11"/>
+      <c r="ABK71" s="11"/>
+      <c r="ABL71" s="11"/>
+      <c r="ABM71" s="11"/>
+      <c r="ABN71" s="11"/>
+      <c r="ABO71" s="11"/>
+      <c r="ABP71" s="11"/>
+      <c r="ABQ71" s="11"/>
+      <c r="ABR71" s="11"/>
+      <c r="ABS71" s="11"/>
+      <c r="ABT71" s="11"/>
+      <c r="ABU71" s="11"/>
+      <c r="ABV71" s="11"/>
+      <c r="ABW71" s="11"/>
+      <c r="ABX71" s="11"/>
+      <c r="ABY71" s="11"/>
+      <c r="ABZ71" s="11"/>
+      <c r="ACA71" s="11"/>
+      <c r="ACB71" s="11"/>
+      <c r="ACC71" s="11"/>
+      <c r="ACD71" s="11"/>
+      <c r="ACE71" s="11"/>
+      <c r="ACF71" s="11"/>
+      <c r="ACG71" s="11"/>
+      <c r="ACH71" s="11"/>
+      <c r="ACI71" s="11"/>
+      <c r="ACJ71" s="11"/>
+      <c r="ACK71" s="11"/>
+      <c r="ACL71" s="11"/>
+      <c r="ACM71" s="11"/>
+      <c r="ACN71" s="11"/>
+      <c r="ACO71" s="11"/>
+      <c r="ACP71" s="11"/>
+      <c r="ACQ71" s="11"/>
+      <c r="ACR71" s="11"/>
+      <c r="ACS71" s="11"/>
+      <c r="ACT71" s="11"/>
+      <c r="ACU71" s="11"/>
+      <c r="ACV71" s="11"/>
+      <c r="ACW71" s="11"/>
+      <c r="ACX71" s="11"/>
+      <c r="ACY71" s="11"/>
+      <c r="ACZ71" s="11"/>
+      <c r="ADA71" s="11"/>
+      <c r="ADB71" s="11"/>
+      <c r="ADC71" s="11"/>
+      <c r="ADD71" s="11"/>
+      <c r="ADE71" s="11"/>
+      <c r="ADF71" s="11"/>
+      <c r="ADG71" s="11"/>
+      <c r="ADH71" s="11"/>
+      <c r="ADI71" s="11"/>
+      <c r="ADJ71" s="11"/>
+      <c r="ADK71" s="11"/>
+      <c r="ADL71" s="11"/>
+      <c r="ADM71" s="11"/>
+      <c r="ADN71" s="11"/>
+      <c r="ADO71" s="11"/>
+      <c r="ADP71" s="11"/>
+      <c r="ADQ71" s="11"/>
+      <c r="ADR71" s="11"/>
+      <c r="ADS71" s="11"/>
+      <c r="ADT71" s="11"/>
+      <c r="ADU71" s="11"/>
+      <c r="ADV71" s="11"/>
+      <c r="ADW71" s="11"/>
+      <c r="ADX71" s="11"/>
+      <c r="ADY71" s="11"/>
+      <c r="ADZ71" s="11"/>
+      <c r="AEA71" s="11"/>
+      <c r="AEB71" s="11"/>
+      <c r="AEC71" s="11"/>
+      <c r="AED71" s="11"/>
+      <c r="AEE71" s="11"/>
+      <c r="AEF71" s="11"/>
+      <c r="AEG71" s="11"/>
+      <c r="AEH71" s="11"/>
+      <c r="AEI71" s="11"/>
+      <c r="AEJ71" s="11"/>
+      <c r="AEK71" s="11"/>
+      <c r="AEL71" s="11"/>
+      <c r="AEM71" s="11"/>
+      <c r="AEN71" s="11"/>
+      <c r="AEO71" s="11"/>
+      <c r="AEP71" s="11"/>
+      <c r="AEQ71" s="11"/>
+      <c r="AER71" s="11"/>
+      <c r="AES71" s="11"/>
+      <c r="AET71" s="11"/>
+      <c r="AEU71" s="11"/>
+      <c r="AEV71" s="11"/>
+      <c r="AEW71" s="11"/>
+      <c r="AEX71" s="11"/>
+      <c r="AEY71" s="11"/>
+      <c r="AEZ71" s="11"/>
+      <c r="AFA71" s="11"/>
+      <c r="AFB71" s="11"/>
+      <c r="AFC71" s="11"/>
+      <c r="AFD71" s="11"/>
+      <c r="AFE71" s="11"/>
+      <c r="AFF71" s="11"/>
+      <c r="AFG71" s="11"/>
+      <c r="AFH71" s="11"/>
+      <c r="AFI71" s="11"/>
+      <c r="AFJ71" s="11"/>
+      <c r="AFK71" s="11"/>
+      <c r="AFL71" s="11"/>
+      <c r="AFM71" s="11"/>
+      <c r="AFN71" s="11"/>
+      <c r="AFO71" s="11"/>
+      <c r="AFP71" s="11"/>
+      <c r="AFQ71" s="11"/>
+      <c r="AFR71" s="11"/>
+      <c r="AFS71" s="11"/>
+      <c r="AFT71" s="11"/>
+      <c r="AFU71" s="11"/>
+      <c r="AFV71" s="11"/>
+      <c r="AFW71" s="11"/>
+      <c r="AFX71" s="11"/>
+      <c r="AFY71" s="11"/>
+      <c r="AFZ71" s="11"/>
+      <c r="AGA71" s="11"/>
+      <c r="AGB71" s="11"/>
+      <c r="AGC71" s="11"/>
+      <c r="AGD71" s="11"/>
+      <c r="AGE71" s="11"/>
+      <c r="AGF71" s="11"/>
+      <c r="AGG71" s="11"/>
+      <c r="AGH71" s="11"/>
+      <c r="AGI71" s="11"/>
+      <c r="AGJ71" s="11"/>
+      <c r="AGK71" s="11"/>
+      <c r="AGL71" s="11"/>
+      <c r="AGM71" s="11"/>
+      <c r="AGN71" s="11"/>
+      <c r="AGO71" s="11"/>
+      <c r="AGP71" s="11"/>
+      <c r="AGQ71" s="11"/>
+      <c r="AGR71" s="11"/>
+      <c r="AGS71" s="11"/>
+      <c r="AGT71" s="11"/>
+      <c r="AGU71" s="11"/>
+      <c r="AGV71" s="11"/>
+      <c r="AGW71" s="11"/>
+      <c r="AGX71" s="11"/>
+      <c r="AGY71" s="11"/>
+      <c r="AGZ71" s="11"/>
+      <c r="AHA71" s="11"/>
+      <c r="AHB71" s="11"/>
+      <c r="AHC71" s="11"/>
+      <c r="AHD71" s="11"/>
+      <c r="AHE71" s="11"/>
+      <c r="AHF71" s="11"/>
+      <c r="AHG71" s="11"/>
+      <c r="AHH71" s="11"/>
+      <c r="AHI71" s="11"/>
+      <c r="AHJ71" s="11"/>
+      <c r="AHK71" s="11"/>
+      <c r="AHL71" s="11"/>
+      <c r="AHM71" s="11"/>
+      <c r="AHN71" s="11"/>
+      <c r="AHO71" s="11"/>
+      <c r="AHP71" s="11"/>
+      <c r="AHQ71" s="11"/>
+      <c r="AHR71" s="11"/>
+      <c r="AHS71" s="11"/>
+      <c r="AHT71" s="11"/>
+      <c r="AHU71" s="11"/>
+      <c r="AHV71" s="11"/>
+      <c r="AHW71" s="11"/>
+      <c r="AHX71" s="11"/>
+      <c r="AHY71" s="11"/>
+      <c r="AHZ71" s="11"/>
+      <c r="AIA71" s="11"/>
+      <c r="AIB71" s="11"/>
+      <c r="AIC71" s="11"/>
+      <c r="AID71" s="11"/>
+      <c r="AIE71" s="11"/>
+      <c r="AIF71" s="11"/>
+      <c r="AIG71" s="11"/>
+      <c r="AIH71" s="11"/>
+      <c r="AII71" s="11"/>
+      <c r="AIJ71" s="11"/>
+      <c r="AIK71" s="11"/>
+      <c r="AIL71" s="11"/>
+      <c r="AIM71" s="11"/>
+      <c r="AIN71" s="11"/>
+      <c r="AIO71" s="11"/>
+      <c r="AIP71" s="11"/>
+      <c r="AIQ71" s="11"/>
+      <c r="AIR71" s="11"/>
+      <c r="AIS71" s="11"/>
+      <c r="AIT71" s="11"/>
+      <c r="AIU71" s="11"/>
+      <c r="AIV71" s="11"/>
+      <c r="AIW71" s="11"/>
+      <c r="AIX71" s="11"/>
+      <c r="AIY71" s="11"/>
+      <c r="AIZ71" s="11"/>
+      <c r="AJA71" s="11"/>
+      <c r="AJB71" s="11"/>
+      <c r="AJC71" s="11"/>
+      <c r="AJD71" s="11"/>
+      <c r="AJE71" s="11"/>
+      <c r="AJF71" s="11"/>
+      <c r="AJG71" s="11"/>
+      <c r="AJH71" s="11"/>
+      <c r="AJI71" s="11"/>
+      <c r="AJJ71" s="11"/>
+      <c r="AJK71" s="11"/>
+      <c r="AJL71" s="11"/>
+      <c r="AJM71" s="11"/>
+      <c r="AJN71" s="11"/>
+      <c r="AJO71" s="11"/>
+      <c r="AJP71" s="11"/>
+      <c r="AJQ71" s="11"/>
+      <c r="AJR71" s="11"/>
+      <c r="AJS71" s="11"/>
+      <c r="AJT71" s="11"/>
+      <c r="AJU71" s="11"/>
+      <c r="AJV71" s="11"/>
+      <c r="AJW71" s="11"/>
+      <c r="AJX71" s="11"/>
+      <c r="AJY71" s="11"/>
+      <c r="AJZ71" s="11"/>
+      <c r="AKA71" s="11"/>
+      <c r="AKB71" s="11"/>
+      <c r="AKC71" s="11"/>
+      <c r="AKD71" s="11"/>
+      <c r="AKE71" s="11"/>
+      <c r="AKF71" s="11"/>
+      <c r="AKG71" s="11"/>
+      <c r="AKH71" s="11"/>
+      <c r="AKI71" s="11"/>
+      <c r="AKJ71" s="11"/>
+      <c r="AKK71" s="11"/>
+      <c r="AKL71" s="11"/>
+      <c r="AKM71" s="11"/>
+      <c r="AKN71" s="11"/>
+      <c r="AKO71" s="11"/>
+      <c r="AKP71" s="11"/>
+      <c r="AKQ71" s="11"/>
+      <c r="AKR71" s="11"/>
+      <c r="AKS71" s="11"/>
+      <c r="AKT71" s="11"/>
+      <c r="AKU71" s="11"/>
+      <c r="AKV71" s="11"/>
+      <c r="AKW71" s="11"/>
+      <c r="AKX71" s="11"/>
+      <c r="AKY71" s="11"/>
+      <c r="AKZ71" s="11"/>
+      <c r="ALA71" s="11"/>
+      <c r="ALB71" s="11"/>
+      <c r="ALC71" s="11"/>
+      <c r="ALD71" s="11"/>
+      <c r="ALE71" s="11"/>
+      <c r="ALF71" s="11"/>
+      <c r="ALG71" s="11"/>
+      <c r="ALH71" s="11"/>
+      <c r="ALI71" s="11"/>
+      <c r="ALJ71" s="11"/>
+      <c r="ALK71" s="11"/>
+      <c r="ALL71" s="11"/>
+      <c r="ALM71" s="11"/>
+      <c r="ALN71" s="11"/>
+      <c r="ALO71" s="11"/>
+      <c r="ALP71" s="11"/>
+      <c r="ALQ71" s="11"/>
+      <c r="ALR71" s="11"/>
+      <c r="ALS71" s="11"/>
+      <c r="ALT71" s="11"/>
+      <c r="ALU71" s="11"/>
+      <c r="ALV71" s="11"/>
+      <c r="ALW71" s="11"/>
+      <c r="ALX71" s="11"/>
+      <c r="ALY71" s="11"/>
+      <c r="ALZ71" s="11"/>
+      <c r="AMA71" s="11"/>
+      <c r="AMB71" s="11"/>
+      <c r="AMC71" s="11"/>
+      <c r="AMD71" s="11"/>
+      <c r="AME71" s="11"/>
+      <c r="AMF71" s="11"/>
+      <c r="AMG71" s="11"/>
+      <c r="AMH71" s="11"/>
+      <c r="AMI71" s="11"/>
+      <c r="AMJ71" s="11"/>
+    </row>
+    <row r="1048415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>